<commit_message>
All typos in excel fixed
</commit_message>
<xml_diff>
--- a/mappings/kegg_reactome.xlsx
+++ b/mappings/kegg_reactome.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danieldomingo/PycharmProjects/compath_curation/curation/mappings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danieldomingo/PycharmProjects/curation/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2452,8 +2452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y326"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A295" workbookViewId="0">
-      <selection activeCell="D295" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Manually inspected common equivalent mappings
</commit_message>
<xml_diff>
--- a/mappings/kegg_reactome.xlsx
+++ b/mappings/kegg_reactome.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="551">
   <si>
     <t>KEGG References</t>
   </si>
@@ -1823,11 +1823,6 @@
     <t>Synthesis and degradation of ketone bodies - Homo sapiens (human)</t>
   </si>
   <si>
-    <t>Ketone body metabolism isPartOf Synthesis and degradation of ketone bodies - Homo sapiens (human)*
-Synthesis of Ketone Bodies isPartOf Synthesis and degradation of ketone bodies - Homo sapiens (human)*
-Synthesis and degradation of ketone bodies - Homo sapiens (human)* isPartOf Metabolism</t>
-  </si>
-  <si>
     <t>Systemic lupus erythematosus - Homo sapiens (human)</t>
   </si>
   <si>
@@ -2106,6 +2101,15 @@
 TP53 Regulates Transcription of Genes Involved in Cytochrome C Release isPartOf p53 signaling pathway - Homo sapiens (human)*
 Regulation of TP53 Expression and Degradation isPartOf p53 signaling pathway - Homo sapiens (human)*
 Regulation of TP53 Degradation isPartOf p53 signaling pathway - Homo sapiens (human)*</t>
+  </si>
+  <si>
+    <t>Synthesis and degradation of ketone bodies - Homo sapiens (human)* isPartOf Metabolism</t>
+  </si>
+  <si>
+    <t>Synthesis of Ketone Bodies equivalentTo Synthesis and degradation of ketone bodies - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Homology Directed Repair isPartOf Homologous recombination - Homo sapiens (human)*</t>
   </si>
 </sst>
 </file>
@@ -2452,8 +2456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y326"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="A144" sqref="A144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3683,12 +3687,14 @@
         <v>243</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A143" s="3" t="s">
         <v>244</v>
       </c>
       <c r="B143" s="3"/>
-      <c r="C143" s="3"/>
+      <c r="C143" s="3" t="s">
+        <v>550</v>
+      </c>
     </row>
     <row r="144" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A144" s="3" t="s">
@@ -4835,382 +4841,384 @@
         <v>469</v>
       </c>
     </row>
-    <row r="283" spans="1:3" ht="84" x14ac:dyDescent="0.15">
+    <row r="283" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A283" s="3" t="s">
         <v>470</v>
       </c>
-      <c r="B283" s="3"/>
+      <c r="B283" s="3" t="s">
+        <v>549</v>
+      </c>
       <c r="C283" s="3" t="s">
-        <v>471</v>
+        <v>548</v>
       </c>
     </row>
     <row r="284" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A284" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B284" s="3"/>
       <c r="C284" s="3"/>
     </row>
     <row r="285" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A285" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B285" s="3"/>
       <c r="C285" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="286" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A286" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B286" s="3"/>
       <c r="C286" s="3"/>
     </row>
     <row r="287" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A287" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="B287" s="3" t="s">
         <v>476</v>
-      </c>
-      <c r="B287" s="3" t="s">
-        <v>477</v>
       </c>
       <c r="C287" s="3"/>
     </row>
     <row r="288" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A288" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B288" s="3"/>
       <c r="C288" s="3"/>
     </row>
     <row r="289" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A289" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B289" s="3"/>
       <c r="C289" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="290" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A290" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B290" s="3"/>
       <c r="C290" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="291" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A291" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B291" s="3"/>
       <c r="C291" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="292" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A292" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B292" s="3"/>
       <c r="C292" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="293" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A293" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B293" s="3"/>
       <c r="C293" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="294" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A294" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="B294" s="3" t="s">
         <v>489</v>
       </c>
-      <c r="B294" s="3" t="s">
+      <c r="C294" s="3" t="s">
         <v>490</v>
-      </c>
-      <c r="C294" s="3" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="295" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A295" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B295" s="3"/>
       <c r="C295" s="3"/>
     </row>
     <row r="296" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A296" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B296" s="3"/>
       <c r="C296" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="297" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A297" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="B297" s="3" t="s">
         <v>495</v>
-      </c>
-      <c r="B297" s="3" t="s">
-        <v>496</v>
       </c>
       <c r="C297" s="3"/>
     </row>
     <row r="298" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A298" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="B298" s="3" t="s">
         <v>497</v>
       </c>
-      <c r="B298" s="3" t="s">
+      <c r="C298" s="3" t="s">
         <v>498</v>
-      </c>
-      <c r="C298" s="3" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="299" spans="1:3" ht="252" x14ac:dyDescent="0.15">
       <c r="A299" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="B299" s="3" t="s">
         <v>500</v>
       </c>
-      <c r="B299" s="3" t="s">
+      <c r="C299" s="3" t="s">
         <v>501</v>
-      </c>
-      <c r="C299" s="3" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="300" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A300" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B300" s="3"/>
       <c r="C300" s="3"/>
     </row>
     <row r="301" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A301" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B301" s="3"/>
       <c r="C301" s="3"/>
     </row>
     <row r="302" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A302" s="3" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B302" s="3"/>
       <c r="C302" s="3" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="303" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A303" s="3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B303" s="3"/>
       <c r="C303" s="3"/>
     </row>
     <row r="304" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A304" s="3" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B304" s="3"/>
       <c r="C304" s="3"/>
     </row>
     <row r="305" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A305" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B305" s="3"/>
       <c r="C305" s="3"/>
     </row>
     <row r="306" spans="1:3" ht="126" x14ac:dyDescent="0.15">
       <c r="A306" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B306" s="3"/>
       <c r="C306" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="307" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A307" s="3" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B307" s="3"/>
       <c r="C307" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="308" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A308" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B308" s="3"/>
       <c r="C308" s="3"/>
     </row>
     <row r="309" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A309" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B309" s="3"/>
       <c r="C309" s="3"/>
     </row>
     <row r="310" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A310" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B310" s="3"/>
       <c r="C310" s="3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="311" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A311" s="3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B311" s="3"/>
       <c r="C311" s="3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="312" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A312" s="3" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B312" s="3"/>
       <c r="C312" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="313" spans="1:3" ht="42" x14ac:dyDescent="0.15">
       <c r="A313" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="B313" s="3" t="s">
         <v>522</v>
-      </c>
-      <c r="B313" s="3" t="s">
-        <v>523</v>
       </c>
       <c r="C313" s="3"/>
     </row>
     <row r="314" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A314" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B314" s="3"/>
       <c r="C314" s="3"/>
     </row>
     <row r="315" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A315" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B315" s="3"/>
       <c r="C315" s="3"/>
     </row>
     <row r="316" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A316" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B316" s="3"/>
       <c r="C316" s="3"/>
     </row>
     <row r="317" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A317" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B317" s="3"/>
       <c r="C317" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="318" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A318" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B318" s="3"/>
       <c r="C318" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="319" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A319" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="B319" s="3" t="s">
         <v>531</v>
       </c>
-      <c r="B319" s="3" t="s">
+      <c r="C319" s="3" t="s">
         <v>532</v>
-      </c>
-      <c r="C319" s="3" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="320" spans="1:3" ht="42" x14ac:dyDescent="0.15">
       <c r="A320" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="B320" s="3" t="s">
         <v>534</v>
       </c>
-      <c r="B320" s="3" t="s">
+      <c r="C320" s="3" t="s">
         <v>535</v>
-      </c>
-      <c r="C320" s="3" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="321" spans="1:3" ht="42" x14ac:dyDescent="0.15">
       <c r="A321" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B321" s="3"/>
       <c r="C321" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="322" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A322" s="3" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B322" s="3"/>
       <c r="C322" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="323" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A323" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B323" s="3"/>
       <c r="C323" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="324" spans="1:3" ht="182" x14ac:dyDescent="0.15">
       <c r="A324" s="3" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B324" s="3"/>
       <c r="C324" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="325" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A325" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="B325" s="3" t="s">
         <v>545</v>
-      </c>
-      <c r="B325" s="3" t="s">
-        <v>546</v>
       </c>
       <c r="C325" s="3"/>
     </row>
     <row r="326" spans="1:3" ht="350" x14ac:dyDescent="0.15">
       <c r="A326" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B326" s="3"/>
       <c r="C326" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove Apoptosis multiple species mapping
</commit_message>
<xml_diff>
--- a/mappings/kegg_reactome.xlsx
+++ b/mappings/kegg_reactome.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,29 +22,29 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="554">
   <si>
-    <t xml:space="preserve">KEGG References</t>
-  </si>
-  <si>
-    <t xml:space="preserve">equivalentTo Mappings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isPartOf Mappings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-Oxocarboxylic acid metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abnormal conversion of 2-oxoglutarate to 2-hydroxyglutarate isPartOf 2-Oxocarboxylic acid metabolism - Homo sapiens (human)*
+    <t>KEGG References</t>
+  </si>
+  <si>
+    <t>equivalentTo Mappings</t>
+  </si>
+  <si>
+    <t>isPartOf Mappings</t>
+  </si>
+  <si>
+    <t>2-Oxocarboxylic acid metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Abnormal conversion of 2-oxoglutarate to 2-hydroxyglutarate isPartOf 2-Oxocarboxylic acid metabolism - Homo sapiens (human)*
 Pyruvate metabolism and Citric Acid (TCA) cycle isPartOf 2-Oxocarboxylic acid metabolism - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">ABC transporters - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABC transporters - Homo sapiens (human) equivalentTo Mitochondrial ABC transporters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Defective ABCC8 can cause hypoglycemias and hyperglycemias isPartOf ABC transporters - Homo sapiens (human)*
+    <t>ABC transporters - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>ABC transporters - Homo sapiens (human) equivalentTo Mitochondrial ABC transporters</t>
+  </si>
+  <si>
+    <t>Defective ABCC8 can cause hypoglycemias and hyperglycemias isPartOf ABC transporters - Homo sapiens (human)*
 Defective ABCC2 causes Dubin-Johnson syndrome isPartOf ABC transporters - Homo sapiens (human)*
 Defective ABCG5 causes sitosterolemia isPartOf ABC transporters - Homo sapiens (human)*
 Defective ABCD4 causes methylmalonic aciduria and homocystinuria, cblj type (MAHCJ) isPartOf ABC transporters - Homo sapiens (human)*
@@ -64,198 +64,198 @@
 ABC-family proteins mediated transport isPartOf ABC transporters - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">AGE-RAGE signaling pathway in diabetic complications - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AMPK signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AMPK inhibits chREBP transcriptional activation activity isPartOf AMPK signaling pathway - Homo sapiens (human)*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acute myeloid leukemia - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adherens junction - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adherens junction - Homo sapiens (human) equivalentTo Adherens junctions interactions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adipocytokine signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Signaling by Leptin isPartOf Adipocytokine signaling pathway - Homo sapiens (human)*
+    <t>AGE-RAGE signaling pathway in diabetic complications - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>AMPK signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>AMPK inhibits chREBP transcriptional activation activity isPartOf AMPK signaling pathway - Homo sapiens (human)*</t>
+  </si>
+  <si>
+    <t>Acute myeloid leukemia - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Adherens junction - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Adherens junction - Homo sapiens (human) equivalentTo Adherens junctions interactions</t>
+  </si>
+  <si>
+    <t>Adipocytokine signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Signaling by Leptin isPartOf Adipocytokine signaling pathway - Homo sapiens (human)*
 Adipocytokine signaling pathway - Homo sapiens (human)* isPartOf Metabolism</t>
   </si>
   <si>
-    <t xml:space="preserve">Adrenergic signaling in cardiomyocytes - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">African trypanosomiasis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alanine, aspartate and glutamate metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alanine, aspartate and glutamate metabolism - Homo sapiens (human)* isPartOf Metabolism of amino acids and derivatives
+    <t>Adrenergic signaling in cardiomyocytes - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>African trypanosomiasis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Alanine, aspartate and glutamate metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Alanine, aspartate and glutamate metabolism - Homo sapiens (human)* isPartOf Metabolism of amino acids and derivatives
 Alanine, aspartate and glutamate metabolism - Homo sapiens (human)* isPartOf Metabolism</t>
   </si>
   <si>
-    <t xml:space="preserve">Alcoholism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aldosterone synthesis and secretion - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aldosterone synthesis and secretion - Homo sapiens (human)* isPartOf Metabolism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aldosterone-regulated sodium reabsorption - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allograft rejection - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allograft rejection - Homo sapiens (human)* isPartOf Adaptive Immune System
+    <t>Alcoholism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Aldosterone synthesis and secretion - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Aldosterone synthesis and secretion - Homo sapiens (human)* isPartOf Metabolism</t>
+  </si>
+  <si>
+    <t>Aldosterone-regulated sodium reabsorption - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Allograft rejection - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Allograft rejection - Homo sapiens (human)* isPartOf Adaptive Immune System
 Allograft rejection - Homo sapiens (human)* isPartOf Immune System</t>
   </si>
   <si>
-    <t xml:space="preserve">Alzheimer's disease - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deregulated CDK5 triggers multiple neurodegenerative pathways in Alzheimer's disease models isPartOf Alzheimer's disease - Homo sapiens (human)*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amino sugar and nucleotide sugar metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amino sugar and nucleotide sugar metabolism - Homo sapiens (human)* isPartOf Metabolism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aminoacyl-tRNA biosynthesis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aminoacyl-tRNA biosynthesis - Homo sapiens (human)* isPartOf Metabolism
+    <t>Alzheimer's disease - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Deregulated CDK5 triggers multiple neurodegenerative pathways in Alzheimer's disease models isPartOf Alzheimer's disease - Homo sapiens (human)*</t>
+  </si>
+  <si>
+    <t>Amino sugar and nucleotide sugar metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Amino sugar and nucleotide sugar metabolism - Homo sapiens (human)* isPartOf Metabolism</t>
+  </si>
+  <si>
+    <t>Aminoacyl-tRNA biosynthesis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Aminoacyl-tRNA biosynthesis - Homo sapiens (human)* isPartOf Metabolism
 tRNA Aminoacylation isPartOf Aminoacyl-tRNA biosynthesis - Homo sapiens (human)*
 Mitochondrial tRNA aminoacylation isPartOf Aminoacyl-tRNA biosynthesis - Homo sapiens (human)*
 Cytosolic tRNA aminoacylation isPartOf Aminoacyl-tRNA biosynthesis - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Amoebiasis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amphetamine addiction - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amyotrophic lateral sclerosis (ALS) - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Antifolate resistance - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Antigen processing and presentation - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Antigen processing and presentation - Homo sapiens (human) equivalentTo Antigen processing-Cross presentation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MHC class II antigen presentation isPartOf Antigen processing and presentation - Homo sapiens (human)*
+    <t>Amoebiasis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Amphetamine addiction - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Amyotrophic lateral sclerosis (ALS) - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Antifolate resistance - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Antigen processing and presentation - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Antigen processing and presentation - Homo sapiens (human) equivalentTo Antigen processing-Cross presentation</t>
+  </si>
+  <si>
+    <t>MHC class II antigen presentation isPartOf Antigen processing and presentation - Homo sapiens (human)*
 Antigen Presentation: Folding, assembly and peptide loading of class I MHC isPartOf Antigen processing and presentation - Homo sapiens (human)*
 Class I MHC mediated antigen processing &amp; presentation isPartOf Antigen processing and presentation - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Apelin signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apoptosis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apoptosis - Homo sapiens (human) equivalentTo Apoptosis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apoptosis - multiple species - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apoptosis - multiple species - Homo sapiens (human) equivalentTo Apoptosis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arachidonic acid metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arachidonic acid metabolism - Homo sapiens (human) equivalentTo Arachidonic acid metabolism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arginine and proline metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proline catabolism isPartOf Arginine and proline metabolism - Homo sapiens (human)*
+    <t>Apelin signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Apoptosis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Apoptosis - Homo sapiens (human) equivalentTo Apoptosis</t>
+  </si>
+  <si>
+    <t>Apoptosis - multiple species - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Apoptosis isPartOf Apoptosis - multiple species - Homo sapiens (human)*</t>
+  </si>
+  <si>
+    <t>Arachidonic acid metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Arachidonic acid metabolism - Homo sapiens (human) equivalentTo Arachidonic acid metabolism</t>
+  </si>
+  <si>
+    <t>Arginine and proline metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Proline catabolism isPartOf Arginine and proline metabolism - Homo sapiens (human)*
 Arginine and proline metabolism - Homo sapiens (human)* isPartOf Metabolism
 Arginine and proline metabolism - Homo sapiens (human)* isPartOf Metabolism of amino acids and derivatives</t>
   </si>
   <si>
-    <t xml:space="preserve">Arginine biosynthesis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arginine biosynthesis - Homo sapiens (human)* isPartOf Metabolism
+    <t>Arginine biosynthesis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Arginine biosynthesis - Homo sapiens (human)* isPartOf Metabolism
 Arginine biosynthesis - Homo sapiens (human)* isPartOf Metabolism of amino acids and derivatives
 Arginine biosynthesis - Homo sapiens (human)* isPartOf Urea cycle</t>
   </si>
   <si>
-    <t xml:space="preserve">Arrhythmogenic right ventricular cardiomyopathy (ARVC) - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ascorbate and aldarate metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ascorbate and aldarate metabolism - Homo sapiens (human)* isPartOf Metabolism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asthma - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Autoimmune thyroid disease - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Autophagy - animal - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Autophagy - other - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Autophagy - other - Homo sapiens (human) equivalentTo Macroautophagy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Autophagy - other - Homo sapiens (human)* isPartOf Immune System
+    <t>Arrhythmogenic right ventricular cardiomyopathy (ARVC) - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Ascorbate and aldarate metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Ascorbate and aldarate metabolism - Homo sapiens (human)* isPartOf Metabolism</t>
+  </si>
+  <si>
+    <t>Asthma - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Autoimmune thyroid disease - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Autophagy - animal - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Autophagy - other - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Autophagy - other - Homo sapiens (human) equivalentTo Macroautophagy</t>
+  </si>
+  <si>
+    <t>Autophagy - other - Homo sapiens (human)* isPartOf Immune System
 Cellular responses to external stimuli isPartOf Autophagy - other - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Axon guidance - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Axon guidance - Homo sapiens (human) equivalentTo Axon guidance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B cell receptor signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B cell receptor signaling pathway - Homo sapiens (human) equivalentTo Signaling by the B Cell Receptor (BCR)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B cell receptor signaling pathway - Homo sapiens (human)* isPartOf Adaptive Immune System
+    <t>Axon guidance - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Axon guidance - Homo sapiens (human) equivalentTo Axon guidance</t>
+  </si>
+  <si>
+    <t>B cell receptor signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>B cell receptor signaling pathway - Homo sapiens (human) equivalentTo Signaling by the B Cell Receptor (BCR)</t>
+  </si>
+  <si>
+    <t>B cell receptor signaling pathway - Homo sapiens (human)* isPartOf Adaptive Immune System
 B cell receptor signaling pathway - Homo sapiens (human)* isPartOf Immune System</t>
   </si>
   <si>
-    <t xml:space="preserve">Bacterial invasion of epithelial cells - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basal cell carcinoma - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basal transcription factors - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RNA polymerase II transcribes snRNA genes isPartOf Basal transcription factors - Homo sapiens (human)*
+    <t>Bacterial invasion of epithelial cells - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Basal cell carcinoma - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Basal transcription factors - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>RNA polymerase II transcribes snRNA genes isPartOf Basal transcription factors - Homo sapiens (human)*
 RNA Polymerase II Pre-transcription Events isPartOf Basal transcription factors - Homo sapiens (human)*
 RNA Polymerase II Promoter Escape isPartOf Basal transcription factors - Homo sapiens (human)*
 RNA Pol II CTD phosphorylation and interaction with CE during HIV infection isPartOf Basal transcription factors - Homo sapiens (human)*
@@ -273,22 +273,22 @@
 RNA Polymerase II Transcription Initiation And Promoter Clearance isPartOf Basal transcription factors - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Base excision repair - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Base excision repair - Homo sapiens (human) equivalentTo Base Excision Repair</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bile secretion - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bile secretion - Homo sapiens (human)* isPartOf Digestion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biosynthesis of amino acids - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amino acid synthesis and interconversion (transamination) isPartOf Biosynthesis of amino acids - Homo sapiens (human)*
+    <t>Base excision repair - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Base excision repair - Homo sapiens (human) equivalentTo Base Excision Repair</t>
+  </si>
+  <si>
+    <t>Bile secretion - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Bile secretion - Homo sapiens (human)* isPartOf Digestion</t>
+  </si>
+  <si>
+    <t>Biosynthesis of amino acids - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Amino acid synthesis and interconversion (transamination) isPartOf Biosynthesis of amino acids - Homo sapiens (human)*
 Cysteine formation from homocysteine isPartOf Biosynthesis of amino acids - Homo sapiens (human)*
 Biosynthesis of amino acids - Homo sapiens (human)* isPartOf Metabolism
 Urea cycle isPartOf Biosynthesis of amino acids - Homo sapiens (human)*
@@ -296,10 +296,10 @@
 Biosynthesis of amino acids - Homo sapiens (human)* isPartOf Metabolism of amino acids and derivatives</t>
   </si>
   <si>
-    <t xml:space="preserve">Biosynthesis of unsaturated fatty acids - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linoleic acid (LA) metabolism isPartOf Biosynthesis of unsaturated fatty acids - Homo sapiens (human)*
+    <t>Biosynthesis of unsaturated fatty acids - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Linoleic acid (LA) metabolism isPartOf Biosynthesis of unsaturated fatty acids - Homo sapiens (human)*
 Fatty acyl-CoA biosynthesis isPartOf Biosynthesis of unsaturated fatty acids - Homo sapiens (human)*
 Synthesis of very long-chain fatty acyl-CoAs isPartOf Biosynthesis of unsaturated fatty acids - Homo sapiens (human)*
 Biosynthesis of unsaturated fatty acids - Homo sapiens (human)* isPartOf Fatty acid metabolism
@@ -308,59 +308,59 @@
 Biosynthesis of unsaturated fatty acids - Homo sapiens (human)* isPartOf Metabolism of lipids</t>
   </si>
   <si>
-    <t xml:space="preserve">Biotin metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biotin metabolism - Homo sapiens (human)* isPartOf Biotin transport and metabolism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bladder cancer - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Breast cancer - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Butanoate metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beta oxidation of hexanoyl-CoA to butanoyl-CoA isPartOf Butanoate metabolism - Homo sapiens (human)*
+    <t>Biotin metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Biotin metabolism - Homo sapiens (human)* isPartOf Biotin transport and metabolism</t>
+  </si>
+  <si>
+    <t>Bladder cancer - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Breast cancer - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Butanoate metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Beta oxidation of hexanoyl-CoA to butanoyl-CoA isPartOf Butanoate metabolism - Homo sapiens (human)*
 Beta oxidation of butanoyl-CoA to acetyl-CoA isPartOf Butanoate metabolism - Homo sapiens (human)*
 Butanoate metabolism - Homo sapiens (human)* isPartOf Metabolism</t>
   </si>
   <si>
-    <t xml:space="preserve">Caffeine metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Caffeine metabolism - Homo sapiens (human)* isPartOf Metabolism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcium signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elevation of cytosolic Ca2+ levels isPartOf Calcium signaling pathway - Homo sapiens (human)*
+    <t>Caffeine metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Caffeine metabolism - Homo sapiens (human)* isPartOf Metabolism</t>
+  </si>
+  <si>
+    <t>Calcium signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Elevation of cytosolic Ca2+ levels isPartOf Calcium signaling pathway - Homo sapiens (human)*
 CaM pathway isPartOf Calcium signaling pathway - Homo sapiens (human)*
 Platelet calcium homeostasis isPartOf Calcium signaling pathway - Homo sapiens (human)*
 Activation of CaMK IV isPartOf Calcium signaling pathway - Homo sapiens (human)*
 Reduction of cytosolic Ca++ levels isPartOf Calcium signaling pathway - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Carbohydrate digestion and absorption - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intestinal absorption isPartOf Carbohydrate digestion and absorption - Homo sapiens (human)*
+    <t>Carbohydrate digestion and absorption - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Intestinal absorption isPartOf Carbohydrate digestion and absorption - Homo sapiens (human)*
 Digestion of dietary carbohydrate isPartOf Carbohydrate digestion and absorption - Homo sapiens (human)*
 Intestinal saccharidase deficiencies isPartOf Carbohydrate digestion and absorption - Homo sapiens (human)*
 Intestinal hexose absorption isPartOf Carbohydrate digestion and absorption - Homo sapiens (human)*
 Digestion and absorption isPartOf Carbohydrate digestion and absorption - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Carbon metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carbon metabolism - Homo sapiens (human) equivalentTo Metabolism of carbohydrates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glucose metabolism isPartOf Carbon metabolism - Homo sapiens (human)*
+    <t>Carbon metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Carbon metabolism - Homo sapiens (human) equivalentTo Metabolism of carbohydrates</t>
+  </si>
+  <si>
+    <t>Glucose metabolism isPartOf Carbon metabolism - Homo sapiens (human)*
 Fructose metabolism isPartOf Carbon metabolism - Homo sapiens (human)*
 Carbon metabolism - Homo sapiens (human)* isPartOf Metabolism
 5-Phosphoribose 1-diphosphate biosynthesis isPartOf Carbon metabolism - Homo sapiens (human)*
@@ -370,52 +370,52 @@
 Glycolysis isPartOf Carbon metabolism - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Cardiac muscle contraction - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cardiac muscle contraction - Homo sapiens (human)* isPartOf Muscle contraction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cell adhesion molecules (CAMs) - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cell adhesion molecules (CAMs) - Homo sapiens (human)* isPartOf Cell-cell junction organization
+    <t>Cardiac muscle contraction - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Cardiac muscle contraction - Homo sapiens (human)* isPartOf Muscle contraction</t>
+  </si>
+  <si>
+    <t>Cell adhesion molecules (CAMs) - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Cell adhesion molecules (CAMs) - Homo sapiens (human)* isPartOf Cell-cell junction organization
 Neurofascin interactions isPartOf Cell adhesion molecules (CAMs) - Homo sapiens (human)*
 Cell-cell junction organization isPartOf Cell adhesion molecules (CAMs) - Homo sapiens (human)*
 Cell adhesion molecules (CAMs) - Homo sapiens (human)* isPartOf Tight junction interactions</t>
   </si>
   <si>
-    <t xml:space="preserve">Cell cycle - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cell cycle - Homo sapiens (human) equivalentTo Cell Cycle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cellular senescence - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cellular senescence - Homo sapiens (human) equivalentTo Cellular Senescence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central carbon metabolism in cancer - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chagas disease (American trypanosomiasis) - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chemical carcinogenesis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chemokine signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chemokine receptors bind chemokines isPartOf Chemokine signaling pathway - Homo sapiens (human)*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cholesterol metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LDL remodeling isPartOf Cholesterol metabolism - Homo sapiens (human)*
+    <t>Cell cycle - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Cell cycle - Homo sapiens (human) equivalentTo Cell Cycle</t>
+  </si>
+  <si>
+    <t>Cellular senescence - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Cellular senescence - Homo sapiens (human) equivalentTo Cellular Senescence</t>
+  </si>
+  <si>
+    <t>Central carbon metabolism in cancer - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Chagas disease (American trypanosomiasis) - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Chemical carcinogenesis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Chemokine signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Chemokine receptors bind chemokines isPartOf Chemokine signaling pathway - Homo sapiens (human)*</t>
+  </si>
+  <si>
+    <t>Cholesterol metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>LDL remodeling isPartOf Cholesterol metabolism - Homo sapiens (human)*
 Chylomicron assembly isPartOf Cholesterol metabolism - Homo sapiens (human)*
 Cholesterol metabolism - Homo sapiens (human)* isPartOf Metabolism
 HDL clearance isPartOf Cholesterol metabolism - Homo sapiens (human)*
@@ -428,48 +428,48 @@
 LDL clearance isPartOf Cholesterol metabolism - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Choline metabolism in cancer - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cholinergic synapse - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Muscarinic acetylcholine receptors isPartOf Cholinergic synapse - Homo sapiens (human)*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chronic myeloid leukemia - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Circadian entrainment - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Circadian rhythm - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Citrate cycle (TCA cycle) - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Citrate cycle (TCA cycle) - Homo sapiens (human) equivalentTo Citric acid cycle (TCA cycle)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cocaine addiction - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Collecting duct acid secretion - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Colorectal cancer - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Defective Mismatch Repair Associated With MSH3 isPartOf Colorectal cancer - Homo sapiens (human)*
+    <t>Choline metabolism in cancer - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Cholinergic synapse - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Muscarinic acetylcholine receptors isPartOf Cholinergic synapse - Homo sapiens (human)*</t>
+  </si>
+  <si>
+    <t>Chronic myeloid leukemia - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Circadian entrainment - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Circadian rhythm - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Citrate cycle (TCA cycle) - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Citrate cycle (TCA cycle) - Homo sapiens (human) equivalentTo Citric acid cycle (TCA cycle)</t>
+  </si>
+  <si>
+    <t>Cocaine addiction - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Collecting duct acid secretion - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Colorectal cancer - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Defective Mismatch Repair Associated With MSH3 isPartOf Colorectal cancer - Homo sapiens (human)*
 Defective Mismatch Repair Associated With MSH2 isPartOf Colorectal cancer - Homo sapiens (human)*
 Defective Mismatch Repair Associated With MSH6 isPartOf Colorectal cancer - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Complement and coagulation cascades - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Complement and coagulation cascades - Homo sapiens (human)* isPartOf Immune System
+    <t>Complement and coagulation cascades - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Complement and coagulation cascades - Homo sapiens (human)* isPartOf Immune System
 Hemostasis isPartOf Complement and coagulation cascades - Homo sapiens (human)*
 Alternative complement activation isPartOf Complement and coagulation cascades - Homo sapiens (human)*
 Activation of C3 and C5 isPartOf Complement and coagulation cascades - Homo sapiens (human)*
@@ -483,29 +483,29 @@
 Intrinsic Pathway of Fibrin Clot Formation isPartOf Complement and coagulation cascades - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Cortisol synthesis and secretion - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mineralocorticoid biosynthesis isPartOf Cortisol synthesis and secretion - Homo sapiens (human)*
+    <t>Cortisol synthesis and secretion - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Mineralocorticoid biosynthesis isPartOf Cortisol synthesis and secretion - Homo sapiens (human)*
 Cholesterol biosynthesis via desmosterol isPartOf Cortisol synthesis and secretion - Homo sapiens (human)*
 Cholesterol biosynthesis via lathosterol isPartOf Cortisol synthesis and secretion - Homo sapiens (human)*
 Glucocorticoid biosynthesis isPartOf Cortisol synthesis and secretion - Homo sapiens (human)*
 Cortisol synthesis and secretion - Homo sapiens (human)* isPartOf Metabolism</t>
   </si>
   <si>
-    <t xml:space="preserve">Cysteine and methionine metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cysteine and methionine metabolism - Homo sapiens (human)* isPartOf Sulfur amino acid metabolism
+    <t>Cysteine and methionine metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Cysteine and methionine metabolism - Homo sapiens (human)* isPartOf Sulfur amino acid metabolism
 Cysteine formation from homocysteine isPartOf Cysteine and methionine metabolism - Homo sapiens (human)*
 Cysteine and methionine metabolism - Homo sapiens (human)* isPartOf Metabolism
 Cysteine and methionine metabolism - Homo sapiens (human)* isPartOf Metabolism of amino acids and derivatives</t>
   </si>
   <si>
-    <t xml:space="preserve">Cytokine-cytokine receptor interaction - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cytokine-cytokine receptor interaction - Homo sapiens (human)* isPartOf Cytokine Signaling in Immune system
+    <t>Cytokine-cytokine receptor interaction - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Cytokine-cytokine receptor interaction - Homo sapiens (human)* isPartOf Cytokine Signaling in Immune system
 Cytokine-cytokine receptor interaction - Homo sapiens (human)* isPartOf Immune System
 IL-6-type cytokine receptor ligand interactions isPartOf Cytokine-cytokine receptor interaction - Homo sapiens (human)*
 Cytokine-cytokine receptor interaction - Homo sapiens (human)* isPartOf IL-6-type cytokine receptor ligand interactions
@@ -514,40 +514,40 @@
 Cytokine-cytokine receptor interaction - Homo sapiens (human)* isPartOf Ligand-receptor interactions</t>
   </si>
   <si>
-    <t xml:space="preserve">Cytosolic DNA-sensing pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cytosolic DNA-sensing pathway - Homo sapiens (human)* isPartOf Cytosolic sensors of pathogen-associated DNA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D-Arginine and D-ornithine metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D-Arginine and D-ornithine metabolism - Homo sapiens (human)* isPartOf Metabolism
+    <t>Cytosolic DNA-sensing pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Cytosolic DNA-sensing pathway - Homo sapiens (human)* isPartOf Cytosolic sensors of pathogen-associated DNA</t>
+  </si>
+  <si>
+    <t>D-Arginine and D-ornithine metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>D-Arginine and D-ornithine metabolism - Homo sapiens (human)* isPartOf Metabolism
 D-Arginine and D-ornithine metabolism - Homo sapiens (human)* isPartOf Metabolism of amino acids and derivatives</t>
   </si>
   <si>
-    <t xml:space="preserve">D-Glutamine and D-glutamate metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D-Glutamine and D-glutamate metabolism - Homo sapiens (human)* isPartOf Metabolism of amino acids and derivatives
+    <t>D-Glutamine and D-glutamate metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>D-Glutamine and D-glutamate metabolism - Homo sapiens (human)* isPartOf Metabolism of amino acids and derivatives
 D-Glutamine and D-glutamate metabolism - Homo sapiens (human)* isPartOf Metabolism
 D-Glutamine and D-glutamate metabolism - Homo sapiens (human)* isPartOf Amino acid synthesis and interconversion (transamination)</t>
   </si>
   <si>
-    <t xml:space="preserve">DNA replication - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DNA replication - Homo sapiens (human) equivalentTo DNA Replication</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dilated cardiomyopathy (DCM) - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dopaminergic synapse - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dopamine receptors isPartOf Dopaminergic synapse - Homo sapiens (human)*
+    <t>DNA replication - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>DNA replication - Homo sapiens (human) equivalentTo DNA Replication</t>
+  </si>
+  <si>
+    <t>Dilated cardiomyopathy (DCM) - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Dopaminergic synapse - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Dopamine receptors isPartOf Dopaminergic synapse - Homo sapiens (human)*
 Enzymatic degradation of dopamine by COMT isPartOf Dopaminergic synapse - Homo sapiens (human)*
 Activation of AMPA receptors isPartOf Dopaminergic synapse - Homo sapiens (human)*
 Enzymatic degradation of Dopamine by monoamine oxidase isPartOf Dopaminergic synapse - Homo sapiens (human)*
@@ -555,59 +555,59 @@
 Dopamine clearance from the synaptic cleft isPartOf Dopaminergic synapse - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Drug metabolism - cytochrome P450 - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ethanol oxidation isPartOf Drug metabolism - cytochrome P450 - Homo sapiens (human)*
+    <t>Drug metabolism - cytochrome P450 - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Ethanol oxidation isPartOf Drug metabolism - cytochrome P450 - Homo sapiens (human)*
 Biogenic amines are oxidatively deaminated to aldehydes by MAOA and MAOB isPartOf Drug metabolism - cytochrome P450 - Homo sapiens (human)*
 Drug metabolism - cytochrome P450 - Homo sapiens (human)* isPartOf Metabolism
 CYP2E1 reactions isPartOf Drug metabolism - cytochrome P450 - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Drug metabolism - other enzymes - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drug metabolism - other enzymes - Homo sapiens (human)* isPartOf Metabolism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECM-receptor interaction - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECM proteoglycans isPartOf ECM-receptor interaction - Homo sapiens (human)*
+    <t>Drug metabolism - other enzymes - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Drug metabolism - other enzymes - Homo sapiens (human)* isPartOf Metabolism</t>
+  </si>
+  <si>
+    <t>ECM-receptor interaction - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>ECM proteoglycans isPartOf ECM-receptor interaction - Homo sapiens (human)*
 ECM-receptor interaction - Homo sapiens (human)* isPartOf Extracellular matrix organization
 Laminin interactions isPartOf ECM-receptor interaction - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">EGFR tyrosine kinase inhibitor resistance - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endocrine and other factor-regulated calcium reabsorption - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endocrine resistance - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endocytosis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endosomal Sorting Complex Required For Transport (ESCRT) isPartOf Endocytosis - Homo sapiens (human)*
+    <t>EGFR tyrosine kinase inhibitor resistance - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Endocrine and other factor-regulated calcium reabsorption - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Endocrine resistance - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Endocytosis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Endosomal Sorting Complex Required For Transport (ESCRT) isPartOf Endocytosis - Homo sapiens (human)*
 Cargo recognition for clathrin-mediated endocytosis isPartOf Endocytosis - Homo sapiens (human)*
 Clathrin-mediated endocytosis isPartOf Endocytosis - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Endometrial cancer - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Epithelial cell signaling in Helicobacter pylori infection - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Epstein-Barr virus infection - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ErbB signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PI3K events in ERBB4 signaling isPartOf ErbB signaling pathway - Homo sapiens (human)*
+    <t>Endometrial cancer - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Epithelial cell signaling in Helicobacter pylori infection - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Epstein-Barr virus infection - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>ErbB signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>PI3K events in ERBB4 signaling isPartOf ErbB signaling pathway - Homo sapiens (human)*
 Signaling by ERBB4 isPartOf ErbB signaling pathway - Homo sapiens (human)*
 GRB2 events in ERBB2 signaling isPartOf ErbB signaling pathway - Homo sapiens (human)*
 ERBB2 Regulates Cell Motility isPartOf ErbB signaling pathway - Homo sapiens (human)*
@@ -624,44 +624,44 @@
 PLCG1 events in ERBB2 signaling isPartOf ErbB signaling pathway - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Estrogen signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ether lipid metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ether lipid metabolism - Homo sapiens (human)* isPartOf Metabolism of lipids
+    <t>Estrogen signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Ether lipid metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Ether lipid metabolism - Homo sapiens (human)* isPartOf Metabolism of lipids
 Phospholipid metabolism isPartOf Ether lipid metabolism - Homo sapiens (human)*
 Ether lipid metabolism - Homo sapiens (human)* isPartOf Metabolism</t>
   </si>
   <si>
-    <t xml:space="preserve">Fanconi anemia pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fanconi anemia pathway - Homo sapiens (human) equivalentTo Fanconi Anemia Pathway</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fat digestion and absorption - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digestion of dietary lipid isPartOf Fat digestion and absorption - Homo sapiens (human)*
+    <t>Fanconi anemia pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Fanconi anemia pathway - Homo sapiens (human) equivalentTo Fanconi Anemia Pathway</t>
+  </si>
+  <si>
+    <t>Fat digestion and absorption - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Digestion of dietary lipid isPartOf Fat digestion and absorption - Homo sapiens (human)*
 Intestinal lipid absorption isPartOf Fat digestion and absorption - Homo sapiens (human)*
 Fat digestion and absorption - Homo sapiens (human)* isPartOf Intestinal absorption
 Fat digestion and absorption - Homo sapiens (human)* isPartOf Digestion and absorption</t>
   </si>
   <si>
-    <t xml:space="preserve">Fatty acid biosynthesis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fatty acid biosynthesis - Homo sapiens (human)* isPartOf Metabolism
+    <t>Fatty acid biosynthesis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Fatty acid biosynthesis - Homo sapiens (human)* isPartOf Metabolism
 Fatty acyl-CoA biosynthesis isPartOf Fatty acid biosynthesis - Homo sapiens (human)*
 Fatty acid biosynthesis - Homo sapiens (human)* isPartOf Fatty acyl-CoA biosynthesis</t>
   </si>
   <si>
-    <t xml:space="preserve">Fatty acid degradation - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beta oxidation of decanoyl-CoA to octanoyl-CoA-CoA isPartOf Fatty acid degradation - Homo sapiens (human)*
+    <t>Fatty acid degradation - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Beta oxidation of decanoyl-CoA to octanoyl-CoA-CoA isPartOf Fatty acid degradation - Homo sapiens (human)*
 Beta oxidation of hexanoyl-CoA to butanoyl-CoA isPartOf Fatty acid degradation - Homo sapiens (human)*
 Beta oxidation of octanoyl-CoA to hexanoyl-CoA isPartOf Fatty acid degradation - Homo sapiens (human)*
 Fatty acid degradation - Homo sapiens (human)* isPartOf Metabolism of lipids
@@ -674,106 +674,106 @@
 Beta oxidation of palmitoyl-CoA to myristoyl-CoA isPartOf Fatty acid degradation - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Fatty acid elongation - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fatty acid elongation - Homo sapiens (human)* isPartOf Metabolism
+    <t>Fatty acid elongation - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Fatty acid elongation - Homo sapiens (human)* isPartOf Metabolism
 Fatty acid elongation - Homo sapiens (human)* isPartOf Metabolism of lipids
 Fatty acid elongation - Homo sapiens (human)* isPartOf Fatty acid metabolism
 Fatty acid elongation - Homo sapiens (human)* isPartOf Fatty acids</t>
   </si>
   <si>
-    <t xml:space="preserve">Fatty acid metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fatty acid metabolism - Homo sapiens (human) equivalentTo Fatty acid metabolism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fatty acid metabolism - Homo sapiens (human)* isPartOf Metabolism of lipids
+    <t>Fatty acid metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Fatty acid metabolism - Homo sapiens (human) equivalentTo Fatty acid metabolism</t>
+  </si>
+  <si>
+    <t>Fatty acid metabolism - Homo sapiens (human)* isPartOf Metabolism of lipids
 Fatty acid metabolism - Homo sapiens (human)* isPartOf Metabolism</t>
   </si>
   <si>
-    <t xml:space="preserve">Fc epsilon RI signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fc epsilon RI signaling pathway - Homo sapiens (human) equivalentTo Fc epsilon receptor (FCERI) signaling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phospho-PLA2 pathway isPartOf Fc epsilon RI signaling pathway - Homo sapiens (human)*
+    <t>Fc epsilon RI signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Fc epsilon RI signaling pathway - Homo sapiens (human) equivalentTo Fc epsilon receptor (FCERI) signaling</t>
+  </si>
+  <si>
+    <t>phospho-PLA2 pathway isPartOf Fc epsilon RI signaling pathway - Homo sapiens (human)*
 Fc epsilon receptor (FCERI) signaling isPartOf Fc epsilon RI signaling pathway - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Fc gamma R-mediated phagocytosis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fc gamma R-mediated phagocytosis - Homo sapiens (human) equivalentTo Fcgamma receptor (FCGR) dependent phagocytosis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ferroptosis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Defective SLC11A2 causes hypochromic microcytic anemia, with iron overload 1 (AHMIO1) isPartOf Ferroptosis - Homo sapiens (human)*
+    <t>Fc gamma R-mediated phagocytosis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Fc gamma R-mediated phagocytosis - Homo sapiens (human) equivalentTo Fcgamma receptor (FCGR) dependent phagocytosis</t>
+  </si>
+  <si>
+    <t>Ferroptosis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Defective SLC11A2 causes hypochromic microcytic anemia, with iron overload 1 (AHMIO1) isPartOf Ferroptosis - Homo sapiens (human)*
 Defective GCLC causes Hemolytic anemia due to gamma-glutamylcysteine synthetase deficiency (HAGGSD) isPartOf Ferroptosis - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Fluid shear stress and atherosclerosis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Focal adhesion - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laminin interactions isPartOf Focal adhesion - Homo sapiens (human)*
+    <t>Fluid shear stress and atherosclerosis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Focal adhesion - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Laminin interactions isPartOf Focal adhesion - Homo sapiens (human)*
 Localization of the PINCH-ILK-PARVIN complex to focal adhesions isPartOf Focal adhesion - Homo sapiens (human)*
 Integrin signaling isPartOf Focal adhesion - Homo sapiens (human)*
 Non-integrin membrane-ECM interactions isPartOf Focal adhesion - Homo sapiens (human)*
 Integrin alphaIIb beta3 signaling isPartOf Focal adhesion - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Folate biosynthesis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Folate biosynthesis - Homo sapiens (human)* isPartOf Metabolism
+    <t>Folate biosynthesis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Folate biosynthesis - Homo sapiens (human)* isPartOf Metabolism
 Molybdenum cofactor biosynthesis isPartOf Folate biosynthesis - Homo sapiens (human)*
 Folate biosynthesis - Homo sapiens (human)* isPartOf Metabolism of water-soluble vitamins and cofactors
 Folate biosynthesis - Homo sapiens (human)* isPartOf Metabolism of vitamins and cofactors
 Folate biosynthesis - Homo sapiens (human)* isPartOf Metabolism</t>
   </si>
   <si>
-    <t xml:space="preserve">FoxO signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AKT-mediated inactivation of FOXO1A isPartOf FoxO signaling pathway - Homo sapiens (human)*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fructose and mannose metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fructose biosynthesis isPartOf Fructose and mannose metabolism - Homo sapiens (human)*
+    <t>FoxO signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>AKT-mediated inactivation of FOXO1A isPartOf FoxO signaling pathway - Homo sapiens (human)*</t>
+  </si>
+  <si>
+    <t>Fructose and mannose metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Fructose biosynthesis isPartOf Fructose and mannose metabolism - Homo sapiens (human)*
 Synthesis of GDP-mannose isPartOf Fructose and mannose metabolism - Homo sapiens (human)*
 Fructose and mannose metabolism - Homo sapiens (human)* isPartOf Metabolism
 Fructose catabolism isPartOf Fructose and mannose metabolism - Homo sapiens (human)*
 Fructose metabolism isPartOf Fructose and mannose metabolism - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">GABAergic synapse - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GABA receptor activation isPartOf GABAergic synapse - Homo sapiens (human)*
+    <t>GABAergic synapse - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>GABA receptor activation isPartOf GABAergic synapse - Homo sapiens (human)*
 GABA B receptor activation isPartOf GABAergic synapse - Homo sapiens (human)*
 GABA A (rho) receptor activation isPartOf GABAergic synapse - Homo sapiens (human)*
 GABA A receptor activation isPartOf GABAergic synapse - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Galactose metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Galactose catabolism isPartOf Galactose metabolism - Homo sapiens (human)*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gap junction - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gap junction degradation isPartOf Gap junction - Homo sapiens (human)*
+    <t>Galactose metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Galactose catabolism isPartOf Galactose metabolism - Homo sapiens (human)*</t>
+  </si>
+  <si>
+    <t>Gap junction - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Gap junction degradation isPartOf Gap junction - Homo sapiens (human)*
 c-src mediated regulation of Cx43 function and closure of gap junctions isPartOf Gap junction - Homo sapiens (human)*
 Gap junction trafficking isPartOf Gap junction - Homo sapiens (human)*
 Formation of annular gap junctions isPartOf Gap junction - Homo sapiens (human)*
@@ -782,25 +782,25 @@
 Regulation of gap junction activity isPartOf Gap junction - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Gastric acid secretion - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gastric cancer - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glioma - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glucagon signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glucagon signaling pathway - Homo sapiens (human) equivalentTo Glucagon signaling in metabolic regulation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glutamatergic synapse - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activation of kainate receptors upon glutamate binding isPartOf Glutamatergic synapse - Homo sapiens (human)*
+    <t>Gastric acid secretion - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Gastric cancer - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Glioma - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Glucagon signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Glucagon signaling pathway - Homo sapiens (human) equivalentTo Glucagon signaling in metabolic regulation</t>
+  </si>
+  <si>
+    <t>Glutamatergic synapse - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Activation of kainate receptors upon glutamate binding isPartOf Glutamatergic synapse - Homo sapiens (human)*
 Glutamatergic synapse - Homo sapiens (human)* isPartOf Neurotransmitter uptake and metabolism In glial cells
 Unblocking of NMDA receptor, glutamate binding and activation isPartOf Glutamatergic synapse - Homo sapiens (human)*
 Activation of AMPA receptors isPartOf Glutamatergic synapse - Homo sapiens (human)*
@@ -809,25 +809,25 @@
 Neurotransmitter uptake and metabolism In glial cells isPartOf Glutamatergic synapse - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Glutathione metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glutathione metabolism - Homo sapiens (human) equivalentTo Glutathione synthesis and recycling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glycerolipid metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glycerolipid metabolism - Homo sapiens (human)* isPartOf Metabolism of lipids
+    <t>Glutathione metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Glutathione metabolism - Homo sapiens (human) equivalentTo Glutathione synthesis and recycling</t>
+  </si>
+  <si>
+    <t>Glycerolipid metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Glycerolipid metabolism - Homo sapiens (human)* isPartOf Metabolism of lipids
 Glycerolipid metabolism - Homo sapiens (human)* isPartOf Metabolism
 Acyl chain remodeling of DAG and TAG isPartOf Glycerolipid metabolism - Homo sapiens (human)*
 Glycerophospholipid catabolism isPartOf Glycerolipid metabolism - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Glycerophospholipid metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acyl chain remodelling of PI isPartOf Glycerophospholipid metabolism - Homo sapiens (human)*
+    <t>Glycerophospholipid metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Acyl chain remodelling of PI isPartOf Glycerophospholipid metabolism - Homo sapiens (human)*
 Synthesis of PS isPartOf Glycerophospholipid metabolism - Homo sapiens (human)*
 Glycerophospholipid metabolism - Homo sapiens (human)* isPartOf Metabolism of lipids
 Synthesis of PE isPartOf Glycerophospholipid metabolism - Homo sapiens (human)*
@@ -838,236 +838,236 @@
 Acyl chain remodelling of PC isPartOf Glycerophospholipid metabolism - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Glycine, serine and threonine metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glycine, serine and threonine metabolism - Homo sapiens (human)* isPartOf Metabolism
+    <t>Glycine, serine and threonine metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Glycine, serine and threonine metabolism - Homo sapiens (human)* isPartOf Metabolism
 Glycine, serine and threonine metabolism - Homo sapiens (human)* isPartOf Amine Oxidase reactions
 Glycine degradation isPartOf Glycine, serine and threonine metabolism - Homo sapiens (human)*
 Glycine, serine and threonine metabolism - Homo sapiens (human)* isPartOf Amino acid synthesis and interconversion (transamination)
 Glycine, serine and threonine metabolism - Homo sapiens (human)* isPartOf Metabolism of amino acids and derivatives</t>
   </si>
   <si>
-    <t xml:space="preserve">Glycolysis / Gluconeogenesis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glycolysis / Gluconeogenesis - Homo sapiens (human)* isPartOf Glucose metabolism
+    <t>Glycolysis / Gluconeogenesis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Glycolysis / Gluconeogenesis - Homo sapiens (human)* isPartOf Glucose metabolism
 Gluconeogenesis isPartOf Glycolysis / Gluconeogenesis - Homo sapiens (human)*
 Glycolysis / Gluconeogenesis - Homo sapiens (human)* isPartOf Metabolism
 Glycolysis / Gluconeogenesis - Homo sapiens (human)* isPartOf Metabolism of carbohydrates
 Glycolysis isPartOf Glycolysis / Gluconeogenesis - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Glycosaminoglycan biosynthesis - chondroitin sulfate / dermatan sulfate - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glycosaminoglycan biosynthesis - chondroitin sulfate / dermatan sulfate - Homo sapiens (human)* isPartOf Metabolism
+    <t>Glycosaminoglycan biosynthesis - chondroitin sulfate / dermatan sulfate - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Glycosaminoglycan biosynthesis - chondroitin sulfate / dermatan sulfate - Homo sapiens (human)* isPartOf Metabolism
 Chondroitin sulfate biosynthesis isPartOf Glycosaminoglycan biosynthesis - chondroitin sulfate / dermatan sulfate - Homo sapiens (human)*
 Glycosaminoglycan metabolism isPartOf Glycosaminoglycan biosynthesis - chondroitin sulfate / dermatan sulfate - Homo sapiens (human)*
 Chondroitin sulfate/dermatan sulfate metabolism isPartOf Glycosaminoglycan biosynthesis - chondroitin sulfate / dermatan sulfate - Homo sapiens (human)*
 Dermatan sulfate biosynthesis isPartOf Glycosaminoglycan biosynthesis - chondroitin sulfate / dermatan sulfate - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Glycosaminoglycan biosynthesis - heparan sulfate / heparin - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glycosaminoglycan biosynthesis - heparan sulfate / heparin - Homo sapiens (human)* isPartOf Metabolism
+    <t>Glycosaminoglycan biosynthesis - heparan sulfate / heparin - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Glycosaminoglycan biosynthesis - heparan sulfate / heparin - Homo sapiens (human)* isPartOf Metabolism
 Glycosaminoglycan biosynthesis - heparan sulfate / heparin - Homo sapiens (human)* isPartOf Glycosaminoglycan metabolism
 Heparan sulfate/heparin (HS-GAG) metabolism isPartOf Glycosaminoglycan biosynthesis - heparan sulfate / heparin - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Glycosaminoglycan biosynthesis - keratan sulfate - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glycosaminoglycan biosynthesis - keratan sulfate - Homo sapiens (human)* isPartOf Glycosaminoglycan metabolism
+    <t>Glycosaminoglycan biosynthesis - keratan sulfate - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Glycosaminoglycan biosynthesis - keratan sulfate - Homo sapiens (human)* isPartOf Glycosaminoglycan metabolism
 Glycosaminoglycan biosynthesis - keratan sulfate - Homo sapiens (human)* isPartOf Metabolism
 Keratan sulfate biosynthesis isPartOf Glycosaminoglycan biosynthesis - keratan sulfate - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Glycosaminoglycan degradation - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glycosaminoglycan degradation - Homo sapiens (human)* isPartOf Metabolism
+    <t>Glycosaminoglycan degradation - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Glycosaminoglycan degradation - Homo sapiens (human)* isPartOf Metabolism
 Glycosaminoglycan degradation - Homo sapiens (human)* isPartOf Glycosaminoglycan metabolism</t>
   </si>
   <si>
-    <t xml:space="preserve">Glycosphingolipid biosynthesis - ganglio series - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glycosphingolipid biosynthesis - globo and isoglobo series - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glycosphingolipid biosynthesis - globo and isoglobo series - Homo sapiens (human)* isPartOf Sphingolipid metabolism
+    <t>Glycosphingolipid biosynthesis - ganglio series - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Glycosphingolipid biosynthesis - globo and isoglobo series - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Glycosphingolipid biosynthesis - globo and isoglobo series - Homo sapiens (human)* isPartOf Sphingolipid metabolism
 Glycosphingolipid biosynthesis - globo and isoglobo series - Homo sapiens (human)* isPartOf Glycosphingolipid metabolism
 Glycosphingolipid biosynthesis - globo and isoglobo series - Homo sapiens (human)* isPartOf Metabolism of lipids</t>
   </si>
   <si>
-    <t xml:space="preserve">Glycosphingolipid biosynthesis - lacto and neolacto series - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glycosphingolipid biosynthesis - lacto and neolacto series - Homo sapiens (human)* isPartOf Metabolism of lipids
+    <t>Glycosphingolipid biosynthesis - lacto and neolacto series - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Glycosphingolipid biosynthesis - lacto and neolacto series - Homo sapiens (human)* isPartOf Metabolism of lipids
 Glycosphingolipid biosynthesis - lacto and neolacto series - Homo sapiens (human)* isPartOf Glycosphingolipid metabolism
 Glycosphingolipid biosynthesis - lacto and neolacto series - Homo sapiens (human)* isPartOf Sphingolipid metabolism</t>
   </si>
   <si>
-    <t xml:space="preserve">Glycosylphosphatidylinositol (GPI)-anchor biosynthesis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glycosylphosphatidylinositol (GPI)-anchor biosynthesis - Homo sapiens (human) equivalentTo Synthesis of glycosylphosphatidylinositol (GPI)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Synthesis of glycosylphosphatidylinositol (GPI) isPartOf Glycosylphosphatidylinositol (GPI)-anchor biosynthesis - Homo sapiens (human)*
+    <t>Glycosylphosphatidylinositol (GPI)-anchor biosynthesis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Glycosylphosphatidylinositol (GPI)-anchor biosynthesis - Homo sapiens (human) equivalentTo Synthesis of glycosylphosphatidylinositol (GPI)</t>
+  </si>
+  <si>
+    <t>Synthesis of glycosylphosphatidylinositol (GPI) isPartOf Glycosylphosphatidylinositol (GPI)-anchor biosynthesis - Homo sapiens (human)*
 Post-translational modification: synthesis of GPI-anchored proteins isPartOf Glycosylphosphatidylinositol (GPI)-anchor biosynthesis - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Glyoxylate and dicarboxylate metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glyoxylate metabolism and glycine degradation isPartOf Glyoxylate and dicarboxylate metabolism - Homo sapiens (human)*
+    <t>Glyoxylate and dicarboxylate metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Glyoxylate metabolism and glycine degradation isPartOf Glyoxylate and dicarboxylate metabolism - Homo sapiens (human)*
 Glyoxylate and dicarboxylate metabolism - Homo sapiens (human)* isPartOf Metabolism
 Glyoxylate and dicarboxylate metabolism - Homo sapiens (human)* isPartOf Metabolism of amino acids and derivatives</t>
   </si>
   <si>
-    <t xml:space="preserve">GnRH signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Graft-versus-host disease - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Graft-versus-host disease - Homo sapiens (human)* isPartOf Adaptive Immune System
+    <t>GnRH signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Graft-versus-host disease - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Graft-versus-host disease - Homo sapiens (human)* isPartOf Adaptive Immune System
 Graft-versus-host disease - Homo sapiens (human)* isPartOf Immune System</t>
   </si>
   <si>
-    <t xml:space="preserve">HIF-1 signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HTLV-I infection - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hedgehog signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hedgehog signaling pathway - Homo sapiens (human) equivalentTo Signaling by Hedgehog</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hedgehog 'on' state isPartOf Hedgehog signaling pathway - Homo sapiens (human)*
+    <t>HIF-1 signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>HTLV-I infection - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Hedgehog signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Hedgehog signaling pathway - Homo sapiens (human) equivalentTo Signaling by Hedgehog</t>
+  </si>
+  <si>
+    <t>Hedgehog 'on' state isPartOf Hedgehog signaling pathway - Homo sapiens (human)*
 Hedgehog ligand biogenesis isPartOf Hedgehog signaling pathway - Homo sapiens (human)*
 Signaling by Hedgehog isPartOf Hedgehog signaling pathway - Homo sapiens (human)*
 Hedgehog 'off' state isPartOf Hedgehog signaling pathway - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Hematopoietic cell lineage - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hepatitis B - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hepatitis C - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hepatocellular carcinoma - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Herpes simplex infection - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hippo signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hippo signaling pathway - Homo sapiens (human) equivalentTo Signaling by Hippo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hippo signaling pathway - multiple species - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hippo signaling pathway - multiple species - Homo sapiens (human) equivalentTo Signaling by Hippo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Histidine metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Histidine metabolism - Homo sapiens (human)* isPartOf Histidine, lysine, phenylalanine, tyrosine, proline and tryptophan catabolism
+    <t>Hematopoietic cell lineage - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Hepatitis B - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Hepatitis C - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Hepatocellular carcinoma - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Herpes simplex infection - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Hippo signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Hippo signaling pathway - Homo sapiens (human) equivalentTo Signaling by Hippo</t>
+  </si>
+  <si>
+    <t>Hippo signaling pathway - multiple species - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Hippo signaling pathway - multiple species - Homo sapiens (human) equivalentTo Signaling by Hippo</t>
+  </si>
+  <si>
+    <t>Histidine metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Histidine metabolism - Homo sapiens (human)* isPartOf Histidine, lysine, phenylalanine, tyrosine, proline and tryptophan catabolism
 Histidine metabolism - Homo sapiens (human)* isPartOf Metabolism
 Histidine metabolism - Homo sapiens (human)* isPartOf Amine Oxidase reactions
 Histidine metabolism - Homo sapiens (human)* isPartOf Metabolism of amino acids and derivatives
 Histidine catabolism isPartOf Histidine metabolism - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Homologous recombination - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Homology Directed Repair isPartOf Homologous recombination - Homo sapiens (human)*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Human papillomavirus infection - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Huntington's disease - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hypertrophic cardiomyopathy (HCM) - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IL-17 signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IL-17 signaling pathway - Homo sapiens (human) equivalentTo Interleukin-17 signaling </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IL-17 signaling pathway - Homo sapiens (human)* isPartOf Cytokine Signaling in Immune system
+    <t>Homologous recombination - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Homology Directed Repair isPartOf Homologous recombination - Homo sapiens (human)*</t>
+  </si>
+  <si>
+    <t>Human papillomavirus infection - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Huntington's disease - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Hypertrophic cardiomyopathy (HCM) - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>IL-17 signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>IL-17 signaling pathway - Homo sapiens (human) equivalentTo Interleukin-17 signaling </t>
+  </si>
+  <si>
+    <t>IL-17 signaling pathway - Homo sapiens (human)* isPartOf Cytokine Signaling in Immune system
 IL-17 signaling pathway - Homo sapiens (human)* isPartOf Signaling by Interleukins
 IL-17 signaling pathway - Homo sapiens (human)* isPartOf Immune System</t>
   </si>
   <si>
-    <t xml:space="preserve">Inflammatory bowel disease (IBD) - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inflammatory mediator regulation of TRP channels - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Influenza A - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Influenza Virus Induced Apoptosis isPartOf Influenza A - Homo sapiens (human)*
+    <t>Inflammatory bowel disease (IBD) - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Inflammatory mediator regulation of TRP channels - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Influenza A - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Influenza Virus Induced Apoptosis isPartOf Influenza A - Homo sapiens (human)*
 Influenza Life Cycle isPartOf Influenza A - Homo sapiens (human)*
 Influenza A - Homo sapiens (human)* isPartOf Influenza Life Cycle
 Influenza A - Homo sapiens (human)* isPartOf Influenza Infection
 Influenza Infection isPartOf Influenza A - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Inositol phosphate metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inositol phosphate metabolism - Homo sapiens (human) equivalentTo Inositol phosphate metabolism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Insulin resistance - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Insulin secretion - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Insulin secretion - Homo sapiens (human) equivalentTo Regulation of insulin secretion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Insulin signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Signaling by Insulin receptor isPartOf Insulin signaling pathway - Homo sapiens (human)*
+    <t>Inositol phosphate metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Inositol phosphate metabolism - Homo sapiens (human) equivalentTo Inositol phosphate metabolism</t>
+  </si>
+  <si>
+    <t>Insulin resistance - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Insulin secretion - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Insulin secretion - Homo sapiens (human) equivalentTo Regulation of insulin secretion</t>
+  </si>
+  <si>
+    <t>Insulin signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Signaling by Insulin receptor isPartOf Insulin signaling pathway - Homo sapiens (human)*
 Insulin receptor signalling cascade isPartOf Insulin signaling pathway - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Intestinal immune network for IgA production - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intestinal immune network for IgA production - Homo sapiens (human)* isPartOf Immune System
+    <t>Intestinal immune network for IgA production - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Intestinal immune network for IgA production - Homo sapiens (human)* isPartOf Immune System
 Intestinal immune network for IgA production - Homo sapiens (human)* isPartOf Adaptive Immune System</t>
   </si>
   <si>
-    <t xml:space="preserve">Jak-STAT signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regulation of IFNG signaling isPartOf Jak-STAT signaling pathway - Homo sapiens (human)*
+    <t>Jak-STAT signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Regulation of IFNG signaling isPartOf Jak-STAT signaling pathway - Homo sapiens (human)*
 Interleukin-21 signaling isPartOf Jak-STAT signaling pathway - Homo sapiens (human)*
 Interleukin-15 signaling isPartOf Jak-STAT signaling pathway - Homo sapiens (human)*
 Interleukin-9 signaling isPartOf Jak-STAT signaling pathway - Homo sapiens (human)*
@@ -1076,67 +1076,67 @@
 Interleukin-23 signaling isPartOf Jak-STAT signaling pathway - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Kaposi's sarcoma-associated herpesvirus infection - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Legionellosis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leishmaniasis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leukocyte transendothelial migration - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linoleic acid metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linoleic acid metabolism - Homo sapiens (human) equivalentTo Linoleic acid (LA) metabolism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linoleic acid metabolism - Homo sapiens (human)* isPartOf Metabolism
+    <t>Kaposi's sarcoma-associated herpesvirus infection - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Legionellosis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Leishmaniasis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Leukocyte transendothelial migration - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Linoleic acid metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Linoleic acid metabolism - Homo sapiens (human) equivalentTo Linoleic acid (LA) metabolism</t>
+  </si>
+  <si>
+    <t>Linoleic acid metabolism - Homo sapiens (human)* isPartOf Metabolism
 Linoleic acid metabolism - Homo sapiens (human)* isPartOf Metabolism of lipids</t>
   </si>
   <si>
-    <t xml:space="preserve">Lipoic acid metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lipoic acid metabolism - Homo sapiens (human)* isPartOf Fatty acid metabolism
+    <t>Lipoic acid metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Lipoic acid metabolism - Homo sapiens (human)* isPartOf Fatty acid metabolism
 Lipoic acid metabolism - Homo sapiens (human)* isPartOf Metabolism</t>
   </si>
   <si>
-    <t xml:space="preserve">Long-term depression - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Long-term potentiation - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Longevity regulating pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Longevity regulating pathway - multiple species - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lysine degradation - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lysine degradation - Homo sapiens (human) equivalentTo Lysine catabolism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lysosome - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lysosomal oligosaccharide catabolism isPartOf Lysosome - Homo sapiens (human)*
+    <t>Long-term depression - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Long-term potentiation - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Longevity regulating pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Longevity regulating pathway - multiple species - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Lysine degradation - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Lysine degradation - Homo sapiens (human) equivalentTo Lysine catabolism</t>
+  </si>
+  <si>
+    <t>Lysosome - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Lysosomal oligosaccharide catabolism isPartOf Lysosome - Homo sapiens (human)*
 Lysosome Vesicle Biogenesis isPartOf Lysosome - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">MAPK signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAPK signaling pathway - Homo sapiens (human) equivalentTo MAPK family signaling cascades</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERK/MAPK targets isPartOf MAPK signaling pathway - Homo sapiens (human)*
+    <t>MAPK signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>MAPK signaling pathway - Homo sapiens (human) equivalentTo MAPK family signaling cascades</t>
+  </si>
+  <si>
+    <t>ERK/MAPK targets isPartOf MAPK signaling pathway - Homo sapiens (human)*
 MAPK1/MAPK3 signaling isPartOf MAPK signaling pathway - Homo sapiens (human)*
 Negative regulation of MAPK pathway isPartOf MAPK signaling pathway - Homo sapiens (human)*
 Negative feedback regulation of MAPK pathway isPartOf MAPK signaling pathway - Homo sapiens (human)*
@@ -1154,255 +1154,255 @@
 Gastrin-CREB signalling pathway via PKC and MAPK isPartOf MAPK signaling pathway - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Malaria - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mannose type O-glycan biosynthesis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Termination of O-glycan biosynthesis isPartOf Mannose type O-glycan biosynthesis - Homo sapiens (human)*
+    <t>Malaria - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Mannose type O-glycan biosynthesis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Termination of O-glycan biosynthesis isPartOf Mannose type O-glycan biosynthesis - Homo sapiens (human)*
 O-linked glycosylation isPartOf Mannose type O-glycan biosynthesis - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Maturity onset diabetes of the young - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Defective GCK causes maturity-onset diabetes of the young 2 (MODY2) isPartOf Maturity onset diabetes of the young - Homo sapiens (human)*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Measles - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Melanogenesis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Melanogenesis - Homo sapiens (human) equivalentTo Melanin biosynthesis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Melanin biosynthesis isPartOf Melanogenesis - Homo sapiens (human)*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Melanoma - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metabolic pathways - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metabolic pathways - Homo sapiens (human) equivalentTo Metabolism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metabolism of xenobiotics by cytochrome P450 - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metabolism of xenobiotics by cytochrome P450 - Homo sapiens (human)* isPartOf Xenobiotics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MicroRNAs in cancer - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mineral absorption - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mineral absorption - Homo sapiens (human)* isPartOf Intestinal absorption
+    <t>Maturity onset diabetes of the young - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Defective GCK causes maturity-onset diabetes of the young 2 (MODY2) isPartOf Maturity onset diabetes of the young - Homo sapiens (human)*</t>
+  </si>
+  <si>
+    <t>Measles - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Melanogenesis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Melanogenesis - Homo sapiens (human) equivalentTo Melanin biosynthesis</t>
+  </si>
+  <si>
+    <t>Melanin biosynthesis isPartOf Melanogenesis - Homo sapiens (human)*</t>
+  </si>
+  <si>
+    <t>Melanoma - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Metabolic pathways - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Metabolic pathways - Homo sapiens (human) equivalentTo Metabolism</t>
+  </si>
+  <si>
+    <t>Metabolism of xenobiotics by cytochrome P450 - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Metabolism of xenobiotics by cytochrome P450 - Homo sapiens (human)* isPartOf Xenobiotics</t>
+  </si>
+  <si>
+    <t>MicroRNAs in cancer - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Mineral absorption - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Mineral absorption - Homo sapiens (human)* isPartOf Intestinal absorption
 Mineral absorption - Homo sapiens (human)* isPartOf Digestion and absorption
 Mineral absorption - Homo sapiens (human)* isPartOf Transport of small molecules</t>
   </si>
   <si>
-    <t xml:space="preserve">Mismatch repair - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mismatch repair - Homo sapiens (human) equivalentTo Mismatch Repair</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mitophagy - animal - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mitophagy - animal - Homo sapiens (human) equivalentTo Mitophagy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Morphine addiction - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mucin type O-glycan biosynthesis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N-Glycan biosynthesis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N-glycan trimming and elongation in the cis-Golgi isPartOf N-Glycan biosynthesis - Homo sapiens (human)*
+    <t>Mismatch repair - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Mismatch repair - Homo sapiens (human) equivalentTo Mismatch Repair</t>
+  </si>
+  <si>
+    <t>Mitophagy - animal - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Mitophagy - animal - Homo sapiens (human) equivalentTo Mitophagy</t>
+  </si>
+  <si>
+    <t>Morphine addiction - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Mucin type O-glycan biosynthesis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>N-Glycan biosynthesis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>N-glycan trimming and elongation in the cis-Golgi isPartOf N-Glycan biosynthesis - Homo sapiens (human)*
 N-Glycan antennae elongation isPartOf N-Glycan biosynthesis - Homo sapiens (human)*
 N-glycan antennae elongation in the medial/trans-Golgi isPartOf N-Glycan biosynthesis - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">NF-kappa B signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TNFR1-induced NFkappaB signaling pathway isPartOf NF-kappa B signaling pathway - Homo sapiens (human)
+    <t>NF-kappa B signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>TNFR1-induced NFkappaB signaling pathway isPartOf NF-kappa B signaling pathway - Homo sapiens (human)
 NF-kB is activated and signals survival isPartOf NF-kappa B signaling pathway - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">NOD-like receptor signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Natural killer cell mediated cytotoxicity - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Natural killer cell mediated cytotoxicity - Homo sapiens (human)* isPartOf Immune System</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Necroptosis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Necroptosis - Homo sapiens (human) equivalentTo Regulation of necroptotic cell death</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neomycin, kanamycin and gentamicin biosynthesis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neomycin, kanamycin and gentamicin biosynthesis - Homo sapiens (human)* isPartOf Metabolism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neuroactive ligand-receptor interaction - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neurotrophin signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NFG and proNGF binds to p75NTR isPartOf Neurotrophin signaling pathway - Homo sapiens (human)*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nicotinate and nicotinamide metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nicotinate and nicotinamide metabolism - Homo sapiens (human)* isPartOf Metabolism
+    <t>NOD-like receptor signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Natural killer cell mediated cytotoxicity - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Natural killer cell mediated cytotoxicity - Homo sapiens (human)* isPartOf Immune System</t>
+  </si>
+  <si>
+    <t>Necroptosis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Necroptosis - Homo sapiens (human) equivalentTo Regulation of necroptotic cell death</t>
+  </si>
+  <si>
+    <t>Neomycin, kanamycin and gentamicin biosynthesis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Neomycin, kanamycin and gentamicin biosynthesis - Homo sapiens (human)* isPartOf Metabolism</t>
+  </si>
+  <si>
+    <t>Neuroactive ligand-receptor interaction - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Neurotrophin signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>NFG and proNGF binds to p75NTR isPartOf Neurotrophin signaling pathway - Homo sapiens (human)*</t>
+  </si>
+  <si>
+    <t>Nicotinate and nicotinamide metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Nicotinate and nicotinamide metabolism - Homo sapiens (human)* isPartOf Metabolism
 Nicotinate metabolism isPartOf Nicotinate and nicotinamide metabolism - Homo sapiens (human)*
 Nicotinamide salvaging isPartOf Nicotinate and nicotinamide metabolism - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Nicotine addiction - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nitrogen metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nitrogen metabolism - Homo sapiens (human)* isPartOf Metabolism
+    <t>Nicotine addiction - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Nitrogen metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Nitrogen metabolism - Homo sapiens (human)* isPartOf Metabolism
 Nitrogen metabolism - Homo sapiens (human)* isPartOf Amino acid synthesis and interconversion (transamination)
 Nitrogen metabolism - Homo sapiens (human)* isPartOf Metabolism of amino acids and derivatives</t>
   </si>
   <si>
-    <t xml:space="preserve">Non-alcoholic fatty liver disease (NAFLD) - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-homologous end-joining - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-homologous end-joining - Homo sapiens (human) equivalentTo Nonhomologous End-Joining (NHEJ)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-small cell lung cancer - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notch signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notch signaling pathway - Homo sapiens (human) equivalentTo Signaling by NOTCH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nucleotide excision repair - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nucleotide excision repair - Homo sapiens (human) equivalentTo Nucleotide Excision Repair</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Olfactory transduction - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Olfactory transduction - Homo sapiens (human) equivalentTo Olfactory Signaling Pathway</t>
-  </si>
-  <si>
-    <t xml:space="preserve">One carbon pool by folate - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">One carbon pool by folate - Homo sapiens (human)* isPartOf Metabolism of folate and pterines
+    <t>Non-alcoholic fatty liver disease (NAFLD) - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Non-homologous end-joining - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Non-homologous end-joining - Homo sapiens (human) equivalentTo Nonhomologous End-Joining (NHEJ)</t>
+  </si>
+  <si>
+    <t>Non-small cell lung cancer - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Notch signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Notch signaling pathway - Homo sapiens (human) equivalentTo Signaling by NOTCH</t>
+  </si>
+  <si>
+    <t>Nucleotide excision repair - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Nucleotide excision repair - Homo sapiens (human) equivalentTo Nucleotide Excision Repair</t>
+  </si>
+  <si>
+    <t>Olfactory transduction - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Olfactory transduction - Homo sapiens (human) equivalentTo Olfactory Signaling Pathway</t>
+  </si>
+  <si>
+    <t>One carbon pool by folate - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>One carbon pool by folate - Homo sapiens (human)* isPartOf Metabolism of folate and pterines
 One carbon pool by folate - Homo sapiens (human)* isPartOf Metabolism
 One carbon pool by folate - Homo sapiens (human)* isPartOf Metabolism of vitamins and cofactors</t>
   </si>
   <si>
-    <t xml:space="preserve">Oocyte meiosis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Osteoclast differentiation - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other glycan degradation - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other glycan degradation - Homo sapiens (human)* isPartOf Metabolism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other types of O-glycan biosynthesis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Termination of O-glycan biosynthesis isPartOf Other types of O-glycan biosynthesis - Homo sapiens (human)*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ovarian steroidogenesis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estrogen biosynthesis isPartOf Ovarian steroidogenesis - Homo sapiens (human)*
+    <t>Oocyte meiosis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Osteoclast differentiation - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Other glycan degradation - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Other glycan degradation - Homo sapiens (human)* isPartOf Metabolism</t>
+  </si>
+  <si>
+    <t>Other types of O-glycan biosynthesis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Termination of O-glycan biosynthesis isPartOf Other types of O-glycan biosynthesis - Homo sapiens (human)*</t>
+  </si>
+  <si>
+    <t>Ovarian steroidogenesis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Estrogen biosynthesis isPartOf Ovarian steroidogenesis - Homo sapiens (human)*
 Androgen biosynthesis isPartOf Ovarian steroidogenesis - Homo sapiens (human)*
 Ovarian steroidogenesis - Homo sapiens (human)* isPartOf Metabolism</t>
   </si>
   <si>
-    <t xml:space="preserve">Oxidative phosphorylation - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oxidative phosphorylation - Homo sapiens (human)* isPartOf Metabolism
+    <t>Oxidative phosphorylation - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Oxidative phosphorylation - Homo sapiens (human)* isPartOf Metabolism
 Pyrophosphate hydrolysis isPartOf Oxidative phosphorylation - Homo sapiens (human)*
 Oxidative phosphorylation - Homo sapiens (human)* isPartOf The citric acid (TCA) cycle and respiratory electron transport
 Formation of ATP by chemiosmotic coupling isPartOf Oxidative phosphorylation - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Oxytocin signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PI3K-Akt signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PI3K-Akt signaling pathway - Homo sapiens (human) equivalentTo PI3K/AKT activation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PPAR signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pancreatic cancer - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pancreatic secretion - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pantothenate and CoA biosynthesis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coenzyme A biosynthesis isPartOf Pantothenate and CoA biosynthesis - Homo sapiens (human)*
+    <t>Oxytocin signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>PI3K-Akt signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>PI3K-Akt signaling pathway - Homo sapiens (human) equivalentTo PI3K/AKT activation</t>
+  </si>
+  <si>
+    <t>PPAR signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Pancreatic cancer - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Pancreatic secretion - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Pantothenate and CoA biosynthesis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Coenzyme A biosynthesis isPartOf Pantothenate and CoA biosynthesis - Homo sapiens (human)*
 Pantothenate and CoA biosynthesis - Homo sapiens (human)* isPartOf Metabolism of vitamins and cofactors
 Pantothenate and CoA biosynthesis - Homo sapiens (human)* isPartOf Metabolism
 Vitamin B5 (pantothenate) metabolism isPartOf Pantothenate and CoA biosynthesis - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Parkinson's disease - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Defective SLC6A3 causes Parkinsonism-dystonia infantile (PKDYS) isPartOf Parkinson's disease - Homo sapiens (human)*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pathogenic Escherichia coli infection - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pathways in cancer - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activation and oligomerization of BAK protein isPartOf Pathways in cancer - Homo sapiens (human)*
+    <t>Parkinson's disease - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Defective SLC6A3 causes Parkinsonism-dystonia infantile (PKDYS) isPartOf Parkinson's disease - Homo sapiens (human)*</t>
+  </si>
+  <si>
+    <t>Pathogenic Escherichia coli infection - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Pathways in cancer - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Activation and oligomerization of BAK protein isPartOf Pathways in cancer - Homo sapiens (human)*
 Defective Mismatch Repair Associated With MSH2 isPartOf Pathways in cancer - Homo sapiens (human)*
 AKT-mediated inactivation of FOXO1A isPartOf Pathways in cancer - Homo sapiens (human)*
 Cytochrome c-mediated apoptotic response isPartOf Pathways in cancer - Homo sapiens (human)*
@@ -1411,43 +1411,43 @@
 Activated point mutants of FGFR2 isPartOf Pathways in cancer - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Pentose and glucuronate interconversions - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Catabolism of glucuronate to xylulose-5-phosphate isPartOf Pentose and glucuronate interconversions - Homo sapiens (human)*
+    <t>Pentose and glucuronate interconversions - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Catabolism of glucuronate to xylulose-5-phosphate isPartOf Pentose and glucuronate interconversions - Homo sapiens (human)*
 Pentose and glucuronate interconversions - Homo sapiens (human)* isPartOf Metabolism</t>
   </si>
   <si>
-    <t xml:space="preserve">Pentose phosphate pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pentose phosphate pathway - Homo sapiens (human) equivalentTo Pentose phosphate pathway (hexose monophosphate shunt)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peroxisome - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peroxisomal lipid metabolism isPartOf Peroxisome - Homo sapiens (human)*
+    <t>Pentose phosphate pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Pentose phosphate pathway - Homo sapiens (human) equivalentTo Pentose phosphate pathway (hexose monophosphate shunt)</t>
+  </si>
+  <si>
+    <t>Peroxisome - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Peroxisomal lipid metabolism isPartOf Peroxisome - Homo sapiens (human)*
 NADPH regeneration isPartOf Peroxisome - Homo sapiens (human)*
 Peroxisome - Homo sapiens (human)* isPartOf Metabolism</t>
   </si>
   <si>
-    <t xml:space="preserve">Pertussis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phagosome - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phagosome - Homo sapiens (human)* isPartOf Adaptive Immune System
+    <t>Pertussis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Phagosome - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Phagosome - Homo sapiens (human)* isPartOf Adaptive Immune System
 ER-Phagosome pathway isPartOf Phagosome - Homo sapiens (human)*
 Phagosome - Homo sapiens (human)* isPartOf Immune System
 Phagosome - Homo sapiens (human)* isPartOf Innate Immune System</t>
   </si>
   <si>
-    <t xml:space="preserve">Phenylalanine metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phenylalanine metabolism - Homo sapiens (human)* isPartOf Metabolism
+    <t>Phenylalanine metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Phenylalanine metabolism - Homo sapiens (human)* isPartOf Metabolism
 Phenylalanine metabolism - Homo sapiens (human)* isPartOf Metabolism of amino acids and derivatives
 Phenylalanine metabolism - Homo sapiens (human)* isPartOf Phenylalanine and tyrosine catabolism
 Phenylalanine metabolism - Homo sapiens (human)* isPartOf Amino acid synthesis and interconversion (transamination)
@@ -1455,20 +1455,20 @@
 Phenylalanine and tyrosine catabolism isPartOf Phenylalanine metabolism - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Phenylalanine, tyrosine and tryptophan biosynthesis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phenylalanine, tyrosine and tryptophan biosynthesis - Homo sapiens (human)* isPartOf Metabolism
+    <t>Phenylalanine, tyrosine and tryptophan biosynthesis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Phenylalanine, tyrosine and tryptophan biosynthesis - Homo sapiens (human)* isPartOf Metabolism
 Phenylalanine and tyrosine catabolism isPartOf Phenylalanine, tyrosine and tryptophan biosynthesis - Homo sapiens (human)*
 Phenylalanine, tyrosine and tryptophan biosynthesis - Homo sapiens (human)* isPartOf Metabolism of amino acids and derivatives
 Phenylalanine, tyrosine and tryptophan biosynthesis - Homo sapiens (human)* isPartOf Amino acid synthesis and interconversion (transamination)
 Phenylalanine, tyrosine and tryptophan biosynthesis - Homo sapiens (human)* isPartOf Histidine, lysine, phenylalanine, tyrosine, proline and tryptophan catabolism</t>
   </si>
   <si>
-    <t xml:space="preserve">Phosphatidylinositol signaling system - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Synthesis of PIPs in the nucleus isPartOf Phosphatidylinositol signaling system - Homo sapiens (human)*
+    <t>Phosphatidylinositol signaling system - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Synthesis of PIPs in the nucleus isPartOf Phosphatidylinositol signaling system - Homo sapiens (human)*
 Synthesis of PIPs at the early endosome membrane isPartOf Phosphatidylinositol signaling system - Homo sapiens (human)*
 Synthesis of PIPs at the late endosome membrane isPartOf Phosphatidylinositol signaling system - Homo sapiens (human)*
 Inositol phosphate metabolism isPartOf Phosphatidylinositol signaling system - Homo sapiens (human)*
@@ -1481,78 +1481,78 @@
 Synthesis of PIPs at the Golgi membrane isPartOf Phosphatidylinositol signaling system - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Phospholipase D signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phosphonate and phosphinate metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phosphonate and phosphinate metabolism - Homo sapiens (human)* isPartOf Metabolism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phototransduction - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phototransduction - Homo sapiens (human) equivalentTo Visual phototransduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Platelet activation - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Platelet Adhesion to exposed collagen isPartOf Platelet activation - Homo sapiens (human)*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Platinum drug resistance - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Porphyrin and chlorophyll metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Porphyrin and chlorophyll metabolism - Homo sapiens (human)* isPartOf Metabolism
+    <t>Phospholipase D signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Phosphonate and phosphinate metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Phosphonate and phosphinate metabolism - Homo sapiens (human)* isPartOf Metabolism</t>
+  </si>
+  <si>
+    <t>Phototransduction - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Phototransduction - Homo sapiens (human) equivalentTo Visual phototransduction</t>
+  </si>
+  <si>
+    <t>Platelet activation - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Platelet Adhesion to exposed collagen isPartOf Platelet activation - Homo sapiens (human)*</t>
+  </si>
+  <si>
+    <t>Platinum drug resistance - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Porphyrin and chlorophyll metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Porphyrin and chlorophyll metabolism - Homo sapiens (human)* isPartOf Metabolism
 Heme degradation isPartOf Porphyrin and chlorophyll metabolism - Homo sapiens (human)*
 Metabolism of porphyrins isPartOf Porphyrin and chlorophyll metabolism - Homo sapiens (human)*
 Heme biosynthesis isPartOf Porphyrin and chlorophyll metabolism - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Primary bile acid biosynthesis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primary bile acid biosynthesis - Homo sapiens (human)* isPartOf Synthesis of bile acids and bile salts via 7alpha-hydroxycholesterol
+    <t>Primary bile acid biosynthesis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Primary bile acid biosynthesis - Homo sapiens (human)* isPartOf Synthesis of bile acids and bile salts via 7alpha-hydroxycholesterol
 Primary bile acid biosynthesis - Homo sapiens (human)* isPartOf Metabolism
 Primary bile acid biosynthesis - Homo sapiens (human)* isPartOf Synthesis of bile acids and bile salts
 Primary bile acid biosynthesis - Homo sapiens (human)* isPartOf Synthesis of bile acids and bile salts via 24-hydroxycholesterol
 Primary bile acid biosynthesis - Homo sapiens (human)* isPartOf Bile acid and bile salt metabolism</t>
   </si>
   <si>
-    <t xml:space="preserve">Primary immunodeficiency - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prion diseases - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Progesterone-mediated oocyte maturation - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prolactin signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prolactin signaling pathway - Homo sapiens (human) equivalentTo Prolactin receptor signaling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Propanoate metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Propionyl-CoA catabolism isPartOf Propanoate metabolism - Homo sapiens (human)*
+    <t>Primary immunodeficiency - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Prion diseases - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Progesterone-mediated oocyte maturation - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Prolactin signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Prolactin signaling pathway - Homo sapiens (human) equivalentTo Prolactin receptor signaling</t>
+  </si>
+  <si>
+    <t>Propanoate metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Propionyl-CoA catabolism isPartOf Propanoate metabolism - Homo sapiens (human)*
 Propanoate metabolism - Homo sapiens (human)* isPartOf Metabolism</t>
   </si>
   <si>
-    <t xml:space="preserve">Prostate cancer - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proteasome - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GLI3 is processed to GLI3R by the proteasome isPartOf Proteasome - Homo sapiens (human)*
+    <t>Prostate cancer - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Proteasome - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>GLI3 is processed to GLI3R by the proteasome isPartOf Proteasome - Homo sapiens (human)*
 Ub-specific processing proteases isPartOf Proteasome - Homo sapiens (human)*
 Regulation of activated PAK-2p34 by proteasome mediated degradation isPartOf Proteasome - Homo sapiens (human)*
 Proteasome - Homo sapiens (human)* isPartOf Metabolism of proteins
@@ -1562,93 +1562,93 @@
 Antigen processing: Ubiquitination &amp; Proteasome degradation isPartOf Proteasome - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Protein digestion and absorption - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protein digestion and absorption - Homo sapiens (human)* isPartOf Intestinal absorption
+    <t>Protein digestion and absorption - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Protein digestion and absorption - Homo sapiens (human)* isPartOf Intestinal absorption
 Protein digestion and absorption - Homo sapiens (human)* isPartOf Digestion and absorption
 Protein digestion and absorption - Homo sapiens (human)* isPartOf Metabolism of proteins</t>
   </si>
   <si>
-    <t xml:space="preserve">Protein export - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protein processing in endoplasmic reticulum - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protein processing in endoplasmic reticulum - Homo sapiens (human)* isPartOf Metabolism of proteins
+    <t>Protein export - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Protein processing in endoplasmic reticulum - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Protein processing in endoplasmic reticulum - Homo sapiens (human)* isPartOf Metabolism of proteins
 Pre-NOTCH Processing in the Endoplasmic Reticulum isPartOf Protein processing in endoplasmic reticulum - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Proteoglycans in cancer - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proximal tubule bicarbonate reclamation - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Purine metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Purine metabolism - Homo sapiens (human)* isPartOf Nucleobase catabolism
+    <t>Proteoglycans in cancer - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Proximal tubule bicarbonate reclamation - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Purine metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Purine metabolism - Homo sapiens (human)* isPartOf Nucleobase catabolism
 Purine catabolism isPartOf Purine metabolism - Homo sapiens (human)*
 Purine ribonucleoside monophosphate biosynthesis isPartOf Purine metabolism - Homo sapiens (human)*
 Purine salvage isPartOf Purine metabolism - Homo sapiens (human)*
 Purine metabolism - Homo sapiens (human)* isPartOf Metabolism of nucleotides</t>
   </si>
   <si>
-    <t xml:space="preserve">Pyrimidine metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pyrimidine catabolism isPartOf Pyrimidine metabolism - Homo sapiens (human)*
+    <t>Pyrimidine metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Pyrimidine catabolism isPartOf Pyrimidine metabolism - Homo sapiens (human)*
 Pyrimidine salvage isPartOf Pyrimidine metabolism - Homo sapiens (human)*
 Pyrimidine metabolism - Homo sapiens (human)* isPartOf Metabolism of nucleotides
 Pyrimidine biosynthesis isPartOf Pyrimidine metabolism - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Pyruvate metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pyruvate metabolism - Homo sapiens (human) equivalentTo Pyruvate metabolism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RIG-I-like receptor signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RIG-I-like receptor signaling pathway - Homo sapiens (human)* isPartOf Immune System
+    <t>Pyruvate metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Pyruvate metabolism - Homo sapiens (human) equivalentTo Pyruvate metabolism</t>
+  </si>
+  <si>
+    <t>RIG-I-like receptor signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>RIG-I-like receptor signaling pathway - Homo sapiens (human)* isPartOf Immune System
 RIG-I-like receptor signaling pathway - Homo sapiens (human)* isPartOf Innate Immune System</t>
   </si>
   <si>
-    <t xml:space="preserve">RNA degradation - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mRNA decay by 3' to 5' exoribonuclease isPartOf RNA degradation - Homo sapiens (human)*
+    <t>RNA degradation - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>mRNA decay by 3' to 5' exoribonuclease isPartOf RNA degradation - Homo sapiens (human)*
 RNA degradation - Homo sapiens (human)* isPartOf Metabolism of RNA
 mRNA decay by 5' to 3' exoribonuclease isPartOf RNA degradation - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">RNA polymerase - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RNA transport - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transport of Mature mRNAs Derived from Intronless Transcripts isPartOf RNA transport - Homo sapiens (human)*
+    <t>RNA polymerase - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>RNA transport - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Transport of Mature mRNAs Derived from Intronless Transcripts isPartOf RNA transport - Homo sapiens (human)*
 Rev-mediated nuclear export of HIV RNA isPartOf RNA transport - Homo sapiens (human)*
 Transport of Mature mRNA Derived from an Intronless Transcript isPartOf RNA transport - Homo sapiens (human)*
 Transport of the SLBP Dependant Mature mRNA isPartOf RNA transport - Homo sapiens (human)*
 Transport of the SLBP independent Mature mRNA isPartOf RNA transport - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Rap1 signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rap1 signaling pathway - Homo sapiens (human) equivalentTo Rap1 signalling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ras signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Signaling by RAS mutants isPartOf Ras signaling pathway - Homo sapiens (human)*
+    <t>Rap1 signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Rap1 signaling pathway - Homo sapiens (human) equivalentTo Rap1 signalling</t>
+  </si>
+  <si>
+    <t>Ras signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Signaling by RAS mutants isPartOf Ras signaling pathway - Homo sapiens (human)*
 MET activates RAS signaling isPartOf Ras signaling pathway - Homo sapiens (human)*
 CREB phosphorylation through the activation of Ras isPartOf Ras signaling pathway - Homo sapiens (human)*
 Regulation of RAS by GAPs isPartOf Ras signaling pathway - Homo sapiens (human)*
@@ -1657,118 +1657,118 @@
 RAS signaling downstream of NF1 loss-of-function variants isPartOf Ras signaling pathway - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Regulation of actin cytoskeleton - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regulation of lipolysis in adipocytes - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regulation of lipolysis in adipocytes - Homo sapiens (human)* isPartOf Metabolism of lipids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relaxin signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relaxin receptors isPartOf Relaxin signaling pathway - Homo sapiens (human)*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Renal cell carcinoma - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Renin secretion - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Renin-angiotensin system - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metabolism of Angiotensinogen to Angiotensins isPartOf Renin-angiotensin system - Homo sapiens (human)*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retinol metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retinol metabolism - Homo sapiens (human)* isPartOf Vitamins
+    <t>Regulation of actin cytoskeleton - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Regulation of lipolysis in adipocytes - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Regulation of lipolysis in adipocytes - Homo sapiens (human)* isPartOf Metabolism of lipids</t>
+  </si>
+  <si>
+    <t>Relaxin signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Relaxin receptors isPartOf Relaxin signaling pathway - Homo sapiens (human)*</t>
+  </si>
+  <si>
+    <t>Renal cell carcinoma - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Renin secretion - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Renin-angiotensin system - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Metabolism of Angiotensinogen to Angiotensins isPartOf Renin-angiotensin system - Homo sapiens (human)*</t>
+  </si>
+  <si>
+    <t>Retinol metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Retinol metabolism - Homo sapiens (human)* isPartOf Vitamins
 Retinol metabolism - Homo sapiens (human)* isPartOf Metabolism</t>
   </si>
   <si>
-    <t xml:space="preserve">Retrograde endocannabinoid signaling - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rheumatoid arthritis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Riboflavin metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Riboflavin metabolism - Homo sapiens (human) equivalentTo Vitamin B2 (riboflavin) metabolism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ribosome - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ribosome biogenesis in eukaryotes - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rRNA modification in the nucleus and cytosol isPartOf Ribosome biogenesis in eukaryotes - Homo sapiens (human)*
+    <t>Retrograde endocannabinoid signaling - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Rheumatoid arthritis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Riboflavin metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Riboflavin metabolism - Homo sapiens (human) equivalentTo Vitamin B2 (riboflavin) metabolism</t>
+  </si>
+  <si>
+    <t>Ribosome - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Ribosome biogenesis in eukaryotes - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>rRNA modification in the nucleus and cytosol isPartOf Ribosome biogenesis in eukaryotes - Homo sapiens (human)*
 rRNA processing in the nucleus and cytosol isPartOf Ribosome biogenesis in eukaryotes - Homo sapiens (human)*
 rRNA processing isPartOf Ribosome biogenesis in eukaryotes - Homo sapiens (human)*
 Ribosome biogenesis in eukaryotes - Homo sapiens (human)* isPartOf Metabolism of RNA</t>
   </si>
   <si>
-    <t xml:space="preserve">SNARE interactions in vesicular transport - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SNARE interactions in vesicular transport - Homo sapiens (human)* isPartOf Vesicle-mediated transport
+    <t>SNARE interactions in vesicular transport - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>SNARE interactions in vesicular transport - Homo sapiens (human)* isPartOf Vesicle-mediated transport
 SNARE interactions in vesicular transport - Homo sapiens (human)* isPartOf Membrane Trafficking</t>
   </si>
   <si>
-    <t xml:space="preserve">Salivary secretion - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salmonella infection - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Selenocompound metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Selenocompound metabolism - Homo sapiens (human)* isPartOf Metabolism
+    <t>Salivary secretion - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Salmonella infection - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Selenocompound metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Selenocompound metabolism - Homo sapiens (human)* isPartOf Metabolism
 Selenoamino acid metabolism isPartOf Selenocompound metabolism - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Serotonergic synapse - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serotonin receptors isPartOf Serotonergic synapse - Homo sapiens (human)*
+    <t>Serotonergic synapse - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Serotonin receptors isPartOf Serotonergic synapse - Homo sapiens (human)*
 Serotonin clearance from the synaptic cleft isPartOf Serotonergic synapse - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Shigellosis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Signaling pathways regulating pluripotency of stem cells - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POU5F1 (OCT4), SOX2, NANOG repress genes related to differentiation isPartOf Signaling pathways regulating pluripotency of stem cells - Homo sapiens (human)*
+    <t>Shigellosis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Signaling pathways regulating pluripotency of stem cells - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>POU5F1 (OCT4), SOX2, NANOG repress genes related to differentiation isPartOf Signaling pathways regulating pluripotency of stem cells - Homo sapiens (human)*
 Signaling by FGFR1 amplification mutants isPartOf Signaling pathways regulating pluripotency of stem cells - Homo sapiens (human)*
 Signaling by FGFR2 amplification mutants isPartOf Signaling pathways regulating pluripotency of stem cells - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Small cell lung cancer - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sphingolipid metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sphingolipid metabolism - Homo sapiens (human) equivalentTo Sphingolipid metabolism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sphingolipid signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spliceosome - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spliceosome - Homo sapiens (human)* isPartOf Processing of Capped Intronless Pre-mRNA
+    <t>Small cell lung cancer - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Sphingolipid metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Sphingolipid metabolism - Homo sapiens (human) equivalentTo Sphingolipid metabolism</t>
+  </si>
+  <si>
+    <t>Sphingolipid signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Spliceosome - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Spliceosome - Homo sapiens (human)* isPartOf Processing of Capped Intronless Pre-mRNA
 Spliceosome - Homo sapiens (human)* isPartOf mRNA Splicing
 Spliceosome - Homo sapiens (human)* isPartOf Metabolism of RNA
 Spliceosome - Homo sapiens (human)* isPartOf mRNA Splicing - Major Pathway
@@ -1778,159 +1778,159 @@
 Spliceosome - Homo sapiens (human)* isPartOf RNA Polymerase II Transcription Termination</t>
   </si>
   <si>
-    <t xml:space="preserve">Staphylococcus aureus infection - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Starch and sucrose metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Starch and sucrose metabolism - Homo sapiens (human)* isPartOf Metabolism
+    <t>Staphylococcus aureus infection - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Starch and sucrose metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Starch and sucrose metabolism - Homo sapiens (human)* isPartOf Metabolism
 Starch and sucrose metabolism - Homo sapiens (human)* isPartOf Metabolism of carbohydrates</t>
   </si>
   <si>
-    <t xml:space="preserve">Steroid biosynthesis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Steroid biosynthesis - Homo sapiens (human)* isPartOf Metabolism
+    <t>Steroid biosynthesis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Steroid biosynthesis - Homo sapiens (human)* isPartOf Metabolism
 Steroid biosynthesis - Homo sapiens (human)* isPartOf Metabolism of steroids</t>
   </si>
   <si>
-    <t xml:space="preserve">Steroid hormone biosynthesis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Steroid hormone biosynthesis - Homo sapiens (human)* isPartOf Metabolism of steroid hormones
+    <t>Steroid hormone biosynthesis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Steroid hormone biosynthesis - Homo sapiens (human)* isPartOf Metabolism of steroid hormones
 Estrogen biosynthesis isPartOf Steroid hormone biosynthesis - Homo sapiens (human)*
 Glucocorticoid biosynthesis isPartOf Steroid hormone biosynthesis - Homo sapiens (human)*
 Steroid hormone biosynthesis - Homo sapiens (human)* isPartOf Metabolism
 Mineralocorticoid biosynthesis isPartOf Steroid hormone biosynthesis - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Sulfur metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sulfur metabolism - Homo sapiens (human)* isPartOf Metabolism of amino acids and derivatives
+    <t>Sulfur metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Sulfur metabolism - Homo sapiens (human)* isPartOf Metabolism of amino acids and derivatives
 Sulfur metabolism - Homo sapiens (human)* isPartOf Sulfur amino acid metabolism
 Sulfur metabolism - Homo sapiens (human)* isPartOf Metabolism</t>
   </si>
   <si>
-    <t xml:space="preserve">Sulfur relay system - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Synaptic vesicle cycle - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Synaptic vesicle cycle - Homo sapiens (human)* isPartOf Vesicle-mediated transport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Synthesis and degradation of ketone bodies - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Synthesis and degradation of ketone bodies - Homo sapiens (human) equivalentTo Ketone body metabolism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Synthesis and degradation of ketone bodies - Homo sapiens (human)* isPartOf Metabolism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Systemic lupus erythematosus - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T cell receptor signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nef mediated downregulation of CD28 cell surface expression isPartOf T cell receptor signaling pathway - Homo sapiens (human)*
+    <t>Sulfur relay system - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Synaptic vesicle cycle - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Synaptic vesicle cycle - Homo sapiens (human)* isPartOf Vesicle-mediated transport</t>
+  </si>
+  <si>
+    <t>Synthesis and degradation of ketone bodies - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Synthesis and degradation of ketone bodies - Homo sapiens (human) equivalentTo Ketone body metabolism</t>
+  </si>
+  <si>
+    <t>Synthesis and degradation of ketone bodies - Homo sapiens (human)* isPartOf Metabolism</t>
+  </si>
+  <si>
+    <t>Systemic lupus erythematosus - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>T cell receptor signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Nef mediated downregulation of CD28 cell surface expression isPartOf T cell receptor signaling pathway - Homo sapiens (human)*
 T cell receptor signaling pathway - Homo sapiens (human)* isPartOf Immune System
 CD28 dependent Vav1 pathway isPartOf T cell receptor signaling pathway - Homo sapiens (human)*
 CD28 co-stimulation isPartOf T cell receptor signaling pathway - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">TGF-beta signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TGF-beta signaling pathway - Homo sapiens (human) equivalentTo Signaling by TGF-beta family members</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TNF signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TNF signaling pathway - Homo sapiens (human) equivalentTo TNF signaling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taste transduction - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taurine and hypotaurine metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taurine and hypotaurine metabolism - Homo sapiens (human)* isPartOf Metabolism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Terpenoid backbone biosynthesis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Terpenoid backbone biosynthesis - Homo sapiens (human)* isPartOf Metabolism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Th1 and Th2 cell differentiation - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Th1 and Th2 cell differentiation - Homo sapiens (human)* isPartOf Adaptive Immune System</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Th17 cell differentiation - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Th17 cell differentiation - Homo sapiens (human)* isPartOf Immune System</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thermogenesis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thermogenesis - Homo sapiens (human)* isPartOf Formation of ATP by chemiosmotic coupling
+    <t>TGF-beta signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>TGF-beta signaling pathway - Homo sapiens (human) equivalentTo Signaling by TGF-beta family members</t>
+  </si>
+  <si>
+    <t>TNF signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>TNF signaling pathway - Homo sapiens (human) equivalentTo TNF signaling</t>
+  </si>
+  <si>
+    <t>Taste transduction - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Taurine and hypotaurine metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Taurine and hypotaurine metabolism - Homo sapiens (human)* isPartOf Metabolism</t>
+  </si>
+  <si>
+    <t>Terpenoid backbone biosynthesis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Terpenoid backbone biosynthesis - Homo sapiens (human)* isPartOf Metabolism</t>
+  </si>
+  <si>
+    <t>Th1 and Th2 cell differentiation - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Th1 and Th2 cell differentiation - Homo sapiens (human)* isPartOf Adaptive Immune System</t>
+  </si>
+  <si>
+    <t>Th17 cell differentiation - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Th17 cell differentiation - Homo sapiens (human)* isPartOf Immune System</t>
+  </si>
+  <si>
+    <t>Thermogenesis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Thermogenesis - Homo sapiens (human)* isPartOf Formation of ATP by chemiosmotic coupling
 Thermogenesis - Homo sapiens (human)* isPartOf Respiratory electron transport, ATP synthesis by chemiosmotic coupling, and heat production by uncoupling proteins.
 Thermogenesis - Homo sapiens (human)* isPartOf Metabolism
 Thermogenesis - Homo sapiens (human)* isPartOf Respiratory electron transport</t>
   </si>
   <si>
-    <t xml:space="preserve">Thiamine metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thiamine metabolism - Homo sapiens (human) equivalentTo Vitamin B1 (thiamin) metabolism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thiamine metabolism - Homo sapiens (human)* isPartOf Metabolism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thyroid cancer - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thyroid hormone signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regulation of thyroid hormone activity isPartOf Thyroid hormone signaling pathway - Homo sapiens (human)*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thyroid hormone synthesis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thyroid hormone synthesis - Homo sapiens (human) equivalentTo Thyroxine biosynthesis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tight junction - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tight junction - Homo sapiens (human) equivalentTo Tight junction interactions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RUNX1 regulates expression of components of tight junctions isPartOf Tight junction - Homo sapiens (human)*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Toll-like receptor signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Toll-like receptor signaling pathway - Homo sapiens (human) equivalentTo Toll-Like Receptors Cascades</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Toll Like Receptor 4 (TLR4) Cascade isPartOf Toll-like receptor signaling pathway - Homo sapiens (human)*
+    <t>Thiamine metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Thiamine metabolism - Homo sapiens (human) equivalentTo Vitamin B1 (thiamin) metabolism</t>
+  </si>
+  <si>
+    <t>Thiamine metabolism - Homo sapiens (human)* isPartOf Metabolism</t>
+  </si>
+  <si>
+    <t>Thyroid cancer - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Thyroid hormone signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Regulation of thyroid hormone activity isPartOf Thyroid hormone signaling pathway - Homo sapiens (human)*</t>
+  </si>
+  <si>
+    <t>Thyroid hormone synthesis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Thyroid hormone synthesis - Homo sapiens (human) equivalentTo Thyroxine biosynthesis</t>
+  </si>
+  <si>
+    <t>Tight junction - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Tight junction - Homo sapiens (human) equivalentTo Tight junction interactions</t>
+  </si>
+  <si>
+    <t>RUNX1 regulates expression of components of tight junctions isPartOf Tight junction - Homo sapiens (human)*</t>
+  </si>
+  <si>
+    <t>Toll-like receptor signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Toll-like receptor signaling pathway - Homo sapiens (human) equivalentTo Toll-Like Receptors Cascades</t>
+  </si>
+  <si>
+    <t>Toll Like Receptor 4 (TLR4) Cascade isPartOf Toll-like receptor signaling pathway - Homo sapiens (human)*
 Toll Like Receptor 2 (TLR2) Cascade isPartOf Toll-like receptor signaling pathway - Homo sapiens (human)*
 Toll Like Receptor TLR6:TLR2 Cascade isPartOf Toll-like receptor signaling pathway - Homo sapiens (human)*
 Toll Like Receptor 5 (TLR5) Cascade isPartOf Toll-like receptor signaling pathway - Homo sapiens (human)*
@@ -1941,148 +1941,148 @@
 Toll Like Receptor 7/8 (TLR7/8) Cascade isPartOf Toll-like receptor signaling pathway - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Toxoplasmosis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transcriptional misregulation in cancer - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tryptophan metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tryptophan catabolism isPartOf Tryptophan metabolism - Homo sapiens (human)*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tuberculosis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type I diabetes mellitus - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type II diabetes mellitus - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tyrosine metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tyrosine metabolism - Homo sapiens (human)* isPartOf Amino acid synthesis and interconversion (transamination)
+    <t>Toxoplasmosis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Transcriptional misregulation in cancer - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Tryptophan metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Tryptophan catabolism isPartOf Tryptophan metabolism - Homo sapiens (human)*</t>
+  </si>
+  <si>
+    <t>Tuberculosis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Type I diabetes mellitus - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Type II diabetes mellitus - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Tyrosine metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Tyrosine metabolism - Homo sapiens (human)* isPartOf Amino acid synthesis and interconversion (transamination)
 Tyrosine metabolism - Homo sapiens (human)* isPartOf Metabolism of amino acids and derivatives
 Phenylalanine and tyrosine catabolism isPartOf Tyrosine metabolism - Homo sapiens (human)*
 Tyrosine metabolism - Homo sapiens (human)* isPartOf Histidine, lysine, phenylalanine, tyrosine, proline and tryptophan catabolism
 Tyrosine metabolism - Homo sapiens (human)* isPartOf Metabolism</t>
   </si>
   <si>
-    <t xml:space="preserve">Ubiquinone and other terpenoid-quinone biosynthesis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ubiquinone and other terpenoid-quinone biosynthesis - Homo sapiens (human)* isPartOf Metabolism
+    <t>Ubiquinone and other terpenoid-quinone biosynthesis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Ubiquinone and other terpenoid-quinone biosynthesis - Homo sapiens (human)* isPartOf Metabolism
 Ubiquinone and other terpenoid-quinone biosynthesis - Homo sapiens (human)* isPartOf Metabolism of vitamins and cofactors</t>
   </si>
   <si>
-    <t xml:space="preserve">Ubiquitin mediated proteolysis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VEGF signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valine, leucine and isoleucine biosynthesis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valine, leucine and isoleucine biosynthesis - Homo sapiens (human)* isPartOf Metabolism of amino acids and derivatives
+    <t>Ubiquitin mediated proteolysis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>VEGF signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Valine, leucine and isoleucine biosynthesis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Valine, leucine and isoleucine biosynthesis - Homo sapiens (human)* isPartOf Metabolism of amino acids and derivatives
 Valine, leucine and isoleucine biosynthesis - Homo sapiens (human)* isPartOf Metabolism</t>
   </si>
   <si>
-    <t xml:space="preserve">Valine, leucine and isoleucine degradation - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valine, leucine and isoleucine degradation - Homo sapiens (human)* isPartOf Branched-chain amino acid catabolism
+    <t>Valine, leucine and isoleucine degradation - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Valine, leucine and isoleucine degradation - Homo sapiens (human)* isPartOf Branched-chain amino acid catabolism
 Valine, leucine and isoleucine degradation - Homo sapiens (human)* isPartOf Metabolism
 Valine, leucine and isoleucine degradation - Homo sapiens (human)* isPartOf Metabolism of amino acids and derivatives</t>
   </si>
   <si>
-    <t xml:space="preserve">Vascular smooth muscle contraction - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vascular smooth muscle contraction - Homo sapiens (human)* isPartOf Smooth Muscle Contraction
+    <t>Vascular smooth muscle contraction - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Vascular smooth muscle contraction - Homo sapiens (human)* isPartOf Smooth Muscle Contraction
 Vascular smooth muscle contraction - Homo sapiens (human)* isPartOf Muscle contraction</t>
   </si>
   <si>
-    <t xml:space="preserve">Vasopressin-regulated water reabsorption - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vasopressin-regulated water reabsorption - Homo sapiens (human) equivalentTo Vasopressin regulates renal water homeostasis via Aquaporins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vibrio cholerae infection - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Viral carcinogenesis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Viral myocarditis - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitamin B6 metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitamin B6 metabolism - Homo sapiens (human)* isPartOf Metabolism
+    <t>Vasopressin-regulated water reabsorption - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Vasopressin-regulated water reabsorption - Homo sapiens (human) equivalentTo Vasopressin regulates renal water homeostasis via Aquaporins</t>
+  </si>
+  <si>
+    <t>Vibrio cholerae infection - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Viral carcinogenesis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Viral myocarditis - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Vitamin B6 metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Vitamin B6 metabolism - Homo sapiens (human)* isPartOf Metabolism
 Vitamin B6 metabolism - Homo sapiens (human)* isPartOf Metabolism of water-soluble vitamins and cofactors
 Vitamin B6 metabolism - Homo sapiens (human)* isPartOf Metabolism of vitamins and cofactors
 Vitamins B6 activation to pyridoxal phosphate isPartOf Vitamin B6 metabolism - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">Vitamin digestion and absorption - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitamin digestion and absorption - Homo sapiens (human)* isPartOf Intestinal absorption
+    <t>Vitamin digestion and absorption - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Vitamin digestion and absorption - Homo sapiens (human)* isPartOf Intestinal absorption
 Vitamin digestion and absorption - Homo sapiens (human)* isPartOf Digestion and absorption
 Vitamin digestion and absorption - Homo sapiens (human)* isPartOf Metabolism of vitamins and cofactors</t>
   </si>
   <si>
-    <t xml:space="preserve">Wnt signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wnt signaling pathway - Homo sapiens (human) equivalentTo Signaling by WNT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RUNX3 regulates WNT signaling isPartOf Wnt signaling pathway - Homo sapiens (human)*
+    <t>Wnt signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Wnt signaling pathway - Homo sapiens (human) equivalentTo Signaling by WNT</t>
+  </si>
+  <si>
+    <t>RUNX3 regulates WNT signaling isPartOf Wnt signaling pathway - Homo sapiens (human)*
 WNT mediated activation of DVL isPartOf Wnt signaling pathway - Homo sapiens (human)*
 WNT ligand secretion is abrogated by the PORCN inhibitor LGK974 isPartOf Wnt signaling pathway - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">alpha-Linolenic acid metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alpha-Linolenic acid metabolism - Homo sapiens (human) equivalentTo alpha-linolenic acid (ALA) metabolism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alpha-Linolenic acid metabolism - Homo sapiens (human)* isPartOf Metabolism of lipids
+    <t>alpha-Linolenic acid metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>alpha-Linolenic acid metabolism - Homo sapiens (human) equivalentTo alpha-linolenic acid (ALA) metabolism</t>
+  </si>
+  <si>
+    <t>alpha-Linolenic acid metabolism - Homo sapiens (human)* isPartOf Metabolism of lipids
 alpha-Linolenic acid metabolism - Homo sapiens (human)* isPartOf Metabolism</t>
   </si>
   <si>
-    <t xml:space="preserve">beta-Alanine metabolism - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">beta-Alanine metabolism - Homo sapiens (human)* isPartOf Metabolism of amino acids and derivatives
+    <t>beta-Alanine metabolism - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>beta-Alanine metabolism - Homo sapiens (human)* isPartOf Metabolism of amino acids and derivatives
 beta-Alanine metabolism - Homo sapiens (human)* isPartOf Metabolism</t>
   </si>
   <si>
-    <t xml:space="preserve">cAMP signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adenylate cyclase activating pathway isPartOf cAMP signaling pathway - Homo sapiens (human)*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cGMP-PKG signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cGMP effects isPartOf cGMP-PKG signaling pathway - Homo sapiens (human)*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mRNA surveillance pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inhibition of Host mRNA Processing and RNA Silencing isPartOf mRNA surveillance pathway - Homo sapiens (human)*
+    <t>cAMP signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Adenylate cyclase activating pathway isPartOf cAMP signaling pathway - Homo sapiens (human)*</t>
+  </si>
+  <si>
+    <t>cGMP-PKG signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>cGMP effects isPartOf cGMP-PKG signaling pathway - Homo sapiens (human)*</t>
+  </si>
+  <si>
+    <t>mRNA surveillance pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>Inhibition of Host mRNA Processing and RNA Silencing isPartOf mRNA surveillance pathway - Homo sapiens (human)*
 Processing of Capped Intron-Containing Pre-mRNA isPartOf mRNA surveillance pathway - Homo sapiens (human)*
 mRNA Splicing isPartOf mRNA surveillance pathway - Homo sapiens (human)*
 Processing of Capped Intronless Pre-mRNA isPartOf mRNA surveillance pathway - Homo sapiens (human)*
@@ -2091,16 +2091,16 @@
 mRNA Splicing - Major Pathway isPartOf mRNA surveillance pathway - Homo sapiens (human)*</t>
   </si>
   <si>
-    <t xml:space="preserve">mTOR signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mTOR signaling pathway - Homo sapiens (human) equivalentTo mTOR signalling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p53 signaling pathway - Homo sapiens (human)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TP53 Regulates Transcription of Cell Death Genes isPartOf p53 signaling pathway - Homo sapiens (human)*
+    <t>mTOR signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>mTOR signaling pathway - Homo sapiens (human) equivalentTo mTOR signalling</t>
+  </si>
+  <si>
+    <t>p53 signaling pathway - Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>TP53 Regulates Transcription of Cell Death Genes isPartOf p53 signaling pathway - Homo sapiens (human)*
 Regulation of TP53 Expression isPartOf p53 signaling pathway - Homo sapiens (human)*
 TP53 Regulates Transcription of Cell Cycle Genes isPartOf p53 signaling pathway - Homo sapiens (human)*
 TP53 Regulates Transcription of Death Receptors and Ligands isPartOf p53 signaling pathway - Homo sapiens (human)*
@@ -2119,7 +2119,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -2250,16 +2250,15 @@
   </sheetPr>
   <dimension ref="A1:Y326"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A231" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C235" activeCellId="0" sqref="C235"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="71.4081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.3010204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.4183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="70.6020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.7602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="65.6071428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2493,14 +2492,13 @@
       </c>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">

</xml_diff>

<commit_message>
Update excel cytosolic problem
</commit_message>
<xml_diff>
--- a/mappings/kegg_reactome.xlsx
+++ b/mappings/kegg_reactome.xlsx
@@ -2206,7 +2206,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2221,6 +2221,10 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -2250,15 +2254,16 @@
   </sheetPr>
   <dimension ref="A1:Y326"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H74" activeCellId="0" sqref="H74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="70.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.7602040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="65.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="69.7908163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2509,7 +2514,7 @@
       </c>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" customFormat="false" ht="70" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="77.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
         <v>46</v>
       </c>
@@ -2517,6 +2522,7 @@
       <c r="C28" s="3" t="s">
         <v>47</v>
       </c>
+      <c r="D28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
@@ -2568,7 +2574,7 @@
       <c r="A35" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="5" t="s">
         <v>57</v>
       </c>
       <c r="C35" s="3" t="s">
@@ -2588,7 +2594,7 @@
       <c r="A37" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="5" t="s">
         <v>62</v>
       </c>
       <c r="C37" s="3" t="s">
@@ -3266,7 +3272,7 @@
       <c r="A117" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="B117" s="5"/>
+      <c r="B117" s="6"/>
       <c r="C117" s="3" t="s">
         <v>201</v>
       </c>
@@ -3275,7 +3281,7 @@
       <c r="A118" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="B118" s="5"/>
+      <c r="B118" s="6"/>
       <c r="C118" s="3" t="s">
         <v>203</v>
       </c>
@@ -3284,7 +3290,7 @@
       <c r="A119" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="B119" s="5"/>
+      <c r="B119" s="6"/>
       <c r="C119" s="3" t="s">
         <v>205</v>
       </c>
@@ -3293,7 +3299,7 @@
       <c r="A120" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="B120" s="5"/>
+      <c r="B120" s="6"/>
       <c r="C120" s="3" t="s">
         <v>207</v>
       </c>
@@ -3302,7 +3308,7 @@
       <c r="A121" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B121" s="5"/>
+      <c r="B121" s="6"/>
       <c r="C121" s="3" t="s">
         <v>209</v>
       </c>
@@ -3311,7 +3317,7 @@
       <c r="A122" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="B122" s="5"/>
+      <c r="B122" s="6"/>
       <c r="C122" s="3" t="s">
         <v>211</v>
       </c>
@@ -3320,7 +3326,7 @@
       <c r="A123" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="B123" s="5"/>
+      <c r="B123" s="6"/>
       <c r="C123" s="3" t="s">
         <v>213</v>
       </c>
@@ -3329,7 +3335,7 @@
       <c r="A124" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="B124" s="5"/>
+      <c r="B124" s="6"/>
       <c r="C124" s="3" t="s">
         <v>215</v>
       </c>
@@ -3338,14 +3344,14 @@
       <c r="A125" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="B125" s="5"/>
+      <c r="B125" s="6"/>
       <c r="C125" s="3"/>
     </row>
     <row r="126" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="B126" s="5"/>
+      <c r="B126" s="6"/>
       <c r="C126" s="3" t="s">
         <v>218</v>
       </c>
@@ -3714,7 +3720,7 @@
       <c r="A171" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="B171" s="5"/>
+      <c r="B171" s="6"/>
       <c r="C171" s="3" t="s">
         <v>290</v>
       </c>
@@ -3866,7 +3872,7 @@
       <c r="A189" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="B189" s="5"/>
+      <c r="B189" s="6"/>
       <c r="C189" s="3" t="s">
         <v>321</v>
       </c>
@@ -3875,14 +3881,14 @@
       <c r="A190" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="B190" s="5"/>
+      <c r="B190" s="6"/>
       <c r="C190" s="3"/>
     </row>
     <row r="191" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="B191" s="5"/>
+      <c r="B191" s="6"/>
       <c r="C191" s="3" t="s">
         <v>324</v>
       </c>
@@ -3891,7 +3897,7 @@
       <c r="A192" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="B192" s="5"/>
+      <c r="B192" s="6"/>
       <c r="C192" s="3" t="s">
         <v>326</v>
       </c>
@@ -3900,7 +3906,7 @@
       <c r="A193" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="B193" s="5"/>
+      <c r="B193" s="6"/>
       <c r="C193" s="3"/>
     </row>
     <row r="194" customFormat="false" ht="70" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Remove loop in hierarchical mapping
</commit_message>
<xml_diff>
--- a/mappings/kegg_reactome.xlsx
+++ b/mappings/kegg_reactome.xlsx
@@ -1,17 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmarinllao/Desktop/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19120" windowHeight="10480" tabRatio="991"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -1011,7 +1021,7 @@
     <t>IL-17 signaling pathway - Homo sapiens (human)</t>
   </si>
   <si>
-    <t>IL-17 signaling pathway - Homo sapiens (human) equivalentTo Interleukin-17 signaling </t>
+    <t>IL-17 signaling pathway - Homo sapiens (human) equivalentTo Interleukin-17 signaling</t>
   </si>
   <si>
     <t>IL-17 signaling pathway - Homo sapiens (human)* isPartOf Cytokine Signaling in Immune system
@@ -1447,14 +1457,6 @@
     <t>Phenylalanine metabolism - Homo sapiens (human)</t>
   </si>
   <si>
-    <t>Phenylalanine metabolism - Homo sapiens (human)* isPartOf Metabolism
-Phenylalanine metabolism - Homo sapiens (human)* isPartOf Metabolism of amino acids and derivatives
-Phenylalanine metabolism - Homo sapiens (human)* isPartOf Phenylalanine and tyrosine catabolism
-Phenylalanine metabolism - Homo sapiens (human)* isPartOf Amino acid synthesis and interconversion (transamination)
-Phenylalanine metabolism - Homo sapiens (human)* isPartOf Histidine, lysine, phenylalanine, tyrosine, proline and tryptophan catabolism
-Phenylalanine and tyrosine catabolism isPartOf Phenylalanine metabolism - Homo sapiens (human)*</t>
-  </si>
-  <si>
     <t>Phenylalanine, tyrosine and tryptophan biosynthesis - Homo sapiens (human)</t>
   </si>
   <si>
@@ -2113,15 +2115,19 @@
 Regulation of TP53 Expression and Degradation isPartOf p53 signaling pathway - Homo sapiens (human)*
 Regulation of TP53 Degradation isPartOf p53 signaling pathway - Homo sapiens (human)*</t>
   </si>
+  <si>
+    <t>Phenylalanine metabolism - Homo sapiens (human)* isPartOf Metabolism
+Phenylalanine metabolism - Homo sapiens (human)* isPartOf Metabolism of amino acids and derivatives
+Phenylalanine metabolism - Homo sapiens (human)* isPartOf Phenylalanine and tyrosine catabolism
+Phenylalanine metabolism - Homo sapiens (human)* isPartOf Amino acid synthesis and interconversion (transamination)
+Phenylalanine metabolism - Homo sapiens (human)* isPartOf Histidine, lysine, phenylalanine, tyrosine, proline and tryptophan catabolism</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2130,22 +2136,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -2173,7 +2164,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -2181,92 +2172,311 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y326"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H74" activeCellId="0" sqref="H74"/>
+    <sheetView tabSelected="1" topLeftCell="A222" workbookViewId="0">
+      <selection activeCell="C222" sqref="C222"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="69.7908163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.2244897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.7959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:25" ht="56" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2299,7 +2509,7 @@
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="66.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:25" ht="66.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -2308,7 +2518,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="409" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:25" ht="409" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -2319,14 +2529,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:25" ht="154" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:25" ht="196" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -2335,14 +2545,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:25" ht="84" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:25" ht="154" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -2351,7 +2561,7 @@
       </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:25" ht="280" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -2360,21 +2570,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:25" ht="126" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:25" ht="84" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:25" ht="392" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -2383,14 +2593,14 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:25" ht="56" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:25" ht="154" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
@@ -2399,14 +2609,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:25" ht="126" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:25" ht="238" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
@@ -2415,7 +2625,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:25" ht="266" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
@@ -2424,7 +2634,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:4" ht="154" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
         <v>28</v>
       </c>
@@ -2433,7 +2643,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="98" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:4" ht="409" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
         <v>30</v>
       </c>
@@ -2442,35 +2652,35 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:4" ht="56" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:4" ht="84" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:4" ht="112" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:4" ht="70" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:4" ht="409" x14ac:dyDescent="0.15">
       <c r="A23" s="3" t="s">
         <v>36</v>
       </c>
@@ -2481,14 +2691,14 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:4" ht="84" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:4" ht="98" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
         <v>40</v>
       </c>
@@ -2497,7 +2707,7 @@
       </c>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:4" ht="112" x14ac:dyDescent="0.15">
       <c r="A26" s="3" t="s">
         <v>42</v>
       </c>
@@ -2505,7 +2715,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:4" ht="168" x14ac:dyDescent="0.15">
       <c r="A27" s="3" t="s">
         <v>44</v>
       </c>
@@ -2514,7 +2724,7 @@
       </c>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" customFormat="false" ht="77.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:4" ht="409" x14ac:dyDescent="0.15">
       <c r="A28" s="3" t="s">
         <v>46</v>
       </c>
@@ -2524,7 +2734,7 @@
       </c>
       <c r="D28" s="4"/>
     </row>
-    <row r="29" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:4" ht="409" x14ac:dyDescent="0.15">
       <c r="A29" s="3" t="s">
         <v>48</v>
       </c>
@@ -2533,14 +2743,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:4" ht="154" x14ac:dyDescent="0.15">
       <c r="A30" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:4" ht="140" x14ac:dyDescent="0.15">
       <c r="A31" s="3" t="s">
         <v>51</v>
       </c>
@@ -2549,28 +2759,28 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:4" ht="56" x14ac:dyDescent="0.15">
       <c r="A32" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A33" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A34" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:3" ht="266" x14ac:dyDescent="0.15">
       <c r="A35" s="3" t="s">
         <v>56</v>
       </c>
@@ -2581,7 +2791,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:3" ht="112" x14ac:dyDescent="0.15">
       <c r="A36" s="3" t="s">
         <v>59</v>
       </c>
@@ -2590,7 +2800,7 @@
       </c>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" customFormat="false" ht="52.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:3" ht="294" x14ac:dyDescent="0.15">
       <c r="A37" s="3" t="s">
         <v>61</v>
       </c>
@@ -2601,21 +2811,21 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:3" ht="112" x14ac:dyDescent="0.15">
       <c r="A38" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A39" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
     </row>
-    <row r="40" customFormat="false" ht="409" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A40" s="3" t="s">
         <v>66</v>
       </c>
@@ -2624,7 +2834,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:3" ht="140" x14ac:dyDescent="0.15">
       <c r="A41" s="3" t="s">
         <v>68</v>
       </c>
@@ -2633,7 +2843,7 @@
       </c>
       <c r="C41" s="3"/>
     </row>
-    <row r="42" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A42" s="3" t="s">
         <v>70</v>
       </c>
@@ -2642,7 +2852,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="140" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A43" s="3" t="s">
         <v>72</v>
       </c>
@@ -2651,7 +2861,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="182" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A44" s="3" t="s">
         <v>74</v>
       </c>
@@ -2660,7 +2870,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A45" s="3" t="s">
         <v>76</v>
       </c>
@@ -2669,21 +2879,21 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A46" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
     </row>
-    <row r="47" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A47" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" customFormat="false" ht="70" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
         <v>80</v>
       </c>
@@ -2692,7 +2902,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:3" ht="112" x14ac:dyDescent="0.15">
       <c r="A49" s="3" t="s">
         <v>82</v>
       </c>
@@ -2701,7 +2911,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="112" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A50" s="3" t="s">
         <v>84</v>
       </c>
@@ -2710,7 +2920,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="140" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A51" s="3" t="s">
         <v>86</v>
       </c>
@@ -2719,7 +2929,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="154" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A52" s="3" t="s">
         <v>88</v>
       </c>
@@ -2730,7 +2940,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A53" s="3" t="s">
         <v>91</v>
       </c>
@@ -2739,7 +2949,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="112" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A54" s="3" t="s">
         <v>93</v>
       </c>
@@ -2748,7 +2958,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A55" s="3" t="s">
         <v>95</v>
       </c>
@@ -2757,7 +2967,7 @@
       </c>
       <c r="C55" s="3"/>
     </row>
-    <row r="56" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A56" s="3" t="s">
         <v>97</v>
       </c>
@@ -2766,28 +2976,28 @@
       </c>
       <c r="C56" s="3"/>
     </row>
-    <row r="57" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:3" ht="112" x14ac:dyDescent="0.15">
       <c r="A57" s="3" t="s">
         <v>99</v>
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
     </row>
-    <row r="58" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:3" ht="126" x14ac:dyDescent="0.15">
       <c r="A58" s="3" t="s">
         <v>100</v>
       </c>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
     </row>
-    <row r="59" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A59" s="3" t="s">
         <v>101</v>
       </c>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
     </row>
-    <row r="60" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:3" ht="196" x14ac:dyDescent="0.15">
       <c r="A60" s="3" t="s">
         <v>102</v>
       </c>
@@ -2796,7 +3006,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="182" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A61" s="3" t="s">
         <v>104</v>
       </c>
@@ -2805,14 +3015,14 @@
         <v>105</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A62" s="3" t="s">
         <v>106</v>
       </c>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
     </row>
-    <row r="63" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:3" ht="168" x14ac:dyDescent="0.15">
       <c r="A63" s="3" t="s">
         <v>107</v>
       </c>
@@ -2821,28 +3031,28 @@
         <v>108</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A64" s="3" t="s">
         <v>109</v>
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
     </row>
-    <row r="65" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A65" s="3" t="s">
         <v>110</v>
       </c>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
     </row>
-    <row r="66" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A66" s="3" t="s">
         <v>111</v>
       </c>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
     </row>
-    <row r="67" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:3" ht="168" x14ac:dyDescent="0.15">
       <c r="A67" s="3" t="s">
         <v>112</v>
       </c>
@@ -2851,21 +3061,21 @@
       </c>
       <c r="C67" s="3"/>
     </row>
-    <row r="68" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A68" s="3" t="s">
         <v>114</v>
       </c>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
     </row>
-    <row r="69" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A69" s="3" t="s">
         <v>115</v>
       </c>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
     </row>
-    <row r="70" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A70" s="3" t="s">
         <v>116</v>
       </c>
@@ -2874,7 +3084,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="322" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A71" s="3" t="s">
         <v>118</v>
       </c>
@@ -2883,7 +3093,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="126" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A72" s="3" t="s">
         <v>120</v>
       </c>
@@ -2892,7 +3102,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="98" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A73" s="3" t="s">
         <v>122</v>
       </c>
@@ -2901,7 +3111,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="196" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A74" s="3" t="s">
         <v>124</v>
       </c>
@@ -2910,7 +3120,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" spans="1:3" ht="196" x14ac:dyDescent="0.15">
       <c r="A75" s="3" t="s">
         <v>126</v>
       </c>
@@ -2919,7 +3129,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" spans="1:3" ht="364" x14ac:dyDescent="0.15">
       <c r="A76" s="3" t="s">
         <v>128</v>
       </c>
@@ -2928,7 +3138,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A77" s="3" t="s">
         <v>130</v>
       </c>
@@ -2937,7 +3147,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" spans="1:3" ht="126" x14ac:dyDescent="0.15">
       <c r="A78" s="3" t="s">
         <v>132</v>
       </c>
@@ -2946,14 +3156,14 @@
       </c>
       <c r="C78" s="3"/>
     </row>
-    <row r="79" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A79" s="3" t="s">
         <v>134</v>
       </c>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
     </row>
-    <row r="80" customFormat="false" ht="154" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A80" s="3" t="s">
         <v>135</v>
       </c>
@@ -2962,7 +3172,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="98" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A81" s="3" t="s">
         <v>137</v>
       </c>
@@ -2971,7 +3181,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" spans="1:3" ht="140" x14ac:dyDescent="0.15">
       <c r="A82" s="3" t="s">
         <v>139</v>
       </c>
@@ -2980,7 +3190,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A83" s="3" t="s">
         <v>141</v>
       </c>
@@ -2989,28 +3199,28 @@
         <v>142</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" spans="1:3" ht="112" x14ac:dyDescent="0.15">
       <c r="A84" s="3" t="s">
         <v>143</v>
       </c>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
     </row>
-    <row r="85" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A85" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
     </row>
-    <row r="86" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A86" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
     </row>
-    <row r="87" customFormat="false" ht="70" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A87" s="3" t="s">
         <v>146</v>
       </c>
@@ -3019,28 +3229,28 @@
         <v>147</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A88" s="3" t="s">
         <v>148</v>
       </c>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
     </row>
-    <row r="89" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" spans="1:3" ht="140" x14ac:dyDescent="0.15">
       <c r="A89" s="3" t="s">
         <v>149</v>
       </c>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
     </row>
-    <row r="90" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A90" s="3" t="s">
         <v>150</v>
       </c>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
     </row>
-    <row r="91" customFormat="false" ht="392" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A91" s="3" t="s">
         <v>151</v>
       </c>
@@ -3049,14 +3259,14 @@
         <v>152</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A92" s="3" t="s">
         <v>153</v>
       </c>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
     </row>
-    <row r="93" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A93" s="3" t="s">
         <v>154</v>
       </c>
@@ -3065,7 +3275,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A94" s="3" t="s">
         <v>156</v>
       </c>
@@ -3074,7 +3284,7 @@
       </c>
       <c r="C94" s="3"/>
     </row>
-    <row r="95" customFormat="false" ht="98" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A95" s="3" t="s">
         <v>158</v>
       </c>
@@ -3083,7 +3293,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A96" s="3" t="s">
         <v>160</v>
       </c>
@@ -3092,7 +3302,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="266" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A97" s="3" t="s">
         <v>162</v>
       </c>
@@ -3101,7 +3311,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A98" s="3" t="s">
         <v>164</v>
       </c>
@@ -3110,7 +3320,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" spans="1:3" ht="238" x14ac:dyDescent="0.15">
       <c r="A99" s="3" t="s">
         <v>166</v>
       </c>
@@ -3121,7 +3331,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" spans="1:3" ht="364" x14ac:dyDescent="0.15">
       <c r="A100" s="3" t="s">
         <v>169</v>
       </c>
@@ -3132,7 +3342,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" spans="1:3" ht="238" x14ac:dyDescent="0.15">
       <c r="A101" s="3" t="s">
         <v>172</v>
       </c>
@@ -3141,7 +3351,7 @@
       </c>
       <c r="C101" s="3"/>
     </row>
-    <row r="102" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A102" s="3" t="s">
         <v>174</v>
       </c>
@@ -3150,14 +3360,14 @@
         <v>175</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" spans="1:3" ht="126" x14ac:dyDescent="0.15">
       <c r="A103" s="3" t="s">
         <v>176</v>
       </c>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
     </row>
-    <row r="104" customFormat="false" ht="98" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A104" s="3" t="s">
         <v>177</v>
       </c>
@@ -3166,7 +3376,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="112" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A105" s="3" t="s">
         <v>179</v>
       </c>
@@ -3175,7 +3385,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" spans="1:3" ht="168" x14ac:dyDescent="0.15">
       <c r="A106" s="3" t="s">
         <v>181</v>
       </c>
@@ -3184,7 +3394,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="126" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A107" s="3" t="s">
         <v>183</v>
       </c>
@@ -3193,7 +3403,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="70" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A108" s="3" t="s">
         <v>185</v>
       </c>
@@ -3202,7 +3412,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" spans="1:3" ht="126" x14ac:dyDescent="0.15">
       <c r="A109" s="3" t="s">
         <v>187</v>
       </c>
@@ -3211,7 +3421,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="126" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A110" s="3" t="s">
         <v>189</v>
       </c>
@@ -3220,28 +3430,28 @@
         <v>190</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A111" s="3" t="s">
         <v>191</v>
       </c>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
     </row>
-    <row r="112" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A112" s="3" t="s">
         <v>192</v>
       </c>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
     </row>
-    <row r="113" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A113" s="3" t="s">
         <v>193</v>
       </c>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
     </row>
-    <row r="114" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" spans="1:3" ht="196" x14ac:dyDescent="0.15">
       <c r="A114" s="3" t="s">
         <v>194</v>
       </c>
@@ -3250,7 +3460,7 @@
       </c>
       <c r="C114" s="3"/>
     </row>
-    <row r="115" customFormat="false" ht="196" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A115" s="3" t="s">
         <v>196</v>
       </c>
@@ -3259,7 +3469,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" spans="1:3" ht="182" x14ac:dyDescent="0.15">
       <c r="A116" s="3" t="s">
         <v>198</v>
       </c>
@@ -3268,7 +3478,7 @@
       </c>
       <c r="C116" s="3"/>
     </row>
-    <row r="117" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A117" s="3" t="s">
         <v>200</v>
       </c>
@@ -3277,7 +3487,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="210" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A118" s="3" t="s">
         <v>202</v>
       </c>
@@ -3286,7 +3496,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="140" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A119" s="3" t="s">
         <v>204</v>
       </c>
@@ -3295,7 +3505,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A120" s="3" t="s">
         <v>206</v>
       </c>
@@ -3304,7 +3514,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="140" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A121" s="3" t="s">
         <v>208</v>
       </c>
@@ -3313,7 +3523,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A122" s="3" t="s">
         <v>210</v>
       </c>
@@ -3322,7 +3532,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A123" s="3" t="s">
         <v>212</v>
       </c>
@@ -3331,7 +3541,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" spans="1:3" ht="308" x14ac:dyDescent="0.15">
       <c r="A124" s="3" t="s">
         <v>214</v>
       </c>
@@ -3340,14 +3550,14 @@
         <v>215</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" spans="1:3" ht="126" x14ac:dyDescent="0.15">
       <c r="A125" s="3" t="s">
         <v>216</v>
       </c>
       <c r="B125" s="6"/>
       <c r="C125" s="3"/>
     </row>
-    <row r="126" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A126" s="3" t="s">
         <v>217</v>
       </c>
@@ -3356,7 +3566,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A127" s="3" t="s">
         <v>219</v>
       </c>
@@ -3365,7 +3575,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A128" s="3" t="s">
         <v>221</v>
       </c>
@@ -3376,7 +3586,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A129" s="3" t="s">
         <v>224</v>
       </c>
@@ -3385,14 +3595,14 @@
         <v>225</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A130" s="3" t="s">
         <v>226</v>
       </c>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
     </row>
-    <row r="131" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" spans="1:3" ht="294" x14ac:dyDescent="0.15">
       <c r="A131" s="3" t="s">
         <v>227</v>
       </c>
@@ -3401,21 +3611,21 @@
         <v>228</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A132" s="3" t="s">
         <v>229</v>
       </c>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
     </row>
-    <row r="133" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A133" s="3" t="s">
         <v>230</v>
       </c>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
     </row>
-    <row r="134" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A134" s="3" t="s">
         <v>231</v>
       </c>
@@ -3426,42 +3636,42 @@
         <v>233</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A135" s="3" t="s">
         <v>234</v>
       </c>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
     </row>
-    <row r="136" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A136" s="3" t="s">
         <v>235</v>
       </c>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
     </row>
-    <row r="137" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A137" s="3" t="s">
         <v>236</v>
       </c>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
     </row>
-    <row r="138" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A138" s="3" t="s">
         <v>237</v>
       </c>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
     </row>
-    <row r="139" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A139" s="3" t="s">
         <v>238</v>
       </c>
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
     </row>
-    <row r="140" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" spans="1:3" ht="140" x14ac:dyDescent="0.15">
       <c r="A140" s="3" t="s">
         <v>239</v>
       </c>
@@ -3470,7 +3680,7 @@
       </c>
       <c r="C140" s="3"/>
     </row>
-    <row r="141" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" spans="1:3" ht="168" x14ac:dyDescent="0.15">
       <c r="A141" s="3" t="s">
         <v>241</v>
       </c>
@@ -3479,7 +3689,7 @@
       </c>
       <c r="C141" s="3"/>
     </row>
-    <row r="142" customFormat="false" ht="98" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A142" s="3" t="s">
         <v>243</v>
       </c>
@@ -3488,7 +3698,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" spans="1:3" ht="168" x14ac:dyDescent="0.15">
       <c r="A143" s="3" t="s">
         <v>245</v>
       </c>
@@ -3497,28 +3707,28 @@
         <v>246</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A144" s="3" t="s">
         <v>247</v>
       </c>
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
     </row>
-    <row r="145" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A145" s="3" t="s">
         <v>248</v>
       </c>
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
     </row>
-    <row r="146" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" spans="1:3" ht="112" x14ac:dyDescent="0.15">
       <c r="A146" s="3" t="s">
         <v>249</v>
       </c>
       <c r="B146" s="3"/>
       <c r="C146" s="3"/>
     </row>
-    <row r="147" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A147" s="3" t="s">
         <v>250</v>
       </c>
@@ -3529,21 +3739,21 @@
         <v>252</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" spans="1:3" ht="112" x14ac:dyDescent="0.15">
       <c r="A148" s="3" t="s">
         <v>253</v>
       </c>
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
     </row>
-    <row r="149" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" spans="1:3" ht="126" x14ac:dyDescent="0.15">
       <c r="A149" s="3" t="s">
         <v>254</v>
       </c>
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
     </row>
-    <row r="150" customFormat="false" ht="70" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A150" s="3" t="s">
         <v>255</v>
       </c>
@@ -3552,7 +3762,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" spans="1:3" ht="196" x14ac:dyDescent="0.15">
       <c r="A151" s="3" t="s">
         <v>257</v>
       </c>
@@ -3561,14 +3771,14 @@
       </c>
       <c r="C151" s="3"/>
     </row>
-    <row r="152" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A152" s="3" t="s">
         <v>259</v>
       </c>
       <c r="B152" s="3"/>
       <c r="C152" s="3"/>
     </row>
-    <row r="153" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A153" s="3" t="s">
         <v>260</v>
       </c>
@@ -3577,7 +3787,7 @@
       </c>
       <c r="C153" s="3"/>
     </row>
-    <row r="154" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" spans="1:3" ht="294" x14ac:dyDescent="0.15">
       <c r="A154" s="3" t="s">
         <v>262</v>
       </c>
@@ -3586,7 +3796,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" spans="1:3" ht="322" x14ac:dyDescent="0.15">
       <c r="A155" s="3" t="s">
         <v>264</v>
       </c>
@@ -3595,7 +3805,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="168" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A156" s="3" t="s">
         <v>266</v>
       </c>
@@ -3604,35 +3814,35 @@
         <v>267</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" spans="1:3" ht="140" x14ac:dyDescent="0.15">
       <c r="A157" s="3" t="s">
         <v>268</v>
       </c>
       <c r="B157" s="3"/>
       <c r="C157" s="3"/>
     </row>
-    <row r="158" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A158" s="3" t="s">
         <v>269</v>
       </c>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
     </row>
-    <row r="159" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A159" s="3" t="s">
         <v>270</v>
       </c>
       <c r="B159" s="3"/>
       <c r="C159" s="3"/>
     </row>
-    <row r="160" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" spans="1:3" ht="112" x14ac:dyDescent="0.15">
       <c r="A160" s="3" t="s">
         <v>271</v>
       </c>
       <c r="B160" s="3"/>
       <c r="C160" s="3"/>
     </row>
-    <row r="161" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" spans="1:3" ht="266" x14ac:dyDescent="0.15">
       <c r="A161" s="3" t="s">
         <v>272</v>
       </c>
@@ -3643,7 +3853,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" spans="1:3" ht="266" x14ac:dyDescent="0.15">
       <c r="A162" s="3" t="s">
         <v>275</v>
       </c>
@@ -3652,35 +3862,35 @@
         <v>276</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A163" s="3" t="s">
         <v>277</v>
       </c>
       <c r="B163" s="3"/>
       <c r="C163" s="3"/>
     </row>
-    <row r="164" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A164" s="3" t="s">
         <v>278</v>
       </c>
       <c r="B164" s="3"/>
       <c r="C164" s="3"/>
     </row>
-    <row r="165" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A165" s="3" t="s">
         <v>279</v>
       </c>
       <c r="B165" s="3"/>
       <c r="C165" s="3"/>
     </row>
-    <row r="166" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" spans="1:3" ht="126" x14ac:dyDescent="0.15">
       <c r="A166" s="3" t="s">
         <v>280</v>
       </c>
       <c r="B166" s="3"/>
       <c r="C166" s="3"/>
     </row>
-    <row r="167" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A167" s="3" t="s">
         <v>281</v>
       </c>
@@ -3689,7 +3899,7 @@
       </c>
       <c r="C167" s="3"/>
     </row>
-    <row r="168" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" spans="1:3" ht="266" x14ac:dyDescent="0.15">
       <c r="A168" s="3" t="s">
         <v>283</v>
       </c>
@@ -3698,7 +3908,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="364" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A169" s="3" t="s">
         <v>285</v>
       </c>
@@ -3709,14 +3919,14 @@
         <v>287</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A170" s="3" t="s">
         <v>288</v>
       </c>
       <c r="B170" s="3"/>
       <c r="C170" s="3"/>
     </row>
-    <row r="171" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" spans="1:3" ht="364" x14ac:dyDescent="0.15">
       <c r="A171" s="3" t="s">
         <v>289</v>
       </c>
@@ -3725,7 +3935,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" spans="1:3" ht="252" x14ac:dyDescent="0.15">
       <c r="A172" s="3" t="s">
         <v>291</v>
       </c>
@@ -3734,14 +3944,14 @@
         <v>292</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A173" s="3" t="s">
         <v>293</v>
       </c>
       <c r="B173" s="3"/>
       <c r="C173" s="3"/>
     </row>
-    <row r="174" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" spans="1:3" ht="140" x14ac:dyDescent="0.15">
       <c r="A174" s="3" t="s">
         <v>294</v>
       </c>
@@ -3752,14 +3962,14 @@
         <v>296</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A175" s="3" t="s">
         <v>297</v>
       </c>
       <c r="B175" s="3"/>
       <c r="C175" s="3"/>
     </row>
-    <row r="176" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" spans="1:3" ht="126" x14ac:dyDescent="0.15">
       <c r="A176" s="3" t="s">
         <v>298</v>
       </c>
@@ -3768,7 +3978,7 @@
       </c>
       <c r="C176" s="3"/>
     </row>
-    <row r="177" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" spans="1:3" ht="168" x14ac:dyDescent="0.15">
       <c r="A177" s="3" t="s">
         <v>300</v>
       </c>
@@ -3777,14 +3987,14 @@
         <v>301</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A178" s="3" t="s">
         <v>302</v>
       </c>
       <c r="B178" s="3"/>
       <c r="C178" s="3"/>
     </row>
-    <row r="179" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" spans="1:3" ht="406" x14ac:dyDescent="0.15">
       <c r="A179" s="3" t="s">
         <v>303</v>
       </c>
@@ -3793,7 +4003,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" spans="1:3" ht="126" x14ac:dyDescent="0.15">
       <c r="A180" s="3" t="s">
         <v>305</v>
       </c>
@@ -3802,7 +4012,7 @@
       </c>
       <c r="C180" s="3"/>
     </row>
-    <row r="181" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" spans="1:3" ht="126" x14ac:dyDescent="0.15">
       <c r="A181" s="3" t="s">
         <v>307</v>
       </c>
@@ -3811,21 +4021,21 @@
       </c>
       <c r="C181" s="3"/>
     </row>
-    <row r="182" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A182" s="3" t="s">
         <v>309</v>
       </c>
       <c r="B182" s="3"/>
       <c r="C182" s="3"/>
     </row>
-    <row r="183" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" spans="1:3" ht="112" x14ac:dyDescent="0.15">
       <c r="A183" s="3" t="s">
         <v>310</v>
       </c>
       <c r="B183" s="3"/>
       <c r="C183" s="3"/>
     </row>
-    <row r="184" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A184" s="3" t="s">
         <v>311</v>
       </c>
@@ -3834,7 +4044,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" spans="1:3" ht="378" x14ac:dyDescent="0.15">
       <c r="A185" s="3" t="s">
         <v>313</v>
       </c>
@@ -3843,14 +4053,14 @@
         <v>314</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A186" s="3" t="s">
         <v>315</v>
       </c>
       <c r="B186" s="3"/>
       <c r="C186" s="3"/>
     </row>
-    <row r="187" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" spans="1:3" ht="140" x14ac:dyDescent="0.15">
       <c r="A187" s="3" t="s">
         <v>316</v>
       </c>
@@ -3859,7 +4069,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" spans="1:3" ht="168" x14ac:dyDescent="0.15">
       <c r="A188" s="3" t="s">
         <v>318</v>
       </c>
@@ -3868,7 +4078,7 @@
       </c>
       <c r="C188" s="3"/>
     </row>
-    <row r="189" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" spans="1:3" ht="196" x14ac:dyDescent="0.15">
       <c r="A189" s="3" t="s">
         <v>320</v>
       </c>
@@ -3877,14 +4087,14 @@
         <v>321</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A190" s="3" t="s">
         <v>322</v>
       </c>
       <c r="B190" s="6"/>
       <c r="C190" s="3"/>
     </row>
-    <row r="191" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" spans="1:3" ht="168" x14ac:dyDescent="0.15">
       <c r="A191" s="3" t="s">
         <v>323</v>
       </c>
@@ -3893,7 +4103,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A192" s="3" t="s">
         <v>325</v>
       </c>
@@ -3902,14 +4112,14 @@
         <v>326</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="193" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A193" s="3" t="s">
         <v>327</v>
       </c>
       <c r="B193" s="6"/>
       <c r="C193" s="3"/>
     </row>
-    <row r="194" customFormat="false" ht="70" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A194" s="3" t="s">
         <v>328</v>
       </c>
@@ -3918,14 +4128,14 @@
         <v>329</v>
       </c>
     </row>
-    <row r="195" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="195" spans="1:3" ht="112" x14ac:dyDescent="0.15">
       <c r="A195" s="3" t="s">
         <v>330</v>
       </c>
       <c r="B195" s="3"/>
       <c r="C195" s="3"/>
     </row>
-    <row r="196" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" spans="1:3" ht="196" x14ac:dyDescent="0.15">
       <c r="A196" s="3" t="s">
         <v>331</v>
       </c>
@@ -3934,14 +4144,14 @@
       </c>
       <c r="C196" s="3"/>
     </row>
-    <row r="197" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A197" s="3" t="s">
         <v>333</v>
       </c>
       <c r="B197" s="3"/>
       <c r="C197" s="3"/>
     </row>
-    <row r="198" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A198" s="3" t="s">
         <v>334</v>
       </c>
@@ -3950,7 +4160,7 @@
       </c>
       <c r="C198" s="3"/>
     </row>
-    <row r="199" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" spans="1:3" ht="168" x14ac:dyDescent="0.15">
       <c r="A199" s="3" t="s">
         <v>336</v>
       </c>
@@ -3959,7 +4169,7 @@
       </c>
       <c r="C199" s="3"/>
     </row>
-    <row r="200" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="200" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A200" s="3" t="s">
         <v>338</v>
       </c>
@@ -3968,7 +4178,7 @@
       </c>
       <c r="C200" s="3"/>
     </row>
-    <row r="201" customFormat="false" ht="70" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A201" s="3" t="s">
         <v>340</v>
       </c>
@@ -3977,21 +4187,21 @@
         <v>341</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A202" s="3" t="s">
         <v>342</v>
       </c>
       <c r="B202" s="3"/>
       <c r="C202" s="3"/>
     </row>
-    <row r="203" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A203" s="3" t="s">
         <v>343</v>
       </c>
       <c r="B203" s="3"/>
       <c r="C203" s="3"/>
     </row>
-    <row r="204" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" spans="1:3" ht="140" x14ac:dyDescent="0.15">
       <c r="A204" s="3" t="s">
         <v>344</v>
       </c>
@@ -4000,7 +4210,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="205" spans="1:3" ht="196" x14ac:dyDescent="0.15">
       <c r="A205" s="3" t="s">
         <v>346</v>
       </c>
@@ -4009,7 +4219,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="206" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="206" spans="1:3" ht="406" x14ac:dyDescent="0.15">
       <c r="A206" s="3" t="s">
         <v>348</v>
       </c>
@@ -4018,7 +4228,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="207" customFormat="false" ht="98" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="207" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A207" s="3" t="s">
         <v>350</v>
       </c>
@@ -4027,14 +4237,14 @@
         <v>351</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="208" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A208" s="3" t="s">
         <v>352</v>
       </c>
       <c r="B208" s="3"/>
       <c r="C208" s="3"/>
     </row>
-    <row r="209" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="209" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A209" s="3" t="s">
         <v>353</v>
       </c>
@@ -4043,28 +4253,28 @@
       </c>
       <c r="C209" s="3"/>
     </row>
-    <row r="210" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="210" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A210" s="3" t="s">
         <v>355</v>
       </c>
       <c r="B210" s="3"/>
       <c r="C210" s="3"/>
     </row>
-    <row r="211" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A211" s="3" t="s">
         <v>356</v>
       </c>
       <c r="B211" s="3"/>
       <c r="C211" s="3"/>
     </row>
-    <row r="212" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="212" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A212" s="3" t="s">
         <v>357</v>
       </c>
       <c r="B212" s="3"/>
       <c r="C212" s="3"/>
     </row>
-    <row r="213" customFormat="false" ht="98" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="213" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A213" s="3" t="s">
         <v>358</v>
       </c>
@@ -4073,7 +4283,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="214" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="214" spans="1:3" ht="210" x14ac:dyDescent="0.15">
       <c r="A214" s="3" t="s">
         <v>360</v>
       </c>
@@ -4082,14 +4292,14 @@
         <v>361</v>
       </c>
     </row>
-    <row r="215" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="215" spans="1:3" ht="112" x14ac:dyDescent="0.15">
       <c r="A215" s="3" t="s">
         <v>362</v>
       </c>
       <c r="B215" s="3"/>
       <c r="C215" s="3"/>
     </row>
-    <row r="216" customFormat="false" ht="182" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="216" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A216" s="3" t="s">
         <v>363</v>
       </c>
@@ -4098,7 +4308,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="217" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="217" spans="1:3" ht="406" x14ac:dyDescent="0.15">
       <c r="A217" s="3" t="s">
         <v>365</v>
       </c>
@@ -4107,7 +4317,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="218" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="218" spans="1:3" ht="238" x14ac:dyDescent="0.15">
       <c r="A218" s="3" t="s">
         <v>367</v>
       </c>
@@ -4116,7 +4326,7 @@
       </c>
       <c r="C218" s="3"/>
     </row>
-    <row r="219" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="219" spans="1:3" ht="378" x14ac:dyDescent="0.15">
       <c r="A219" s="3" t="s">
         <v>369</v>
       </c>
@@ -4125,14 +4335,14 @@
         <v>370</v>
       </c>
     </row>
-    <row r="220" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="220" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A220" s="3" t="s">
         <v>371</v>
       </c>
       <c r="B220" s="3"/>
       <c r="C220" s="3"/>
     </row>
-    <row r="221" customFormat="false" ht="70" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="221" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A221" s="3" t="s">
         <v>372</v>
       </c>
@@ -4141,898 +4351,893 @@
         <v>373</v>
       </c>
     </row>
-    <row r="222" customFormat="false" ht="154" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="222" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A222" s="3" t="s">
         <v>374</v>
       </c>
       <c r="B222" s="3"/>
       <c r="C222" s="3" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" ht="409" x14ac:dyDescent="0.15">
+      <c r="A223" s="3" t="s">
         <v>375</v>
-      </c>
-    </row>
-    <row r="223" customFormat="false" ht="140" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="3" t="s">
-        <v>376</v>
       </c>
       <c r="B223" s="3"/>
       <c r="C223" s="3" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" ht="409" x14ac:dyDescent="0.15">
+      <c r="A224" s="3" t="s">
         <v>377</v>
-      </c>
-    </row>
-    <row r="224" customFormat="false" ht="294" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="3" t="s">
-        <v>378</v>
       </c>
       <c r="B224" s="3"/>
       <c r="C224" s="3" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" ht="98" x14ac:dyDescent="0.15">
+      <c r="A225" s="3" t="s">
         <v>379</v>
-      </c>
-    </row>
-    <row r="225" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="3" t="s">
-        <v>380</v>
       </c>
       <c r="B225" s="3"/>
       <c r="C225" s="3"/>
     </row>
-    <row r="226" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="226" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A226" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B226" s="3"/>
       <c r="C226" s="3" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" ht="140" x14ac:dyDescent="0.15">
+      <c r="A227" s="3" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="227" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="3" t="s">
+      <c r="B227" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="B227" s="3" t="s">
+      <c r="C227" s="3"/>
+    </row>
+    <row r="228" spans="1:3" ht="154" x14ac:dyDescent="0.15">
+      <c r="A228" s="3" t="s">
         <v>384</v>
-      </c>
-      <c r="C227" s="3"/>
-    </row>
-    <row r="228" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="3" t="s">
-        <v>385</v>
       </c>
       <c r="B228" s="3"/>
       <c r="C228" s="3" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" ht="84" x14ac:dyDescent="0.15">
+      <c r="A229" s="3" t="s">
         <v>386</v>
-      </c>
-    </row>
-    <row r="229" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="3" t="s">
-        <v>387</v>
       </c>
       <c r="B229" s="3"/>
       <c r="C229" s="3"/>
     </row>
-    <row r="230" customFormat="false" ht="98" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="230" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A230" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B230" s="3"/>
       <c r="C230" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" ht="409" x14ac:dyDescent="0.15">
+      <c r="A231" s="3" t="s">
         <v>389</v>
-      </c>
-    </row>
-    <row r="231" customFormat="false" ht="126" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="3" t="s">
-        <v>390</v>
       </c>
       <c r="B231" s="3"/>
       <c r="C231" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" ht="84" x14ac:dyDescent="0.15">
+      <c r="A232" s="3" t="s">
         <v>391</v>
-      </c>
-    </row>
-    <row r="232" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="3" t="s">
-        <v>392</v>
       </c>
       <c r="B232" s="3"/>
       <c r="C232" s="3"/>
     </row>
-    <row r="233" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="233" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A233" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B233" s="3"/>
       <c r="C233" s="3"/>
     </row>
-    <row r="234" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="234" spans="1:3" ht="112" x14ac:dyDescent="0.15">
       <c r="A234" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B234" s="3"/>
       <c r="C234" s="3"/>
     </row>
-    <row r="235" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="235" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A235" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="B235" s="3" t="s">
         <v>395</v>
       </c>
-      <c r="B235" s="3" t="s">
+      <c r="C235" s="3"/>
+    </row>
+    <row r="236" spans="1:3" ht="280" x14ac:dyDescent="0.15">
+      <c r="A236" s="3" t="s">
         <v>396</v>
-      </c>
-      <c r="C235" s="3"/>
-    </row>
-    <row r="236" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A236" s="3" t="s">
-        <v>397</v>
       </c>
       <c r="B236" s="3"/>
       <c r="C236" s="3" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" ht="70" x14ac:dyDescent="0.15">
+      <c r="A237" s="3" t="s">
         <v>398</v>
-      </c>
-    </row>
-    <row r="237" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A237" s="3" t="s">
-        <v>399</v>
       </c>
       <c r="B237" s="3"/>
       <c r="C237" s="3"/>
     </row>
-    <row r="238" customFormat="false" ht="196" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="238" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A238" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B238" s="3"/>
       <c r="C238" s="3" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" ht="409" x14ac:dyDescent="0.15">
+      <c r="A239" s="3" t="s">
         <v>401</v>
-      </c>
-    </row>
-    <row r="239" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A239" s="3" t="s">
-        <v>402</v>
       </c>
       <c r="B239" s="3"/>
       <c r="C239" s="3" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" ht="70" x14ac:dyDescent="0.15">
+      <c r="A240" s="3" t="s">
         <v>403</v>
-      </c>
-    </row>
-    <row r="240" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A240" s="3" t="s">
-        <v>404</v>
       </c>
       <c r="B240" s="3"/>
       <c r="C240" s="3"/>
     </row>
-    <row r="241" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="241" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A241" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B241" s="3"/>
       <c r="C241" s="3" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" ht="84" x14ac:dyDescent="0.15">
+      <c r="A242" s="3" t="s">
         <v>406</v>
-      </c>
-    </row>
-    <row r="242" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A242" s="3" t="s">
-        <v>407</v>
       </c>
       <c r="B242" s="3"/>
       <c r="C242" s="3"/>
     </row>
-    <row r="243" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="243" spans="1:3" ht="126" x14ac:dyDescent="0.15">
       <c r="A243" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B243" s="3"/>
       <c r="C243" s="3"/>
     </row>
-    <row r="244" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="244" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A244" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B244" s="3"/>
       <c r="C244" s="3" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" ht="409" x14ac:dyDescent="0.15">
+      <c r="A245" s="3" t="s">
         <v>410</v>
-      </c>
-    </row>
-    <row r="245" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="3" t="s">
-        <v>411</v>
       </c>
       <c r="B245" s="3"/>
       <c r="C245" s="3" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" ht="140" x14ac:dyDescent="0.15">
+      <c r="A246" s="3" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="246" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A246" s="3" t="s">
+      <c r="B246" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="B246" s="3" t="s">
+      <c r="C246" s="3"/>
+    </row>
+    <row r="247" spans="1:3" ht="294" x14ac:dyDescent="0.15">
+      <c r="A247" s="3" t="s">
         <v>414</v>
-      </c>
-      <c r="C246" s="3"/>
-    </row>
-    <row r="247" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A247" s="3" t="s">
-        <v>415</v>
       </c>
       <c r="B247" s="3"/>
       <c r="C247" s="3" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" ht="409" x14ac:dyDescent="0.15">
+      <c r="A248" s="3" t="s">
         <v>416</v>
-      </c>
-    </row>
-    <row r="248" customFormat="false" ht="70" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A248" s="3" t="s">
-        <v>417</v>
       </c>
       <c r="B248" s="3"/>
       <c r="C248" s="3" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" ht="70" x14ac:dyDescent="0.15">
+      <c r="A249" s="3" t="s">
         <v>418</v>
-      </c>
-    </row>
-    <row r="249" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="3" t="s">
-        <v>419</v>
       </c>
       <c r="B249" s="3"/>
       <c r="C249" s="3"/>
     </row>
-    <row r="250" customFormat="false" ht="140" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="250" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A250" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B250" s="3"/>
       <c r="C250" s="3" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" ht="126" x14ac:dyDescent="0.15">
+      <c r="A251" s="3" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="251" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A251" s="3" t="s">
+      <c r="B251" s="3" t="s">
         <v>422</v>
       </c>
-      <c r="B251" s="3" t="s">
+      <c r="C251" s="3"/>
+    </row>
+    <row r="252" spans="1:3" ht="409" x14ac:dyDescent="0.15">
+      <c r="A252" s="3" t="s">
         <v>423</v>
-      </c>
-      <c r="C251" s="3"/>
-    </row>
-    <row r="252" customFormat="false" ht="140" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A252" s="3" t="s">
-        <v>424</v>
       </c>
       <c r="B252" s="3"/>
       <c r="C252" s="3" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" ht="98" x14ac:dyDescent="0.15">
+      <c r="A253" s="3" t="s">
         <v>425</v>
-      </c>
-    </row>
-    <row r="253" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A253" s="3" t="s">
-        <v>426</v>
       </c>
       <c r="B253" s="3"/>
       <c r="C253" s="3"/>
     </row>
-    <row r="254" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="254" spans="1:3" ht="168" x14ac:dyDescent="0.15">
       <c r="A254" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B254" s="3"/>
       <c r="C254" s="3" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" ht="126" x14ac:dyDescent="0.15">
+      <c r="A255" s="3" t="s">
         <v>428</v>
-      </c>
-    </row>
-    <row r="255" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="3" t="s">
-        <v>429</v>
       </c>
       <c r="B255" s="3"/>
       <c r="C255" s="3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" ht="70" x14ac:dyDescent="0.15">
+      <c r="A256" s="3" t="s">
         <v>430</v>
-      </c>
-    </row>
-    <row r="256" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A256" s="3" t="s">
-        <v>431</v>
       </c>
       <c r="B256" s="3"/>
       <c r="C256" s="3"/>
     </row>
-    <row r="257" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="257" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A257" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B257" s="3"/>
       <c r="C257" s="3"/>
     </row>
-    <row r="258" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="258" spans="1:3" ht="196" x14ac:dyDescent="0.15">
       <c r="A258" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B258" s="3"/>
       <c r="C258" s="3" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" ht="210" x14ac:dyDescent="0.15">
+      <c r="A259" s="3" t="s">
         <v>434</v>
-      </c>
-    </row>
-    <row r="259" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A259" s="3" t="s">
-        <v>435</v>
       </c>
       <c r="B259" s="3"/>
       <c r="C259" s="3" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" ht="112" x14ac:dyDescent="0.15">
+      <c r="A260" s="3" t="s">
         <v>436</v>
-      </c>
-    </row>
-    <row r="260" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A260" s="3" t="s">
-        <v>437</v>
       </c>
       <c r="B260" s="3"/>
       <c r="C260" s="3"/>
     </row>
-    <row r="261" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="261" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A261" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B261" s="3"/>
       <c r="C261" s="3"/>
     </row>
-    <row r="262" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="262" spans="1:3" ht="196" x14ac:dyDescent="0.15">
       <c r="A262" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="B262" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="B262" s="3" t="s">
+      <c r="C262" s="3"/>
+    </row>
+    <row r="263" spans="1:3" ht="56" x14ac:dyDescent="0.15">
+      <c r="A263" s="3" t="s">
         <v>440</v>
-      </c>
-      <c r="C262" s="3"/>
-    </row>
-    <row r="263" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A263" s="3" t="s">
-        <v>441</v>
       </c>
       <c r="B263" s="3"/>
       <c r="C263" s="3"/>
     </row>
-    <row r="264" customFormat="false" ht="112" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="264" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A264" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B264" s="3"/>
       <c r="C264" s="3" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" ht="350" x14ac:dyDescent="0.15">
+      <c r="A265" s="3" t="s">
         <v>443</v>
-      </c>
-    </row>
-    <row r="265" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A265" s="3" t="s">
-        <v>444</v>
       </c>
       <c r="B265" s="3"/>
       <c r="C265" s="3" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" ht="70" x14ac:dyDescent="0.15">
+      <c r="A266" s="3" t="s">
         <v>445</v>
-      </c>
-    </row>
-    <row r="266" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A266" s="3" t="s">
-        <v>446</v>
       </c>
       <c r="B266" s="3"/>
       <c r="C266" s="3"/>
     </row>
-    <row r="267" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="267" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A267" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B267" s="3"/>
       <c r="C267" s="3"/>
     </row>
-    <row r="268" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="268" spans="1:3" ht="280" x14ac:dyDescent="0.15">
       <c r="A268" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B268" s="3"/>
       <c r="C268" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" ht="294" x14ac:dyDescent="0.15">
+      <c r="A269" s="3" t="s">
         <v>449</v>
-      </c>
-    </row>
-    <row r="269" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A269" s="3" t="s">
-        <v>450</v>
       </c>
       <c r="B269" s="3"/>
       <c r="C269" s="3" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" ht="56" x14ac:dyDescent="0.15">
+      <c r="A270" s="3" t="s">
         <v>451</v>
-      </c>
-    </row>
-    <row r="270" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A270" s="3" t="s">
-        <v>452</v>
       </c>
       <c r="B270" s="3"/>
       <c r="C270" s="3"/>
     </row>
-    <row r="271" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="271" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A271" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B271" s="3"/>
       <c r="C271" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" ht="84" x14ac:dyDescent="0.15">
+      <c r="A272" s="3" t="s">
         <v>454</v>
-      </c>
-    </row>
-    <row r="272" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A272" s="3" t="s">
-        <v>455</v>
       </c>
       <c r="B272" s="3"/>
       <c r="C272" s="3"/>
     </row>
-    <row r="273" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="273" spans="1:3" ht="168" x14ac:dyDescent="0.15">
       <c r="A273" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="B273" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="B273" s="3" t="s">
+      <c r="C273" s="3"/>
+    </row>
+    <row r="274" spans="1:3" ht="98" x14ac:dyDescent="0.15">
+      <c r="A274" s="3" t="s">
         <v>457</v>
-      </c>
-      <c r="C273" s="3"/>
-    </row>
-    <row r="274" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="3" t="s">
-        <v>458</v>
       </c>
       <c r="B274" s="3"/>
       <c r="C274" s="3"/>
     </row>
-    <row r="275" customFormat="false" ht="154" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="275" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A275" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B275" s="3"/>
       <c r="C275" s="3" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" ht="98" x14ac:dyDescent="0.15">
+      <c r="A276" s="3" t="s">
         <v>460</v>
-      </c>
-    </row>
-    <row r="276" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="3" t="s">
-        <v>461</v>
       </c>
       <c r="B276" s="3"/>
       <c r="C276" s="3"/>
     </row>
-    <row r="277" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="277" spans="1:3" ht="308" x14ac:dyDescent="0.15">
       <c r="A277" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B277" s="3"/>
       <c r="C277" s="3" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" ht="266" x14ac:dyDescent="0.15">
+      <c r="A278" s="3" t="s">
         <v>463</v>
-      </c>
-    </row>
-    <row r="278" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A278" s="3" t="s">
-        <v>464</v>
       </c>
       <c r="B278" s="3"/>
       <c r="C278" s="3" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" ht="409" x14ac:dyDescent="0.15">
+      <c r="A279" s="3" t="s">
         <v>465</v>
-      </c>
-    </row>
-    <row r="279" customFormat="false" ht="126" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A279" s="3" t="s">
-        <v>466</v>
       </c>
       <c r="B279" s="3"/>
       <c r="C279" s="3" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" ht="409" x14ac:dyDescent="0.15">
+      <c r="A280" s="3" t="s">
         <v>467</v>
-      </c>
-    </row>
-    <row r="280" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A280" s="3" t="s">
-        <v>468</v>
       </c>
       <c r="B280" s="3"/>
       <c r="C280" s="3" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" ht="84" x14ac:dyDescent="0.15">
+      <c r="A281" s="3" t="s">
         <v>469</v>
-      </c>
-    </row>
-    <row r="281" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A281" s="3" t="s">
-        <v>470</v>
       </c>
       <c r="B281" s="3"/>
       <c r="C281" s="3"/>
     </row>
-    <row r="282" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="282" spans="1:3" ht="140" x14ac:dyDescent="0.15">
       <c r="A282" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B282" s="3"/>
       <c r="C282" s="3" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" ht="210" x14ac:dyDescent="0.15">
+      <c r="A283" s="3" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="283" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A283" s="3" t="s">
+      <c r="B283" s="3" t="s">
         <v>473</v>
       </c>
-      <c r="B283" s="3" t="s">
+      <c r="C283" s="3" t="s">
         <v>474</v>
       </c>
-      <c r="C283" s="3" t="s">
+    </row>
+    <row r="284" spans="1:3" ht="98" x14ac:dyDescent="0.15">
+      <c r="A284" s="3" t="s">
         <v>475</v>
-      </c>
-    </row>
-    <row r="284" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A284" s="3" t="s">
-        <v>476</v>
       </c>
       <c r="B284" s="3"/>
       <c r="C284" s="3"/>
     </row>
-    <row r="285" customFormat="false" ht="98" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="285" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A285" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B285" s="3"/>
       <c r="C285" s="3" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" ht="182" x14ac:dyDescent="0.15">
+      <c r="A286" s="3" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="286" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A286" s="3" t="s">
+      <c r="B286" s="3" t="s">
         <v>479</v>
       </c>
-      <c r="B286" s="3" t="s">
+      <c r="C286" s="3"/>
+    </row>
+    <row r="287" spans="1:3" ht="126" x14ac:dyDescent="0.15">
+      <c r="A287" s="3" t="s">
         <v>480</v>
       </c>
-      <c r="C286" s="3"/>
-    </row>
-    <row r="287" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A287" s="3" t="s">
+      <c r="B287" s="3" t="s">
         <v>481</v>
       </c>
-      <c r="B287" s="3" t="s">
+      <c r="C287" s="3"/>
+    </row>
+    <row r="288" spans="1:3" ht="84" x14ac:dyDescent="0.15">
+      <c r="A288" s="3" t="s">
         <v>482</v>
-      </c>
-      <c r="C287" s="3"/>
-    </row>
-    <row r="288" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A288" s="3" t="s">
-        <v>483</v>
       </c>
       <c r="B288" s="3"/>
       <c r="C288" s="3"/>
     </row>
-    <row r="289" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="289" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A289" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B289" s="3"/>
       <c r="C289" s="3" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" ht="154" x14ac:dyDescent="0.15">
+      <c r="A290" s="3" t="s">
         <v>485</v>
-      </c>
-    </row>
-    <row r="290" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A290" s="3" t="s">
-        <v>486</v>
       </c>
       <c r="B290" s="3"/>
       <c r="C290" s="3" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" ht="154" x14ac:dyDescent="0.15">
+      <c r="A291" s="3" t="s">
         <v>487</v>
-      </c>
-    </row>
-    <row r="291" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A291" s="3" t="s">
-        <v>488</v>
       </c>
       <c r="B291" s="3"/>
       <c r="C291" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" ht="126" x14ac:dyDescent="0.15">
+      <c r="A292" s="3" t="s">
         <v>489</v>
-      </c>
-    </row>
-    <row r="292" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A292" s="3" t="s">
-        <v>490</v>
       </c>
       <c r="B292" s="3"/>
       <c r="C292" s="3" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" ht="409" x14ac:dyDescent="0.15">
+      <c r="A293" s="3" t="s">
         <v>491</v>
-      </c>
-    </row>
-    <row r="293" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A293" s="3" t="s">
-        <v>492</v>
       </c>
       <c r="B293" s="3"/>
       <c r="C293" s="3" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" ht="168" x14ac:dyDescent="0.15">
+      <c r="A294" s="3" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="294" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A294" s="3" t="s">
+      <c r="B294" s="3" t="s">
         <v>494</v>
       </c>
-      <c r="B294" s="3" t="s">
+      <c r="C294" s="3" t="s">
         <v>495</v>
       </c>
-      <c r="C294" s="3" t="s">
+    </row>
+    <row r="295" spans="1:3" ht="70" x14ac:dyDescent="0.15">
+      <c r="A295" s="3" t="s">
         <v>496</v>
-      </c>
-    </row>
-    <row r="295" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A295" s="3" t="s">
-        <v>497</v>
       </c>
       <c r="B295" s="3"/>
       <c r="C295" s="3"/>
     </row>
-    <row r="296" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="296" spans="1:3" ht="182" x14ac:dyDescent="0.15">
       <c r="A296" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B296" s="3"/>
       <c r="C296" s="3" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" ht="168" x14ac:dyDescent="0.15">
+      <c r="A297" s="3" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="297" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A297" s="3" t="s">
+      <c r="B297" s="3" t="s">
         <v>500</v>
       </c>
-      <c r="B297" s="3" t="s">
+      <c r="C297" s="3"/>
+    </row>
+    <row r="298" spans="1:3" ht="196" x14ac:dyDescent="0.15">
+      <c r="A298" s="3" t="s">
         <v>501</v>
       </c>
-      <c r="C297" s="3"/>
-    </row>
-    <row r="298" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A298" s="3" t="s">
+      <c r="B298" s="3" t="s">
         <v>502</v>
       </c>
-      <c r="B298" s="3" t="s">
+      <c r="C298" s="3" t="s">
         <v>503</v>
       </c>
-      <c r="C298" s="3" t="s">
+    </row>
+    <row r="299" spans="1:3" ht="409" x14ac:dyDescent="0.15">
+      <c r="A299" s="3" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="299" customFormat="false" ht="252" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A299" s="3" t="s">
+      <c r="B299" s="3" t="s">
         <v>505</v>
       </c>
-      <c r="B299" s="3" t="s">
+      <c r="C299" s="3" t="s">
         <v>506</v>
       </c>
-      <c r="C299" s="3" t="s">
+    </row>
+    <row r="300" spans="1:3" ht="70" x14ac:dyDescent="0.15">
+      <c r="A300" s="3" t="s">
         <v>507</v>
-      </c>
-    </row>
-    <row r="300" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A300" s="3" t="s">
-        <v>508</v>
       </c>
       <c r="B300" s="3"/>
       <c r="C300" s="3"/>
     </row>
-    <row r="301" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="301" spans="1:3" ht="112" x14ac:dyDescent="0.15">
       <c r="A301" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B301" s="3"/>
       <c r="C301" s="3"/>
     </row>
-    <row r="302" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="302" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A302" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B302" s="3"/>
       <c r="C302" s="3" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" ht="70" x14ac:dyDescent="0.15">
+      <c r="A303" s="3" t="s">
         <v>511</v>
-      </c>
-    </row>
-    <row r="303" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A303" s="3" t="s">
-        <v>512</v>
       </c>
       <c r="B303" s="3"/>
       <c r="C303" s="3"/>
     </row>
-    <row r="304" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="304" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A304" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B304" s="3"/>
       <c r="C304" s="3"/>
     </row>
-    <row r="305" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="305" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A305" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B305" s="3"/>
       <c r="C305" s="3"/>
     </row>
-    <row r="306" customFormat="false" ht="126" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="306" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A306" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B306" s="3"/>
       <c r="C306" s="3" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" ht="406" x14ac:dyDescent="0.15">
+      <c r="A307" s="3" t="s">
         <v>516</v>
-      </c>
-    </row>
-    <row r="307" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A307" s="3" t="s">
-        <v>517</v>
       </c>
       <c r="B307" s="3"/>
       <c r="C307" s="3" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" ht="84" x14ac:dyDescent="0.15">
+      <c r="A308" s="3" t="s">
         <v>518</v>
-      </c>
-    </row>
-    <row r="308" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A308" s="3" t="s">
-        <v>519</v>
       </c>
       <c r="B308" s="3"/>
       <c r="C308" s="3"/>
     </row>
-    <row r="309" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="309" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A309" s="3" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B309" s="3"/>
       <c r="C309" s="3"/>
     </row>
-    <row r="310" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="310" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A310" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B310" s="3"/>
       <c r="C310" s="3" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" ht="409" x14ac:dyDescent="0.15">
+      <c r="A311" s="3" t="s">
         <v>522</v>
-      </c>
-    </row>
-    <row r="311" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A311" s="3" t="s">
-        <v>523</v>
       </c>
       <c r="B311" s="3"/>
       <c r="C311" s="3" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" ht="350" x14ac:dyDescent="0.15">
+      <c r="A312" s="3" t="s">
         <v>524</v>
-      </c>
-    </row>
-    <row r="312" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A312" s="3" t="s">
-        <v>525</v>
       </c>
       <c r="B312" s="3"/>
       <c r="C312" s="3" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" ht="280" x14ac:dyDescent="0.15">
+      <c r="A313" s="3" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="313" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A313" s="3" t="s">
+      <c r="B313" s="3" t="s">
         <v>527</v>
       </c>
-      <c r="B313" s="3" t="s">
+      <c r="C313" s="3"/>
+    </row>
+    <row r="314" spans="1:3" ht="84" x14ac:dyDescent="0.15">
+      <c r="A314" s="3" t="s">
         <v>528</v>
-      </c>
-      <c r="C313" s="3"/>
-    </row>
-    <row r="314" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A314" s="3" t="s">
-        <v>529</v>
       </c>
       <c r="B314" s="3"/>
       <c r="C314" s="3"/>
     </row>
-    <row r="315" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="315" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A315" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B315" s="3"/>
       <c r="C315" s="3"/>
     </row>
-    <row r="316" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="316" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A316" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B316" s="3"/>
       <c r="C316" s="3"/>
     </row>
-    <row r="317" customFormat="false" ht="98" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="317" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A317" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B317" s="3"/>
       <c r="C317" s="3" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" ht="409" x14ac:dyDescent="0.15">
+      <c r="A318" s="3" t="s">
         <v>533</v>
-      </c>
-    </row>
-    <row r="318" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A318" s="3" t="s">
-        <v>534</v>
       </c>
       <c r="B318" s="3"/>
       <c r="C318" s="3" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" ht="409" x14ac:dyDescent="0.15">
+      <c r="A319" s="3" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="319" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A319" s="3" t="s">
+      <c r="B319" s="3" t="s">
         <v>536</v>
       </c>
-      <c r="B319" s="3" t="s">
+      <c r="C319" s="3" t="s">
         <v>537</v>
       </c>
-      <c r="C319" s="3" t="s">
+    </row>
+    <row r="320" spans="1:3" ht="294" x14ac:dyDescent="0.15">
+      <c r="A320" s="3" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="320" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A320" s="3" t="s">
+      <c r="B320" s="3" t="s">
         <v>539</v>
       </c>
-      <c r="B320" s="3" t="s">
+      <c r="C320" s="3" t="s">
         <v>540</v>
       </c>
-      <c r="C320" s="3" t="s">
+    </row>
+    <row r="321" spans="1:3" ht="308" x14ac:dyDescent="0.15">
+      <c r="A321" s="3" t="s">
         <v>541</v>
-      </c>
-    </row>
-    <row r="321" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A321" s="3" t="s">
-        <v>542</v>
       </c>
       <c r="B321" s="3"/>
       <c r="C321" s="3" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" ht="154" x14ac:dyDescent="0.15">
+      <c r="A322" s="3" t="s">
         <v>543</v>
-      </c>
-    </row>
-    <row r="322" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A322" s="3" t="s">
-        <v>544</v>
       </c>
       <c r="B322" s="3"/>
       <c r="C322" s="3" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" ht="140" x14ac:dyDescent="0.15">
+      <c r="A323" s="3" t="s">
         <v>545</v>
-      </c>
-    </row>
-    <row r="323" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A323" s="3" t="s">
-        <v>546</v>
       </c>
       <c r="B323" s="3"/>
       <c r="C323" s="3" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" ht="409" x14ac:dyDescent="0.15">
+      <c r="A324" s="3" t="s">
         <v>547</v>
-      </c>
-    </row>
-    <row r="324" customFormat="false" ht="182" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A324" s="3" t="s">
-        <v>548</v>
       </c>
       <c r="B324" s="3"/>
       <c r="C324" s="3" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" ht="140" x14ac:dyDescent="0.15">
+      <c r="A325" s="3" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="325" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A325" s="3" t="s">
+      <c r="B325" s="3" t="s">
         <v>550</v>
       </c>
-      <c r="B325" s="3" t="s">
+      <c r="C325" s="3"/>
+    </row>
+    <row r="326" spans="1:3" ht="409" x14ac:dyDescent="0.15">
+      <c r="A326" s="3" t="s">
         <v>551</v>
-      </c>
-      <c r="C325" s="3"/>
-    </row>
-    <row r="326" customFormat="false" ht="350" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A326" s="3" t="s">
-        <v>552</v>
       </c>
       <c r="B326" s="3"/>
       <c r="C326" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Clean up hierarchical mapping loops
</commit_message>
<xml_diff>
--- a/mappings/kegg_reactome.xlsx
+++ b/mappings/kegg_reactome.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="1680" windowWidth="29320" windowHeight="13020" tabRatio="991"/>
+    <workbookView xWindow="600" yWindow="500" windowWidth="29320" windowHeight="13020" tabRatio="991"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -515,15 +515,6 @@
     <t>Cytokine-cytokine receptor interaction - Homo sapiens (human)</t>
   </si>
   <si>
-    <t>Cytokine-cytokine receptor interaction - Homo sapiens (human)* isPartOf Cytokine Signaling in Immune system
-Cytokine-cytokine receptor interaction - Homo sapiens (human)* isPartOf Immune System
-IL-6-type cytokine receptor ligand interactions isPartOf Cytokine-cytokine receptor interaction - Homo sapiens (human)*
-Cytokine-cytokine receptor interaction - Homo sapiens (human)* isPartOf IL-6-type cytokine receptor ligand interactions
-TNFs bind their physiological receptors isPartOf Cytokine-cytokine receptor interaction - Homo sapiens (human)*
-Chemokine receptors bind chemokines isPartOf Cytokine-cytokine receptor interaction - Homo sapiens (human)*
-Cytokine-cytokine receptor interaction - Homo sapiens (human)* isPartOf Ligand-receptor interactions</t>
-  </si>
-  <si>
     <t>Cytosolic DNA-sensing pathway - Homo sapiens (human)</t>
   </si>
   <si>
@@ -2119,6 +2110,14 @@
   <si>
     <t>Fatty acid biosynthesis - Homo sapiens (human)* isPartOf Metabolism
 Fatty acyl-CoA biosynthesis isPartOf Fatty acid biosynthesis - Homo sapiens (human)*</t>
+  </si>
+  <si>
+    <t>Cytokine-cytokine receptor interaction - Homo sapiens (human)* isPartOf Cytokine Signaling in Immune system
+Cytokine-cytokine receptor interaction - Homo sapiens (human)* isPartOf Immune System
+IL-6-type cytokine receptor ligand interactions isPartOf Cytokine-cytokine receptor interaction - Homo sapiens (human)*
+TNFs bind their physiological receptors isPartOf Cytokine-cytokine receptor interaction - Homo sapiens (human)*
+Chemokine receptors bind chemokines isPartOf Cytokine-cytokine receptor interaction - Homo sapiens (human)*
+Cytokine-cytokine receptor interaction - Homo sapiens (human)* isPartOf Ligand-receptor interactions</t>
   </si>
 </sst>
 </file>
@@ -2468,8 +2467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y326"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="C96" sqref="C96"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="Q74" sqref="Q74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3115,2123 +3114,2123 @@
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="3" t="s">
-        <v>125</v>
+        <v>553</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="196" x14ac:dyDescent="0.15">
       <c r="A75" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B75" s="3"/>
       <c r="C75" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="364" x14ac:dyDescent="0.15">
       <c r="A76" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A77" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B77" s="3"/>
       <c r="C77" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="126" x14ac:dyDescent="0.15">
       <c r="A78" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B78" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>133</v>
       </c>
       <c r="C78" s="3"/>
     </row>
     <row r="79" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A79" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
     </row>
     <row r="80" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A80" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B80" s="3"/>
       <c r="C80" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A81" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B81" s="3"/>
       <c r="C81" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="140" x14ac:dyDescent="0.15">
       <c r="A82" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B82" s="3"/>
       <c r="C82" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A83" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B83" s="3"/>
       <c r="C83" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="112" x14ac:dyDescent="0.15">
       <c r="A84" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
     </row>
     <row r="85" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A85" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
     </row>
     <row r="86" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A86" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
     </row>
     <row r="87" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A87" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B87" s="3"/>
       <c r="C87" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A88" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
     </row>
     <row r="89" spans="1:3" ht="140" x14ac:dyDescent="0.15">
       <c r="A89" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
     </row>
     <row r="90" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A90" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
     </row>
     <row r="91" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A91" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B91" s="3"/>
       <c r="C91" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A92" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
     </row>
     <row r="93" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A93" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B93" s="3"/>
       <c r="C93" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A94" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B94" s="3" t="s">
         <v>156</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>157</v>
       </c>
       <c r="C94" s="3"/>
     </row>
     <row r="95" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A95" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B95" s="3"/>
       <c r="C95" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="280" x14ac:dyDescent="0.15">
       <c r="A96" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B96" s="3"/>
       <c r="C96" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A97" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B97" s="3"/>
       <c r="C97" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A98" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B98" s="3"/>
       <c r="C98" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="238" x14ac:dyDescent="0.15">
       <c r="A99" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B99" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B99" s="3" t="s">
+      <c r="C99" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="364" x14ac:dyDescent="0.15">
       <c r="A100" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B100" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="C100" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="238" x14ac:dyDescent="0.15">
       <c r="A101" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B101" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>172</v>
       </c>
       <c r="C101" s="3"/>
     </row>
     <row r="102" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A102" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B102" s="3"/>
       <c r="C102" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="126" x14ac:dyDescent="0.15">
       <c r="A103" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
     </row>
     <row r="104" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A104" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B104" s="3"/>
       <c r="C104" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A105" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B105" s="3"/>
       <c r="C105" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="168" x14ac:dyDescent="0.15">
       <c r="A106" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B106" s="3"/>
       <c r="C106" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A107" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B107" s="3"/>
       <c r="C107" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A108" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B108" s="3"/>
       <c r="C108" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="126" x14ac:dyDescent="0.15">
       <c r="A109" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B109" s="3"/>
       <c r="C109" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A110" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B110" s="3"/>
       <c r="C110" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A111" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
     </row>
     <row r="112" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A112" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
     </row>
     <row r="113" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A113" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
     </row>
     <row r="114" spans="1:3" ht="196" x14ac:dyDescent="0.15">
       <c r="A114" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B114" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>194</v>
       </c>
       <c r="C114" s="3"/>
     </row>
     <row r="115" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A115" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B115" s="3"/>
       <c r="C115" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="182" x14ac:dyDescent="0.15">
       <c r="A116" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B116" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>198</v>
       </c>
       <c r="C116" s="3"/>
     </row>
     <row r="117" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A117" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B117" s="6"/>
       <c r="C117" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A118" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B118" s="6"/>
       <c r="C118" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A119" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B119" s="6"/>
       <c r="C119" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A120" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B120" s="6"/>
       <c r="C120" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A121" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B121" s="6"/>
       <c r="C121" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A122" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B122" s="6"/>
       <c r="C122" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A123" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B123" s="6"/>
       <c r="C123" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="308" x14ac:dyDescent="0.15">
       <c r="A124" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B124" s="6"/>
       <c r="C124" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="126" x14ac:dyDescent="0.15">
       <c r="A125" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B125" s="6"/>
       <c r="C125" s="3"/>
     </row>
     <row r="126" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A126" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B126" s="6"/>
       <c r="C126" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A127" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B127" s="3"/>
       <c r="C127" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A128" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B128" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="B128" s="3" t="s">
+      <c r="C128" s="3" t="s">
         <v>221</v>
-      </c>
-      <c r="C128" s="3" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A129" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B129" s="3"/>
       <c r="C129" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A130" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
     </row>
     <row r="131" spans="1:3" ht="294" x14ac:dyDescent="0.15">
       <c r="A131" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B131" s="3"/>
       <c r="C131" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A132" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
     </row>
     <row r="133" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A133" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
     </row>
     <row r="134" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A134" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B134" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="B134" s="3" t="s">
+      <c r="C134" s="3" t="s">
         <v>231</v>
-      </c>
-      <c r="C134" s="3" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A135" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
     </row>
     <row r="136" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A136" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
     </row>
     <row r="137" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A137" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
     </row>
     <row r="138" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A138" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
     </row>
     <row r="139" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A139" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
     </row>
     <row r="140" spans="1:3" ht="140" x14ac:dyDescent="0.15">
       <c r="A140" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B140" s="3" t="s">
         <v>238</v>
-      </c>
-      <c r="B140" s="3" t="s">
-        <v>239</v>
       </c>
       <c r="C140" s="3"/>
     </row>
     <row r="141" spans="1:3" ht="168" x14ac:dyDescent="0.15">
       <c r="A141" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B141" s="3" t="s">
         <v>240</v>
-      </c>
-      <c r="B141" s="3" t="s">
-        <v>241</v>
       </c>
       <c r="C141" s="3"/>
     </row>
     <row r="142" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A142" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B142" s="3"/>
       <c r="C142" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="168" x14ac:dyDescent="0.15">
       <c r="A143" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B143" s="3"/>
       <c r="C143" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A144" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
     </row>
     <row r="145" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A145" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
     </row>
     <row r="146" spans="1:3" ht="112" x14ac:dyDescent="0.15">
       <c r="A146" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B146" s="3"/>
       <c r="C146" s="3"/>
     </row>
     <row r="147" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A147" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B147" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="B147" s="3" t="s">
+      <c r="C147" s="3" t="s">
         <v>250</v>
-      </c>
-      <c r="C147" s="3" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="112" x14ac:dyDescent="0.15">
       <c r="A148" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
     </row>
     <row r="149" spans="1:3" ht="126" x14ac:dyDescent="0.15">
       <c r="A149" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
     </row>
     <row r="150" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A150" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B150" s="3"/>
       <c r="C150" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="196" x14ac:dyDescent="0.15">
       <c r="A151" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B151" s="3" t="s">
         <v>256</v>
-      </c>
-      <c r="B151" s="3" t="s">
-        <v>257</v>
       </c>
       <c r="C151" s="3"/>
     </row>
     <row r="152" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A152" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B152" s="3"/>
       <c r="C152" s="3"/>
     </row>
     <row r="153" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A153" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B153" s="3" t="s">
         <v>259</v>
-      </c>
-      <c r="B153" s="3" t="s">
-        <v>260</v>
       </c>
       <c r="C153" s="3"/>
     </row>
     <row r="154" spans="1:3" ht="294" x14ac:dyDescent="0.15">
       <c r="A154" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B154" s="3"/>
       <c r="C154" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="322" x14ac:dyDescent="0.15">
       <c r="A155" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B155" s="3"/>
       <c r="C155" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A156" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B156" s="3"/>
       <c r="C156" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="140" x14ac:dyDescent="0.15">
       <c r="A157" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B157" s="3"/>
       <c r="C157" s="3"/>
     </row>
     <row r="158" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A158" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
     </row>
     <row r="159" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A159" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B159" s="3"/>
       <c r="C159" s="3"/>
     </row>
     <row r="160" spans="1:3" ht="112" x14ac:dyDescent="0.15">
       <c r="A160" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B160" s="3"/>
       <c r="C160" s="3"/>
     </row>
     <row r="161" spans="1:3" ht="266" x14ac:dyDescent="0.15">
       <c r="A161" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B161" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="B161" s="3" t="s">
+      <c r="C161" s="3" t="s">
         <v>272</v>
-      </c>
-      <c r="C161" s="3" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="266" x14ac:dyDescent="0.15">
       <c r="A162" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B162" s="3"/>
       <c r="C162" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A163" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B163" s="3"/>
       <c r="C163" s="3"/>
     </row>
     <row r="164" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A164" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B164" s="3"/>
       <c r="C164" s="3"/>
     </row>
     <row r="165" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A165" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B165" s="3"/>
       <c r="C165" s="3"/>
     </row>
     <row r="166" spans="1:3" ht="126" x14ac:dyDescent="0.15">
       <c r="A166" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B166" s="3"/>
       <c r="C166" s="3"/>
     </row>
     <row r="167" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A167" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="B167" s="3" t="s">
         <v>280</v>
-      </c>
-      <c r="B167" s="3" t="s">
-        <v>281</v>
       </c>
       <c r="C167" s="3"/>
     </row>
     <row r="168" spans="1:3" ht="266" x14ac:dyDescent="0.15">
       <c r="A168" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B168" s="3"/>
       <c r="C168" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A169" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B169" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="B169" s="3" t="s">
+      <c r="C169" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="C169" s="3" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A170" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B170" s="3"/>
       <c r="C170" s="3"/>
     </row>
     <row r="171" spans="1:3" ht="364" x14ac:dyDescent="0.15">
       <c r="A171" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B171" s="6"/>
       <c r="C171" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="252" x14ac:dyDescent="0.15">
       <c r="A172" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B172" s="3"/>
       <c r="C172" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A173" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B173" s="3"/>
       <c r="C173" s="3"/>
     </row>
     <row r="174" spans="1:3" ht="140" x14ac:dyDescent="0.15">
       <c r="A174" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B174" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="B174" s="3" t="s">
+      <c r="C174" s="3" t="s">
         <v>294</v>
-      </c>
-      <c r="C174" s="3" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="175" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A175" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B175" s="3"/>
       <c r="C175" s="3"/>
     </row>
     <row r="176" spans="1:3" ht="126" x14ac:dyDescent="0.15">
       <c r="A176" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="B176" s="3" t="s">
         <v>297</v>
-      </c>
-      <c r="B176" s="3" t="s">
-        <v>298</v>
       </c>
       <c r="C176" s="3"/>
     </row>
     <row r="177" spans="1:3" ht="168" x14ac:dyDescent="0.15">
       <c r="A177" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B177" s="3"/>
       <c r="C177" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A178" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B178" s="3"/>
       <c r="C178" s="3"/>
     </row>
     <row r="179" spans="1:3" ht="406" x14ac:dyDescent="0.15">
       <c r="A179" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B179" s="3"/>
       <c r="C179" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="126" x14ac:dyDescent="0.15">
       <c r="A180" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B180" s="3" t="s">
         <v>304</v>
-      </c>
-      <c r="B180" s="3" t="s">
-        <v>305</v>
       </c>
       <c r="C180" s="3"/>
     </row>
     <row r="181" spans="1:3" ht="126" x14ac:dyDescent="0.15">
       <c r="A181" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B181" s="3" t="s">
         <v>306</v>
-      </c>
-      <c r="B181" s="3" t="s">
-        <v>307</v>
       </c>
       <c r="C181" s="3"/>
     </row>
     <row r="182" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A182" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B182" s="3"/>
       <c r="C182" s="3"/>
     </row>
     <row r="183" spans="1:3" ht="112" x14ac:dyDescent="0.15">
       <c r="A183" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B183" s="3"/>
       <c r="C183" s="3"/>
     </row>
     <row r="184" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A184" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B184" s="3"/>
       <c r="C184" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="378" x14ac:dyDescent="0.15">
       <c r="A185" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B185" s="3"/>
       <c r="C185" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A186" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B186" s="3"/>
       <c r="C186" s="3"/>
     </row>
     <row r="187" spans="1:3" ht="140" x14ac:dyDescent="0.15">
       <c r="A187" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B187" s="3"/>
       <c r="C187" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="188" spans="1:3" ht="168" x14ac:dyDescent="0.15">
       <c r="A188" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="B188" s="3" t="s">
         <v>317</v>
-      </c>
-      <c r="B188" s="3" t="s">
-        <v>318</v>
       </c>
       <c r="C188" s="3"/>
     </row>
     <row r="189" spans="1:3" ht="196" x14ac:dyDescent="0.15">
       <c r="A189" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B189" s="6"/>
       <c r="C189" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A190" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B190" s="6"/>
       <c r="C190" s="3"/>
     </row>
     <row r="191" spans="1:3" ht="168" x14ac:dyDescent="0.15">
       <c r="A191" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B191" s="6"/>
       <c r="C191" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="192" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A192" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B192" s="6"/>
       <c r="C192" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A193" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B193" s="6"/>
       <c r="C193" s="3"/>
     </row>
     <row r="194" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A194" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B194" s="3"/>
       <c r="C194" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="195" spans="1:3" ht="112" x14ac:dyDescent="0.15">
       <c r="A195" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B195" s="3"/>
       <c r="C195" s="3"/>
     </row>
     <row r="196" spans="1:3" ht="196" x14ac:dyDescent="0.15">
       <c r="A196" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B196" s="3" t="s">
         <v>330</v>
-      </c>
-      <c r="B196" s="3" t="s">
-        <v>331</v>
       </c>
       <c r="C196" s="3"/>
     </row>
     <row r="197" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A197" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B197" s="3"/>
       <c r="C197" s="3"/>
     </row>
     <row r="198" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A198" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B198" s="3" t="s">
         <v>333</v>
-      </c>
-      <c r="B198" s="3" t="s">
-        <v>334</v>
       </c>
       <c r="C198" s="3"/>
     </row>
     <row r="199" spans="1:3" ht="168" x14ac:dyDescent="0.15">
       <c r="A199" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="B199" s="3" t="s">
         <v>335</v>
-      </c>
-      <c r="B199" s="3" t="s">
-        <v>336</v>
       </c>
       <c r="C199" s="3"/>
     </row>
     <row r="200" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A200" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="B200" s="3" t="s">
         <v>337</v>
-      </c>
-      <c r="B200" s="3" t="s">
-        <v>338</v>
       </c>
       <c r="C200" s="3"/>
     </row>
     <row r="201" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A201" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B201" s="3"/>
       <c r="C201" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="202" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A202" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B202" s="3"/>
       <c r="C202" s="3"/>
     </row>
     <row r="203" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A203" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B203" s="3"/>
       <c r="C203" s="3"/>
     </row>
     <row r="204" spans="1:3" ht="140" x14ac:dyDescent="0.15">
       <c r="A204" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B204" s="3"/>
       <c r="C204" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="205" spans="1:3" ht="196" x14ac:dyDescent="0.15">
       <c r="A205" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B205" s="3"/>
       <c r="C205" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="206" spans="1:3" ht="406" x14ac:dyDescent="0.15">
       <c r="A206" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B206" s="3"/>
       <c r="C206" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="207" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A207" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B207" s="3"/>
       <c r="C207" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="208" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A208" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B208" s="3"/>
       <c r="C208" s="3"/>
     </row>
     <row r="209" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A209" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="B209" s="3" t="s">
         <v>352</v>
-      </c>
-      <c r="B209" s="3" t="s">
-        <v>353</v>
       </c>
       <c r="C209" s="3"/>
     </row>
     <row r="210" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A210" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B210" s="3"/>
       <c r="C210" s="3"/>
     </row>
     <row r="211" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A211" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B211" s="3"/>
       <c r="C211" s="3"/>
     </row>
     <row r="212" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A212" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B212" s="3"/>
       <c r="C212" s="3"/>
     </row>
     <row r="213" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A213" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B213" s="3"/>
       <c r="C213" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="214" spans="1:3" ht="210" x14ac:dyDescent="0.15">
       <c r="A214" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B214" s="3"/>
       <c r="C214" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="112" x14ac:dyDescent="0.15">
       <c r="A215" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B215" s="3"/>
       <c r="C215" s="3"/>
     </row>
     <row r="216" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A216" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B216" s="3"/>
       <c r="C216" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="217" spans="1:3" ht="406" x14ac:dyDescent="0.15">
       <c r="A217" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B217" s="3"/>
       <c r="C217" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="218" spans="1:3" ht="238" x14ac:dyDescent="0.15">
       <c r="A218" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="B218" s="3" t="s">
         <v>366</v>
-      </c>
-      <c r="B218" s="3" t="s">
-        <v>367</v>
       </c>
       <c r="C218" s="3"/>
     </row>
     <row r="219" spans="1:3" ht="378" x14ac:dyDescent="0.15">
       <c r="A219" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B219" s="3"/>
       <c r="C219" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="220" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A220" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B220" s="3"/>
       <c r="C220" s="3"/>
     </row>
     <row r="221" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A221" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B221" s="3"/>
       <c r="C221" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="222" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A222" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B222" s="3"/>
       <c r="C222" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="223" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A223" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B223" s="3"/>
       <c r="C223" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="224" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A224" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B224" s="3"/>
       <c r="C224" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="225" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A225" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B225" s="3"/>
       <c r="C225" s="3"/>
     </row>
     <row r="226" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A226" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B226" s="3"/>
       <c r="C226" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="227" spans="1:3" ht="140" x14ac:dyDescent="0.15">
       <c r="A227" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="B227" s="3" t="s">
         <v>381</v>
-      </c>
-      <c r="B227" s="3" t="s">
-        <v>382</v>
       </c>
       <c r="C227" s="3"/>
     </row>
     <row r="228" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A228" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B228" s="3"/>
       <c r="C228" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="229" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A229" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B229" s="3"/>
       <c r="C229" s="3"/>
     </row>
     <row r="230" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A230" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B230" s="3"/>
       <c r="C230" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="231" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A231" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B231" s="3"/>
       <c r="C231" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="232" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A232" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B232" s="3"/>
       <c r="C232" s="3"/>
     </row>
     <row r="233" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A233" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B233" s="3"/>
       <c r="C233" s="3"/>
     </row>
     <row r="234" spans="1:3" ht="112" x14ac:dyDescent="0.15">
       <c r="A234" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B234" s="3"/>
       <c r="C234" s="3"/>
     </row>
     <row r="235" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A235" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="B235" s="3" t="s">
         <v>393</v>
-      </c>
-      <c r="B235" s="3" t="s">
-        <v>394</v>
       </c>
       <c r="C235" s="3"/>
     </row>
     <row r="236" spans="1:3" ht="280" x14ac:dyDescent="0.15">
       <c r="A236" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B236" s="3"/>
       <c r="C236" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="237" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A237" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B237" s="3"/>
       <c r="C237" s="3"/>
     </row>
     <row r="238" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A238" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B238" s="3"/>
       <c r="C238" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="239" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A239" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B239" s="3"/>
       <c r="C239" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="240" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A240" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B240" s="3"/>
       <c r="C240" s="3"/>
     </row>
     <row r="241" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A241" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B241" s="3"/>
       <c r="C241" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="242" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A242" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B242" s="3"/>
       <c r="C242" s="3"/>
     </row>
     <row r="243" spans="1:3" ht="126" x14ac:dyDescent="0.15">
       <c r="A243" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B243" s="3"/>
       <c r="C243" s="3"/>
     </row>
     <row r="244" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A244" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B244" s="3"/>
       <c r="C244" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="245" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A245" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B245" s="3"/>
       <c r="C245" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="246" spans="1:3" ht="140" x14ac:dyDescent="0.15">
       <c r="A246" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="B246" s="3" t="s">
         <v>411</v>
-      </c>
-      <c r="B246" s="3" t="s">
-        <v>412</v>
       </c>
       <c r="C246" s="3"/>
     </row>
     <row r="247" spans="1:3" ht="294" x14ac:dyDescent="0.15">
       <c r="A247" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B247" s="3"/>
       <c r="C247" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="248" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A248" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B248" s="3"/>
       <c r="C248" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="249" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A249" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B249" s="3"/>
       <c r="C249" s="3"/>
     </row>
     <row r="250" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A250" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B250" s="3"/>
       <c r="C250" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="251" spans="1:3" ht="126" x14ac:dyDescent="0.15">
       <c r="A251" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="B251" s="3" t="s">
         <v>420</v>
-      </c>
-      <c r="B251" s="3" t="s">
-        <v>421</v>
       </c>
       <c r="C251" s="3"/>
     </row>
     <row r="252" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A252" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B252" s="3"/>
       <c r="C252" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="253" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A253" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B253" s="3"/>
       <c r="C253" s="3"/>
     </row>
     <row r="254" spans="1:3" ht="168" x14ac:dyDescent="0.15">
       <c r="A254" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B254" s="3"/>
       <c r="C254" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="255" spans="1:3" ht="126" x14ac:dyDescent="0.15">
       <c r="A255" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B255" s="3"/>
       <c r="C255" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="256" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A256" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B256" s="3"/>
       <c r="C256" s="3"/>
     </row>
     <row r="257" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A257" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B257" s="3"/>
       <c r="C257" s="3"/>
     </row>
     <row r="258" spans="1:3" ht="196" x14ac:dyDescent="0.15">
       <c r="A258" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B258" s="3"/>
       <c r="C258" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="259" spans="1:3" ht="210" x14ac:dyDescent="0.15">
       <c r="A259" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B259" s="3"/>
       <c r="C259" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="260" spans="1:3" ht="112" x14ac:dyDescent="0.15">
       <c r="A260" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B260" s="3"/>
       <c r="C260" s="3"/>
     </row>
     <row r="261" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A261" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B261" s="3"/>
       <c r="C261" s="3"/>
     </row>
     <row r="262" spans="1:3" ht="196" x14ac:dyDescent="0.15">
       <c r="A262" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="B262" s="3" t="s">
         <v>437</v>
-      </c>
-      <c r="B262" s="3" t="s">
-        <v>438</v>
       </c>
       <c r="C262" s="3"/>
     </row>
     <row r="263" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A263" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B263" s="3"/>
       <c r="C263" s="3"/>
     </row>
     <row r="264" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A264" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B264" s="3"/>
       <c r="C264" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="265" spans="1:3" ht="350" x14ac:dyDescent="0.15">
       <c r="A265" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B265" s="3"/>
       <c r="C265" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="266" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A266" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B266" s="3"/>
       <c r="C266" s="3"/>
     </row>
     <row r="267" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A267" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B267" s="3"/>
       <c r="C267" s="3"/>
     </row>
     <row r="268" spans="1:3" ht="280" x14ac:dyDescent="0.15">
       <c r="A268" s="3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B268" s="3"/>
       <c r="C268" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="269" spans="1:3" ht="294" x14ac:dyDescent="0.15">
       <c r="A269" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B269" s="3"/>
       <c r="C269" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="270" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A270" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B270" s="3"/>
       <c r="C270" s="3"/>
     </row>
     <row r="271" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A271" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B271" s="3"/>
       <c r="C271" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="272" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A272" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B272" s="3"/>
       <c r="C272" s="3"/>
     </row>
     <row r="273" spans="1:3" ht="168" x14ac:dyDescent="0.15">
       <c r="A273" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="B273" s="3" t="s">
         <v>454</v>
-      </c>
-      <c r="B273" s="3" t="s">
-        <v>455</v>
       </c>
       <c r="C273" s="3"/>
     </row>
     <row r="274" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A274" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B274" s="3"/>
       <c r="C274" s="3"/>
     </row>
     <row r="275" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A275" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B275" s="3"/>
       <c r="C275" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="276" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A276" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B276" s="3"/>
       <c r="C276" s="3"/>
     </row>
     <row r="277" spans="1:3" ht="308" x14ac:dyDescent="0.15">
       <c r="A277" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B277" s="3"/>
       <c r="C277" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="278" spans="1:3" ht="266" x14ac:dyDescent="0.15">
       <c r="A278" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B278" s="3"/>
       <c r="C278" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="279" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A279" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B279" s="3"/>
       <c r="C279" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="280" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A280" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B280" s="3"/>
       <c r="C280" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="281" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A281" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B281" s="3"/>
       <c r="C281" s="3"/>
     </row>
     <row r="282" spans="1:3" ht="140" x14ac:dyDescent="0.15">
       <c r="A282" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B282" s="3"/>
       <c r="C282" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="283" spans="1:3" ht="210" x14ac:dyDescent="0.15">
       <c r="A283" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="B283" s="3" t="s">
         <v>471</v>
       </c>
-      <c r="B283" s="3" t="s">
+      <c r="C283" s="3" t="s">
         <v>472</v>
-      </c>
-      <c r="C283" s="3" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="284" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A284" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B284" s="3"/>
       <c r="C284" s="3"/>
     </row>
     <row r="285" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A285" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B285" s="3"/>
       <c r="C285" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="286" spans="1:3" ht="182" x14ac:dyDescent="0.15">
       <c r="A286" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="B286" s="3" t="s">
         <v>477</v>
-      </c>
-      <c r="B286" s="3" t="s">
-        <v>478</v>
       </c>
       <c r="C286" s="3"/>
     </row>
     <row r="287" spans="1:3" ht="126" x14ac:dyDescent="0.15">
       <c r="A287" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="B287" s="3" t="s">
         <v>479</v>
-      </c>
-      <c r="B287" s="3" t="s">
-        <v>480</v>
       </c>
       <c r="C287" s="3"/>
     </row>
     <row r="288" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A288" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B288" s="3"/>
       <c r="C288" s="3"/>
     </row>
     <row r="289" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A289" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B289" s="3"/>
       <c r="C289" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="290" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A290" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B290" s="3"/>
       <c r="C290" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="291" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A291" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B291" s="3"/>
       <c r="C291" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="292" spans="1:3" ht="126" x14ac:dyDescent="0.15">
       <c r="A292" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B292" s="3"/>
       <c r="C292" s="3" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="293" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A293" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B293" s="3"/>
       <c r="C293" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="294" spans="1:3" ht="168" x14ac:dyDescent="0.15">
       <c r="A294" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="B294" s="3" t="s">
         <v>492</v>
       </c>
-      <c r="B294" s="3" t="s">
+      <c r="C294" s="3" t="s">
         <v>493</v>
-      </c>
-      <c r="C294" s="3" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="295" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A295" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B295" s="3"/>
       <c r="C295" s="3"/>
     </row>
     <row r="296" spans="1:3" ht="182" x14ac:dyDescent="0.15">
       <c r="A296" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B296" s="3"/>
       <c r="C296" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="297" spans="1:3" ht="168" x14ac:dyDescent="0.15">
       <c r="A297" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="B297" s="3" t="s">
         <v>498</v>
-      </c>
-      <c r="B297" s="3" t="s">
-        <v>499</v>
       </c>
       <c r="C297" s="3"/>
     </row>
     <row r="298" spans="1:3" ht="196" x14ac:dyDescent="0.15">
       <c r="A298" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="B298" s="3" t="s">
         <v>500</v>
       </c>
-      <c r="B298" s="3" t="s">
+      <c r="C298" s="3" t="s">
         <v>501</v>
-      </c>
-      <c r="C298" s="3" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="299" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A299" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="B299" s="3" t="s">
         <v>503</v>
       </c>
-      <c r="B299" s="3" t="s">
+      <c r="C299" s="3" t="s">
         <v>504</v>
-      </c>
-      <c r="C299" s="3" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="300" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A300" s="3" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B300" s="3"/>
       <c r="C300" s="3"/>
     </row>
     <row r="301" spans="1:3" ht="112" x14ac:dyDescent="0.15">
       <c r="A301" s="3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B301" s="3"/>
       <c r="C301" s="3"/>
     </row>
     <row r="302" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A302" s="3" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B302" s="3"/>
       <c r="C302" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="303" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A303" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B303" s="3"/>
       <c r="C303" s="3"/>
     </row>
     <row r="304" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A304" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B304" s="3"/>
       <c r="C304" s="3"/>
     </row>
     <row r="305" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A305" s="3" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B305" s="3"/>
       <c r="C305" s="3"/>
     </row>
     <row r="306" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A306" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B306" s="3"/>
       <c r="C306" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="307" spans="1:3" ht="406" x14ac:dyDescent="0.15">
       <c r="A307" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B307" s="3"/>
       <c r="C307" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="308" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A308" s="3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B308" s="3"/>
       <c r="C308" s="3"/>
     </row>
     <row r="309" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A309" s="3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B309" s="3"/>
       <c r="C309" s="3"/>
     </row>
     <row r="310" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A310" s="3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B310" s="3"/>
       <c r="C310" s="3" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="311" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A311" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B311" s="3"/>
       <c r="C311" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="312" spans="1:3" ht="350" x14ac:dyDescent="0.15">
       <c r="A312" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B312" s="3"/>
       <c r="C312" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="313" spans="1:3" ht="280" x14ac:dyDescent="0.15">
       <c r="A313" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="B313" s="3" t="s">
         <v>525</v>
-      </c>
-      <c r="B313" s="3" t="s">
-        <v>526</v>
       </c>
       <c r="C313" s="3"/>
     </row>
     <row r="314" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A314" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B314" s="3"/>
       <c r="C314" s="3"/>
     </row>
     <row r="315" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A315" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B315" s="3"/>
       <c r="C315" s="3"/>
     </row>
     <row r="316" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A316" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B316" s="3"/>
       <c r="C316" s="3"/>
     </row>
     <row r="317" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A317" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B317" s="3"/>
       <c r="C317" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="318" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A318" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B318" s="3"/>
       <c r="C318" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="319" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A319" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="B319" s="3" t="s">
         <v>534</v>
       </c>
-      <c r="B319" s="3" t="s">
+      <c r="C319" s="3" t="s">
         <v>535</v>
-      </c>
-      <c r="C319" s="3" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="320" spans="1:3" ht="294" x14ac:dyDescent="0.15">
       <c r="A320" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="B320" s="3" t="s">
         <v>537</v>
       </c>
-      <c r="B320" s="3" t="s">
+      <c r="C320" s="3" t="s">
         <v>538</v>
-      </c>
-      <c r="C320" s="3" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="321" spans="1:3" ht="308" x14ac:dyDescent="0.15">
       <c r="A321" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B321" s="3"/>
       <c r="C321" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="322" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A322" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B322" s="3"/>
       <c r="C322" s="3" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="323" spans="1:3" ht="140" x14ac:dyDescent="0.15">
       <c r="A323" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B323" s="3"/>
       <c r="C323" s="3" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="324" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A324" s="3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B324" s="3"/>
       <c r="C324" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="325" spans="1:3" ht="140" x14ac:dyDescent="0.15">
       <c r="A325" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="B325" s="3" t="s">
         <v>548</v>
-      </c>
-      <c r="B325" s="3" t="s">
-        <v>549</v>
       </c>
       <c r="C325" s="3"/>
     </row>
     <row r="326" spans="1:3" ht="409" x14ac:dyDescent="0.15">
       <c r="A326" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B326" s="3"/>
       <c r="C326" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix kegg alzheimer's pathway name
</commit_message>
<xml_diff>
--- a/mappings/kegg_reactome.xlsx
+++ b/mappings/kegg_reactome.xlsx
@@ -124,7 +124,7 @@
     <t xml:space="preserve">Alzheimer disease - Homo sapiens (human)</t>
   </si>
   <si>
-    <t xml:space="preserve">Deregulated CDK5 triggers multiple neurodegenerative pathways in Alzheimer's disease models isPartOf Alzheimer's disease - Homo sapiens (human)*</t>
+    <t xml:space="preserve">Deregulated CDK5 triggers multiple neurodegenerative pathways in Alzheimer's disease models isPartOf Alzheimer disease - Homo sapiens (human)*</t>
   </si>
   <si>
     <t xml:space="preserve">Amino sugar and nucleotide sugar metabolism - Homo sapiens (human)</t>
@@ -2251,7 +2251,7 @@
   <dimension ref="A1:Y326"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2408,7 +2408,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="255.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="242.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
         <v>26</v>
       </c>

</xml_diff>